<commit_message>
update to data collection
</commit_message>
<xml_diff>
--- a/Data Collection.xlsx
+++ b/Data Collection.xlsx
@@ -5,17 +5,24 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yoga\Desktop\University\Thesis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yoga\Desktop\University\Thesis\TrustChain-Simulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E981EEE-89D0-421A-B352-1E5F7509359B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED6D5495-CA97-4E4E-85A0-D336204738D2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9405" yWindow="1665" windowWidth="16605" windowHeight="11535" xr2:uid="{BCACAF04-D4C4-41AE-BAB0-4F6EFB70057E}"/>
+    <workbookView xWindow="690" yWindow="14415" windowWidth="14130" windowHeight="12375" xr2:uid="{BCACAF04-D4C4-41AE-BAB0-4F6EFB70057E}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Planning" sheetId="3" r:id="rId1"/>
     <sheet name="Set1" sheetId="4" r:id="rId2"/>
+    <sheet name="Set2" sheetId="6" r:id="rId3"/>
+    <sheet name="Set3" sheetId="7" r:id="rId4"/>
+    <sheet name="Normal Distribution Test" sheetId="5" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">'Normal Distribution Test'!$D$5:$D$54</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'Normal Distribution Test'!$D$5:$D$54</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -32,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="31">
   <si>
     <t>Evil Node Sleeping Transactions</t>
   </si>
@@ -110,6 +117,21 @@
   </si>
   <si>
     <t>Set</t>
+  </si>
+  <si>
+    <t>1 - Number of nodes</t>
+  </si>
+  <si>
+    <t>2 - Numer of evil node</t>
+  </si>
+  <si>
+    <t>3 - Transmission speed</t>
+  </si>
+  <si>
+    <t>To compute</t>
+  </si>
+  <si>
+    <t>t student (non normal)</t>
   </si>
 </sst>
 </file>
@@ -259,6 +281,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="4"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -268,7 +291,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Calculation" xfId="4" builtinId="22"/>
@@ -288,6 +310,722 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.1</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>Chart Title</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1" compatLnSpc="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>Chart Title</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="clusteredColumn" uniqueId="{25ED4015-0958-4046-9F1F-E31B8E1A9E9A}">
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:binning intervalClosed="r"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="0.330000013"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>519112</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>214312</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="2" name="Chart 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{958A89FF-0374-4007-AE46-8A77DC831195}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2957512" y="1157287"/>
+              <a:ext cx="4572000" cy="2743200"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -587,14 +1325,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4891D42F-3971-43B5-986A-C0853C8465A0}">
-  <dimension ref="A1:P60"/>
+  <dimension ref="A1:P38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
@@ -657,8 +1396,8 @@
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="7">
-        <v>1</v>
+      <c r="A2" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
@@ -700,7 +1439,7 @@
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
+      <c r="A3" s="9"/>
       <c r="B3" s="4">
         <v>2</v>
       </c>
@@ -712,7 +1451,7 @@
         <v>0.13695052585936646</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" ref="E3:E12" si="0">LN(C3)/(C3)</f>
+        <f t="shared" ref="E3:E13" si="0">LN(C3)/(C3)</f>
         <v>0.14978661367769955</v>
       </c>
       <c r="F3" s="1">
@@ -744,7 +1483,7 @@
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
+      <c r="A4" s="9"/>
       <c r="B4" s="4">
         <v>3</v>
       </c>
@@ -752,7 +1491,7 @@
         <v>50</v>
       </c>
       <c r="D4" s="1">
-        <f>2*LOG(C4)/(C4-1)</f>
+        <f t="shared" ref="D4:D13" si="1">2*LOG(C4)/(C4-1)</f>
         <v>6.9345714462694649E-2</v>
       </c>
       <c r="E4" s="1">
@@ -791,7 +1530,7 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
+      <c r="A5" s="9"/>
       <c r="B5" s="4">
         <v>4</v>
       </c>
@@ -799,7 +1538,7 @@
         <v>100</v>
       </c>
       <c r="D5" s="1">
-        <f>2*LOG(C5)/(C5-1)</f>
+        <f t="shared" si="1"/>
         <v>4.0404040404040407E-2</v>
       </c>
       <c r="E5" s="1">
@@ -835,7 +1574,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
+      <c r="A6" s="9"/>
       <c r="B6" s="4">
         <v>5</v>
       </c>
@@ -843,14 +1582,17 @@
         <v>1000</v>
       </c>
       <c r="D6" s="1">
-        <f>2*LOG(C6)/(C6-1)</f>
+        <f t="shared" si="1"/>
         <v>6.006006006006006E-3</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
         <v>6.9077552789821367E-3</v>
       </c>
-      <c r="F6" s="1"/>
+      <c r="F6" s="1">
+        <f>E6</f>
+        <v>6.9077552789821367E-3</v>
+      </c>
       <c r="G6" s="1">
         <v>10</v>
       </c>
@@ -877,7 +1619,7 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
+      <c r="A7" s="9"/>
       <c r="B7" s="4">
         <v>6</v>
       </c>
@@ -885,7 +1627,7 @@
         <v>10000</v>
       </c>
       <c r="D7" s="1">
-        <f>2*LOG(C7)/(C7-1)</f>
+        <f t="shared" si="1"/>
         <v>8.0008000800080011E-4</v>
       </c>
       <c r="E7" s="1">
@@ -919,24 +1661,26 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="9">
-        <v>2</v>
+      <c r="A8" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="B8" s="5">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C8" s="1">
-        <v>10000</v>
+        <v>100</v>
       </c>
       <c r="D8" s="1">
         <f>2*LOG(C8)/(C8-1)</f>
-        <v>8.0008000800080011E-4</v>
+        <v>4.0404040404040407E-2</v>
       </c>
       <c r="E8" s="1">
-        <f t="shared" si="0"/>
-        <v>9.210340371976184E-4</v>
-      </c>
-      <c r="F8" s="1"/>
+        <f>LN(C8)/(C8)</f>
+        <v>4.6051701859880917E-2</v>
+      </c>
+      <c r="F8" s="1">
+        <v>4.7E-2</v>
+      </c>
       <c r="G8" s="1">
         <v>10</v>
       </c>
@@ -944,7 +1688,7 @@
         <v>100</v>
       </c>
       <c r="I8" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>8</v>
@@ -956,29 +1700,31 @@
         <v>10</v>
       </c>
       <c r="M8" s="1">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
+      <c r="A9" s="10"/>
       <c r="B9" s="5">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C9" s="1">
-        <v>10000</v>
+        <v>100</v>
       </c>
       <c r="D9" s="1">
         <f>2*LOG(C9)/(C9-1)</f>
-        <v>8.0008000800080011E-4</v>
+        <v>4.0404040404040407E-2</v>
       </c>
       <c r="E9" s="1">
-        <f t="shared" si="0"/>
-        <v>9.210340371976184E-4</v>
-      </c>
-      <c r="F9" s="1"/>
+        <f>LN(C9)/(C9)</f>
+        <v>4.6051701859880917E-2</v>
+      </c>
+      <c r="F9" s="1">
+        <v>4.7E-2</v>
+      </c>
       <c r="G9" s="1">
         <v>10</v>
       </c>
@@ -986,7 +1732,7 @@
         <v>100</v>
       </c>
       <c r="I9" s="1">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>8</v>
@@ -998,28 +1744,31 @@
         <v>10</v>
       </c>
       <c r="M9" s="1">
+        <v>50</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="10"/>
+      <c r="B10" s="5">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1">
         <v>100</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="9">
-        <v>3</v>
-      </c>
-      <c r="B10" s="6">
-        <v>9</v>
-      </c>
-      <c r="C10" s="1">
-        <v>10000</v>
-      </c>
       <c r="D10" s="1">
-        <f>2*LOG(C10)/(C10-1)</f>
-        <v>8.0008000800080011E-4</v>
+        <f t="shared" si="1"/>
+        <v>4.0404040404040407E-2</v>
       </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>9.210340371976184E-4</v>
-      </c>
-      <c r="F10" s="1"/>
+        <v>4.6051701859880917E-2</v>
+      </c>
+      <c r="F10" s="1">
+        <v>4.7E-2</v>
+      </c>
       <c r="G10" s="1">
         <v>10</v>
       </c>
@@ -1027,38 +1776,42 @@
         <v>100</v>
       </c>
       <c r="I10" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="M10" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="6">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1">
         <v>100</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
-      <c r="B11" s="6">
-        <v>10</v>
-      </c>
-      <c r="C11" s="1">
-        <v>10000</v>
-      </c>
       <c r="D11" s="1">
-        <f>2*LOG(C11)/(C11-1)</f>
-        <v>8.0008000800080011E-4</v>
+        <f t="shared" si="1"/>
+        <v>4.0404040404040407E-2</v>
       </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>9.210340371976184E-4</v>
-      </c>
-      <c r="F11" s="1"/>
+        <v>4.6051701859880917E-2</v>
+      </c>
+      <c r="F11" s="1">
+        <v>4.7E-2</v>
+      </c>
       <c r="G11" s="1">
         <v>10</v>
       </c>
@@ -1072,32 +1825,34 @@
         <v>8</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>10</v>
       </c>
       <c r="M11" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="10"/>
+      <c r="B12" s="6">
+        <v>2</v>
+      </c>
+      <c r="C12" s="1">
         <v>100</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-      <c r="B12" s="6">
-        <v>11</v>
-      </c>
-      <c r="C12" s="1">
-        <v>10000</v>
-      </c>
       <c r="D12" s="1">
-        <f>2*LOG(C12)/(C12-1)</f>
-        <v>8.0008000800080011E-4</v>
+        <f t="shared" si="1"/>
+        <v>4.0404040404040407E-2</v>
       </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>9.210340371976184E-4</v>
-      </c>
-      <c r="F12" s="1"/>
+        <v>4.6051701859880917E-2</v>
+      </c>
+      <c r="F12" s="1">
+        <v>4.7E-2</v>
+      </c>
       <c r="G12" s="1">
         <v>10</v>
       </c>
@@ -1111,35 +1866,57 @@
         <v>8</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="M12" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="10"/>
+      <c r="B13" s="6">
+        <v>3</v>
+      </c>
+      <c r="C13" s="1">
         <v>100</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B13">
-        <v>12</v>
-      </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
+      <c r="D13" s="1">
+        <f t="shared" si="1"/>
+        <v>4.0404040404040407E-2</v>
+      </c>
+      <c r="E13" s="1">
+        <f t="shared" si="0"/>
+        <v>4.6051701859880917E-2</v>
+      </c>
+      <c r="F13" s="1">
+        <v>4.7E-2</v>
+      </c>
+      <c r="G13" s="1">
+        <v>10</v>
+      </c>
+      <c r="H13" s="1">
+        <v>100</v>
+      </c>
+      <c r="I13" s="1">
+        <v>1</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M13" s="1">
+        <v>50</v>
+      </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B14">
-        <v>13</v>
-      </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -1153,9 +1930,6 @@
       <c r="M14" s="1"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B15">
-        <v>14</v>
-      </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -1169,9 +1943,6 @@
       <c r="M15" s="1"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B16">
-        <v>15</v>
-      </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -1184,10 +1955,7 @@
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B17">
-        <v>16</v>
-      </c>
+    <row r="17" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -1200,10 +1968,7 @@
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B18">
-        <v>17</v>
-      </c>
+    <row r="18" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -1216,10 +1981,7 @@
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B19">
-        <v>18</v>
-      </c>
+    <row r="19" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -1232,10 +1994,7 @@
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B20">
-        <v>19</v>
-      </c>
+    <row r="20" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -1248,10 +2007,7 @@
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B21">
-        <v>20</v>
-      </c>
+    <row r="21" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -1264,10 +2020,7 @@
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B22">
-        <v>21</v>
-      </c>
+    <row r="22" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -1280,10 +2033,7 @@
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B23">
-        <v>22</v>
-      </c>
+    <row r="23" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -1296,10 +2046,7 @@
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B24">
-        <v>23</v>
-      </c>
+    <row r="24" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -1312,10 +2059,7 @@
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B25">
-        <v>24</v>
-      </c>
+    <row r="25" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -1328,10 +2072,7 @@
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B26">
-        <v>25</v>
-      </c>
+    <row r="26" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -1344,10 +2085,7 @@
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B27">
-        <v>26</v>
-      </c>
+    <row r="27" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -1360,10 +2098,7 @@
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B28">
-        <v>27</v>
-      </c>
+    <row r="28" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -1376,10 +2111,7 @@
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B29">
-        <v>28</v>
-      </c>
+    <row r="29" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -1392,10 +2124,7 @@
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B30">
-        <v>29</v>
-      </c>
+    <row r="30" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
@@ -1408,10 +2137,7 @@
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B31">
-        <v>30</v>
-      </c>
+    <row r="31" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
@@ -1424,10 +2150,7 @@
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B32">
-        <v>31</v>
-      </c>
+    <row r="32" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -1440,10 +2163,7 @@
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
     </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B33">
-        <v>32</v>
-      </c>
+    <row r="33" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
@@ -1456,10 +2176,7 @@
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
     </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B34">
-        <v>33</v>
-      </c>
+    <row r="34" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
@@ -1472,10 +2189,7 @@
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
     </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B35">
-        <v>34</v>
-      </c>
+    <row r="35" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
@@ -1488,10 +2202,7 @@
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
     </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B36">
-        <v>35</v>
-      </c>
+    <row r="36" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
@@ -1504,10 +2215,7 @@
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
     </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B37">
-        <v>36</v>
-      </c>
+    <row r="37" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
@@ -1520,126 +2228,24 @@
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
     </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B38">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B39">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B40">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B41">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B42">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B43">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B44">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="45" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B45">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="46" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B46">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="47" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B47">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B48">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B49">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B50">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B51">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B52">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B53">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B54">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B55">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B56">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B57">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B58">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B59">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B60">
-        <v>59</v>
-      </c>
+    <row r="38" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+      <c r="L38" s="1"/>
+      <c r="M38" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A11:A13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1650,8 +2256,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF874DAA-691A-4835-ACA3-DB30922CFD6B}">
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1695,6 +2301,9 @@
       <c r="E2">
         <v>0.91530000000300005</v>
       </c>
+      <c r="F2">
+        <v>0.91530000000300005</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3">
@@ -1709,6 +2318,9 @@
       <c r="E3">
         <v>0.91530000000300005</v>
       </c>
+      <c r="F3">
+        <v>0.99268824148599999</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4">
@@ -1723,6 +2335,9 @@
       <c r="E4">
         <v>1.2204000000040001</v>
       </c>
+      <c r="F4">
+        <v>0.94797846390899998</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5">
@@ -1737,6 +2352,9 @@
       <c r="E5">
         <v>0.61020000000200003</v>
       </c>
+      <c r="F5">
+        <v>1.2216387008730001</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6">
@@ -1751,6 +2369,9 @@
       <c r="E6">
         <v>0.91530000000300005</v>
       </c>
+      <c r="F6">
+        <v>1.423855858874</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7">
@@ -1764,6 +2385,9 @@
       </c>
       <c r="E7">
         <v>0.30510000000100002</v>
+      </c>
+      <c r="F7">
+        <v>0.91560787649700004</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2383,27 +3007,27 @@
       </c>
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B52" s="10">
+      <c r="B52" s="7">
         <f>AVERAGE(B2:B51)</f>
         <v>0.65907088731205998</v>
       </c>
-      <c r="C52" s="10">
+      <c r="C52" s="7">
         <f t="shared" ref="C52:F52" si="0">AVERAGE(C2:C51)</f>
         <v>0.96447097937686022</v>
       </c>
-      <c r="D52" s="10">
+      <c r="D52" s="7">
         <f t="shared" ref="D52" si="1">AVERAGE(D2:D51)</f>
         <v>0.89090111111418024</v>
       </c>
-      <c r="E52" s="10">
+      <c r="E52" s="7">
         <f t="shared" ref="E52" si="2">AVERAGE(E2:E51)</f>
         <v>0.91610186017854023</v>
       </c>
-      <c r="F52" s="10" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G52" s="10" t="e">
+      <c r="F52" s="7">
+        <f>AVERAGE(F2:F7)</f>
+        <v>1.0695115236070001</v>
+      </c>
+      <c r="G52" s="7" t="e">
         <f>AVERAGE(G2:G51)</f>
         <v>#DIV/0!</v>
       </c>
@@ -2411,4 +3035,2064 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A8ADDF3-F6DC-49DE-90F6-6F07047D1F12}">
+  <dimension ref="A1:D172"/>
+  <sheetViews>
+    <sheetView topLeftCell="A171" workbookViewId="0">
+      <selection activeCell="D172" sqref="D172"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="5">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="C2">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="D2">
+        <v>0.30510000000100002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="C3">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="D3">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>1.2204000000040001</v>
+      </c>
+      <c r="C4">
+        <v>0.915806248366</v>
+      </c>
+      <c r="D4">
+        <v>0.30510000000100002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>0.61020000000200003</v>
+      </c>
+      <c r="C5">
+        <v>0.61020000000200003</v>
+      </c>
+      <c r="D5">
+        <v>0.30510000000100002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="C6">
+        <v>1.2204000000040001</v>
+      </c>
+      <c r="D6">
+        <v>1.5255000000050001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>0.30510000000100002</v>
+      </c>
+      <c r="C7">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="D7">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>1.5506994742060001</v>
+      </c>
+      <c r="C8">
+        <v>0.61020000000200003</v>
+      </c>
+      <c r="D8">
+        <v>1.2204000000040001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="C9">
+        <v>1.280352210762</v>
+      </c>
+      <c r="D9">
+        <v>0.94558310152400005</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>0.61020000000200003</v>
+      </c>
+      <c r="C10">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="D10">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>0.91610358299899997</v>
+      </c>
+      <c r="C11">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="D11">
+        <v>1.2204000000040001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>1.221610090177</v>
+      </c>
+      <c r="C12">
+        <v>0.30510000000100002</v>
+      </c>
+      <c r="D12">
+        <v>1.2204000000040001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="C13">
+        <v>1.2204000000040001</v>
+      </c>
+      <c r="D13">
+        <v>0.30510000000100002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>0.91621382376299998</v>
+      </c>
+      <c r="C14">
+        <v>0.61020000000200003</v>
+      </c>
+      <c r="D14">
+        <v>0.61020000000200003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>0.92268943506099999</v>
+      </c>
+      <c r="C15">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="D15">
+        <v>0.61020000000200003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>0.61020000000200003</v>
+      </c>
+      <c r="C16">
+        <v>1.2204000000040001</v>
+      </c>
+      <c r="D16">
+        <v>0.61020000000200003</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="C17">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="D17">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="C18">
+        <v>0.61020000000200003</v>
+      </c>
+      <c r="D18">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="C19">
+        <v>1.2204000000040001</v>
+      </c>
+      <c r="D19">
+        <v>0.61020000000200003</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>1.2204000000040001</v>
+      </c>
+      <c r="C20">
+        <v>0.91610358299899997</v>
+      </c>
+      <c r="D20">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="C21">
+        <v>1.5255000000050001</v>
+      </c>
+      <c r="D21">
+        <v>0.61020000000200003</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>0.30510000000100002</v>
+      </c>
+      <c r="C22">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="D22">
+        <v>1.2204000000040001</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="C23">
+        <v>1.222405676763</v>
+      </c>
+      <c r="D23">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>1.2204000000040001</v>
+      </c>
+      <c r="C24">
+        <v>1.2204000000040001</v>
+      </c>
+      <c r="D24">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="C25">
+        <v>1.5255000000050001</v>
+      </c>
+      <c r="D25">
+        <v>0.30510000000100002</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>0.91572428847099996</v>
+      </c>
+      <c r="C26">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="D26">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="C27">
+        <v>1.2204000000040001</v>
+      </c>
+      <c r="D27">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>0.91580119928699999</v>
+      </c>
+      <c r="C28">
+        <v>0.92268943506099999</v>
+      </c>
+      <c r="D28">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>1.220789647273</v>
+      </c>
+      <c r="C29">
+        <v>1.2204000000040001</v>
+      </c>
+      <c r="D29">
+        <v>0.92352396971999995</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>1.2204000000040001</v>
+      </c>
+      <c r="C30">
+        <v>1.656184664959</v>
+      </c>
+      <c r="D30">
+        <v>0.61020000000200003</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>0.61020000000200003</v>
+      </c>
+      <c r="C31">
+        <v>0.30510000000100002</v>
+      </c>
+      <c r="D31">
+        <v>0.61022222222400002</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>0.91639452465600002</v>
+      </c>
+      <c r="C32">
+        <v>0.30510000000100002</v>
+      </c>
+      <c r="D32">
+        <v>0.61020000000200003</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="C33">
+        <v>0.91691372466400001</v>
+      </c>
+      <c r="D33">
+        <v>1.2204000000040001</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="C34">
+        <v>1.5255000000050001</v>
+      </c>
+      <c r="D34">
+        <v>0.30510000000100002</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>0.91533333333599998</v>
+      </c>
+      <c r="C35">
+        <v>1.2204000000040001</v>
+      </c>
+      <c r="D35">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="C36">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="D36">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="C37">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="D37">
+        <v>0.91718800025799996</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>0.61020000000200003</v>
+      </c>
+      <c r="C38">
+        <v>1.220444444448</v>
+      </c>
+      <c r="D38">
+        <v>1.2204000000040001</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>0.915326595774</v>
+      </c>
+      <c r="C39">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="D39">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="C40">
+        <v>1.2204000000040001</v>
+      </c>
+      <c r="D40">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>0.61020000000200003</v>
+      </c>
+      <c r="C41">
+        <v>0.61020000000200003</v>
+      </c>
+      <c r="D41">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>1.222507013815</v>
+      </c>
+      <c r="C42">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="D42">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>1.2204000000040001</v>
+      </c>
+      <c r="C43">
+        <v>1.2204000000040001</v>
+      </c>
+      <c r="D43">
+        <v>1.2204000000040001</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>1.5255000000050001</v>
+      </c>
+      <c r="C44">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="D44">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="C45">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="D45">
+        <v>0.61020000000200003</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <v>1.2204000000040001</v>
+      </c>
+      <c r="C46">
+        <v>1.2204000000040001</v>
+      </c>
+      <c r="D46">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <v>0.61020000000200003</v>
+      </c>
+      <c r="C47">
+        <v>1.5255000000050001</v>
+      </c>
+      <c r="D47">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B48">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="C48">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="D48">
+        <v>1.2204000000040001</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <v>0.30510000000100002</v>
+      </c>
+      <c r="C49">
+        <v>1.5255000000050001</v>
+      </c>
+      <c r="D49">
+        <v>0.61020000000200003</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B50">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="C50">
+        <v>0.61060000000799997</v>
+      </c>
+      <c r="D50">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B51">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="C51">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="D51">
+        <v>0.61020000000200003</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B52" s="7">
+        <f>AVERAGE(B2:B51)</f>
+        <v>0.91610186017854023</v>
+      </c>
+      <c r="C52">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="D52">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C53">
+        <v>1.5395876522780001</v>
+      </c>
+      <c r="D53">
+        <v>1.118633333337</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C54">
+        <v>0.91580119928699999</v>
+      </c>
+      <c r="D54">
+        <v>1.220582246283</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C55">
+        <v>1.2204000000040001</v>
+      </c>
+      <c r="D55">
+        <v>1.2204000000040001</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C56">
+        <v>1.2204000000040001</v>
+      </c>
+      <c r="D56">
+        <v>1.2204000000040001</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C57">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="D57">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C58">
+        <v>1.2204000000040001</v>
+      </c>
+      <c r="D58">
+        <v>0.61020000000200003</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C59">
+        <v>1.5255000000050001</v>
+      </c>
+      <c r="D59">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C60">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="D60">
+        <v>1.2204000000040001</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C61">
+        <v>1.2204000000040001</v>
+      </c>
+      <c r="D61">
+        <v>0.61020000000200003</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C62">
+        <v>1.2204000000040001</v>
+      </c>
+      <c r="D62">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C63">
+        <v>1.2204000000040001</v>
+      </c>
+      <c r="D63">
+        <v>1.2204000000040001</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C64">
+        <v>1.2204000000040001</v>
+      </c>
+      <c r="D64">
+        <v>1.2209736502540001</v>
+      </c>
+    </row>
+    <row r="65" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C65">
+        <v>1.2204000000040001</v>
+      </c>
+      <c r="D65">
+        <v>1.2204000000040001</v>
+      </c>
+    </row>
+    <row r="66" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C66">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="D66">
+        <v>0.92289895828400004</v>
+      </c>
+    </row>
+    <row r="67" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C67">
+        <v>0.61020000000200003</v>
+      </c>
+      <c r="D67">
+        <v>0.30520000000300002</v>
+      </c>
+    </row>
+    <row r="68" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C68">
+        <v>1.2204000000040001</v>
+      </c>
+      <c r="D68">
+        <v>1.2204000000040001</v>
+      </c>
+    </row>
+    <row r="69" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C69">
+        <v>0.61022222222400002</v>
+      </c>
+      <c r="D69">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="70" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C70">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="D70">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="71" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C71">
+        <v>1.5276068351000001</v>
+      </c>
+      <c r="D71">
+        <v>1.2204000000040001</v>
+      </c>
+    </row>
+    <row r="72" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C72">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="D72">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="73" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C73">
+        <v>1.2204000000040001</v>
+      </c>
+      <c r="D73">
+        <v>1.2204000000040001</v>
+      </c>
+    </row>
+    <row r="74" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C74">
+        <v>0.61020000000200003</v>
+      </c>
+      <c r="D74">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="75" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C75">
+        <v>0.61020000000200003</v>
+      </c>
+      <c r="D75">
+        <v>1.3364599372699999</v>
+      </c>
+    </row>
+    <row r="76" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C76">
+        <v>0.915326595774</v>
+      </c>
+      <c r="D76">
+        <v>1.323053183736</v>
+      </c>
+    </row>
+    <row r="77" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C77">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="D77">
+        <v>0.61020000000200003</v>
+      </c>
+    </row>
+    <row r="78" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C78">
+        <v>1.5255000000050001</v>
+      </c>
+      <c r="D78">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="79" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C79">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="D79">
+        <v>1.2204000000040001</v>
+      </c>
+    </row>
+    <row r="80" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C80">
+        <v>0.61020000000200003</v>
+      </c>
+      <c r="D80">
+        <v>0.61020000000200003</v>
+      </c>
+    </row>
+    <row r="81" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C81">
+        <v>1.5255000000050001</v>
+      </c>
+      <c r="D81">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="82" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C82">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="D82">
+        <v>0.61020000000200003</v>
+      </c>
+    </row>
+    <row r="83" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C83">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="D83">
+        <v>0.61084038065199997</v>
+      </c>
+    </row>
+    <row r="84" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C84">
+        <v>1.2204000000040001</v>
+      </c>
+      <c r="D84">
+        <v>0.61020000000200003</v>
+      </c>
+    </row>
+    <row r="85" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C85">
+        <v>0.30510000000100002</v>
+      </c>
+      <c r="D85">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="86" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C86">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="D86">
+        <v>0.61020000000200003</v>
+      </c>
+    </row>
+    <row r="87" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C87">
+        <v>0.61020000000200003</v>
+      </c>
+      <c r="D87">
+        <v>0.30510000000100002</v>
+      </c>
+    </row>
+    <row r="88" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C88">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="D88">
+        <v>0.30510000000100002</v>
+      </c>
+    </row>
+    <row r="89" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C89">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="D89">
+        <v>0.61020000000200003</v>
+      </c>
+    </row>
+    <row r="90" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C90">
+        <v>1.5255000000050001</v>
+      </c>
+      <c r="D90">
+        <v>1.2204000000040001</v>
+      </c>
+    </row>
+    <row r="91" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C91">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="D91">
+        <v>1.5384070988680001</v>
+      </c>
+    </row>
+    <row r="92" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C92">
+        <v>0.30510000000100002</v>
+      </c>
+      <c r="D92">
+        <v>1.2204000000040001</v>
+      </c>
+    </row>
+    <row r="93" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C93">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="D93">
+        <v>1.2204000000040001</v>
+      </c>
+    </row>
+    <row r="94" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C94">
+        <v>1.220600000008</v>
+      </c>
+      <c r="D94">
+        <v>0.61020000000200003</v>
+      </c>
+    </row>
+    <row r="95" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C95">
+        <v>1.2210915012470001</v>
+      </c>
+      <c r="D95">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="96" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C96">
+        <v>0.30510000000100002</v>
+      </c>
+      <c r="D96">
+        <v>0.61020000000200003</v>
+      </c>
+    </row>
+    <row r="97" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C97">
+        <v>0.30511111111200001</v>
+      </c>
+      <c r="D97">
+        <v>0.91550000000700005</v>
+      </c>
+    </row>
+    <row r="98" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C98">
+        <v>1.2204000000040001</v>
+      </c>
+      <c r="D98">
+        <v>0.61020000000200003</v>
+      </c>
+    </row>
+    <row r="99" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C99">
+        <v>0.30510000000100002</v>
+      </c>
+      <c r="D99">
+        <v>1.2204000000040001</v>
+      </c>
+    </row>
+    <row r="100" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C100">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="D100">
+        <v>0.61020000000200003</v>
+      </c>
+    </row>
+    <row r="101" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C101">
+        <v>0.98059810808299996</v>
+      </c>
+      <c r="D101">
+        <v>0.30510000000100002</v>
+      </c>
+    </row>
+    <row r="102" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C102" s="7">
+        <f>AVERAGE(C2:C101)</f>
+        <v>0.99138745213406054</v>
+      </c>
+      <c r="D102">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="103" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D103">
+        <v>0.91686666667000005</v>
+      </c>
+    </row>
+    <row r="104" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D104">
+        <v>0.61020000000200003</v>
+      </c>
+    </row>
+    <row r="105" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D105">
+        <v>1.5304000000060001</v>
+      </c>
+    </row>
+    <row r="106" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D106">
+        <v>0.61020000000200003</v>
+      </c>
+    </row>
+    <row r="107" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D107">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="108" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D108">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="109" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D109">
+        <v>0.61020000000200003</v>
+      </c>
+    </row>
+    <row r="110" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D110">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="111" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D111">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="112" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D112">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="113" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D113">
+        <v>0.61020000000200003</v>
+      </c>
+    </row>
+    <row r="114" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D114">
+        <v>0.61020000000200003</v>
+      </c>
+    </row>
+    <row r="115" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D115">
+        <v>1.2214198581310001</v>
+      </c>
+    </row>
+    <row r="116" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D116">
+        <v>0.30510000000100002</v>
+      </c>
+    </row>
+    <row r="117" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D117">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="118" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D118">
+        <v>1.2204000000040001</v>
+      </c>
+    </row>
+    <row r="119" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D119">
+        <v>0.61020000000200003</v>
+      </c>
+    </row>
+    <row r="120" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D120">
+        <v>0.61020000000200003</v>
+      </c>
+    </row>
+    <row r="121" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D121">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="122" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D122">
+        <v>0.71176666666900001</v>
+      </c>
+    </row>
+    <row r="123" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D123">
+        <v>1.2253000000050001</v>
+      </c>
+    </row>
+    <row r="124" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D124">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="125" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D125">
+        <v>0.91674478006500004</v>
+      </c>
+    </row>
+    <row r="126" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D126">
+        <v>0.61020000000200003</v>
+      </c>
+    </row>
+    <row r="127" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D127">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="128" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D128">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="129" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D129">
+        <v>1.2204000000040001</v>
+      </c>
+    </row>
+    <row r="130" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D130">
+        <v>1.2204000000040001</v>
+      </c>
+    </row>
+    <row r="131" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D131">
+        <v>1.2308922936190001</v>
+      </c>
+    </row>
+    <row r="132" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D132">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="133" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D133">
+        <v>1.2204000000040001</v>
+      </c>
+    </row>
+    <row r="134" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D134">
+        <v>1.221645148516</v>
+      </c>
+    </row>
+    <row r="135" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D135">
+        <v>1.2204000000040001</v>
+      </c>
+    </row>
+    <row r="136" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D136">
+        <v>1.2204000000040001</v>
+      </c>
+    </row>
+    <row r="137" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D137">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="138" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D138">
+        <v>0.61537386395000004</v>
+      </c>
+    </row>
+    <row r="139" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D139">
+        <v>0.30510000000100002</v>
+      </c>
+    </row>
+    <row r="140" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D140">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="141" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D141">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="142" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D142">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="143" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D143">
+        <v>0.93349356470199996</v>
+      </c>
+    </row>
+    <row r="144" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D144">
+        <v>0.61020000000200003</v>
+      </c>
+    </row>
+    <row r="145" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D145">
+        <v>1.5255000000050001</v>
+      </c>
+    </row>
+    <row r="146" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D146">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="147" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D147">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="148" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D148">
+        <v>0.30510000000100002</v>
+      </c>
+    </row>
+    <row r="149" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D149">
+        <v>0.30510000000100002</v>
+      </c>
+    </row>
+    <row r="150" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D150">
+        <v>0.61020000000200003</v>
+      </c>
+    </row>
+    <row r="151" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D151">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="152" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D152">
+        <v>0.61020000000200003</v>
+      </c>
+    </row>
+    <row r="153" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D153">
+        <v>1.2204000000040001</v>
+      </c>
+    </row>
+    <row r="154" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D154">
+        <v>1.2204000000040001</v>
+      </c>
+    </row>
+    <row r="155" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D155">
+        <v>0.93779698294799996</v>
+      </c>
+    </row>
+    <row r="156" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D156">
+        <v>1.2204000000040001</v>
+      </c>
+    </row>
+    <row r="157" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D157">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="158" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D158">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="159" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D159">
+        <v>0.91533333333599998</v>
+      </c>
+    </row>
+    <row r="160" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D160">
+        <v>1.2204000000040001</v>
+      </c>
+    </row>
+    <row r="161" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D161">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="162" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D162">
+        <v>1.5255000000050001</v>
+      </c>
+    </row>
+    <row r="163" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D163">
+        <v>0.91643363415099999</v>
+      </c>
+    </row>
+    <row r="164" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D164">
+        <v>1.2204000000040001</v>
+      </c>
+    </row>
+    <row r="165" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D165">
+        <v>1.2204000000040001</v>
+      </c>
+    </row>
+    <row r="166" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D166">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="167" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D167">
+        <v>0.61020000000200003</v>
+      </c>
+    </row>
+    <row r="168" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D168">
+        <v>0.30510000000100002</v>
+      </c>
+    </row>
+    <row r="169" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D169">
+        <v>1.2204000000040001</v>
+      </c>
+    </row>
+    <row r="170" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D170">
+        <v>0.61020000000200003</v>
+      </c>
+    </row>
+    <row r="171" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D171">
+        <v>0.91588086857700002</v>
+      </c>
+    </row>
+    <row r="172" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D172" s="7">
+        <f>AVERAGE(D2:D171)</f>
+        <v>0.88866890437745838</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DB14316-39CC-412C-A762-31F37CE381A2}">
+  <dimension ref="A1:D52"/>
+  <sheetViews>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="5">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2">
+        <v>0.60014688000000005</v>
+      </c>
+      <c r="D2">
+        <v>0.60007343999999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>0.90022031999999996</v>
+      </c>
+      <c r="D3">
+        <v>0.90011015999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>0.90022031999999996</v>
+      </c>
+      <c r="D4">
+        <v>0.90011015999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>0.90022031999999996</v>
+      </c>
+      <c r="D5">
+        <v>0.90011015999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>0.60014688000000005</v>
+      </c>
+      <c r="D6">
+        <v>0.60007343999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>0.90022031999999996</v>
+      </c>
+      <c r="D7">
+        <v>0.90011015999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>0.90022031999999996</v>
+      </c>
+      <c r="D8">
+        <v>0.90011015999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>0.90022031999999996</v>
+      </c>
+      <c r="D9">
+        <v>0.90011015999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>0.90022031999999996</v>
+      </c>
+      <c r="D10">
+        <v>0.90011015999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>0.60014688000000005</v>
+      </c>
+      <c r="D11">
+        <v>0.60007343999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>0.90022031999999996</v>
+      </c>
+      <c r="D12">
+        <v>0.90011015999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>0.90022031999999996</v>
+      </c>
+      <c r="D13">
+        <v>0.60007359999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>1.2002937600000001</v>
+      </c>
+      <c r="D14">
+        <v>1.2001468799999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>0.90022031999999996</v>
+      </c>
+      <c r="D15">
+        <v>0.90011015999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>0.90022031999999996</v>
+      </c>
+      <c r="D16">
+        <v>0.90011015999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>0.90022031999999996</v>
+      </c>
+      <c r="D17">
+        <v>0.90011015999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>1.2002937600000001</v>
+      </c>
+      <c r="D18">
+        <v>1.2001468799999999</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>0.90022031999999996</v>
+      </c>
+      <c r="D19">
+        <v>0.90011015999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>0.60014688000000005</v>
+      </c>
+      <c r="D20">
+        <v>0.60007343999999996</v>
+      </c>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>0.90022031999999996</v>
+      </c>
+      <c r="D21">
+        <v>0.90011015999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>0.90022080000000004</v>
+      </c>
+      <c r="D22">
+        <v>0.90011039999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <v>0.90022031999999996</v>
+      </c>
+      <c r="D23">
+        <v>0.90011015999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <v>0.60014688000000005</v>
+      </c>
+      <c r="D24">
+        <v>0.60007343999999996</v>
+      </c>
+    </row>
+    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <v>0.90022031999999996</v>
+      </c>
+      <c r="D25">
+        <v>0.90011015999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>0.90022031999999996</v>
+      </c>
+      <c r="D26">
+        <v>0.90011015999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <v>0.90022031999999996</v>
+      </c>
+      <c r="D27">
+        <v>0.90011015999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <v>0.90022031999999996</v>
+      </c>
+      <c r="D28">
+        <v>0.90011015999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <v>1.2002937600000001</v>
+      </c>
+      <c r="D29">
+        <v>1.2001468799999999</v>
+      </c>
+    </row>
+    <row r="30" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <v>0.90022031999999996</v>
+      </c>
+      <c r="D30">
+        <v>0.90011015999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <v>0.90022031999999996</v>
+      </c>
+      <c r="D31">
+        <v>0.90011015999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C32">
+        <v>0.90022031999999996</v>
+      </c>
+      <c r="D32">
+        <v>0.90011015999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C33">
+        <v>0.90022031999999996</v>
+      </c>
+      <c r="D33">
+        <v>0.90011015999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C34">
+        <v>0.90022031999999996</v>
+      </c>
+      <c r="D34">
+        <v>0.90011015999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C35">
+        <v>0.90022031999999996</v>
+      </c>
+      <c r="D35">
+        <v>0.90011015999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C36">
+        <v>0.60014688000000005</v>
+      </c>
+      <c r="D36">
+        <v>0.60007343999999996</v>
+      </c>
+    </row>
+    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C37">
+        <v>0.60014688000000005</v>
+      </c>
+      <c r="D37">
+        <v>0.60007343999999996</v>
+      </c>
+    </row>
+    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C38">
+        <v>0.90022031999999996</v>
+      </c>
+      <c r="D38">
+        <v>0.90011015999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C39">
+        <v>0.90022031999999996</v>
+      </c>
+      <c r="D39">
+        <v>0.90011015999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C40">
+        <v>0.90022031999999996</v>
+      </c>
+      <c r="D40">
+        <v>0.90011015999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C41">
+        <v>0.90022031999999996</v>
+      </c>
+      <c r="D41">
+        <v>0.90011015999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C42">
+        <v>0.90022031999999996</v>
+      </c>
+      <c r="D42">
+        <v>0.90011015999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C43">
+        <v>0.90022031999999996</v>
+      </c>
+      <c r="D43">
+        <v>0.90011015999999999</v>
+      </c>
+    </row>
+    <row r="44" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C44">
+        <v>0.60014688000000005</v>
+      </c>
+      <c r="D44">
+        <v>0.60007343999999996</v>
+      </c>
+    </row>
+    <row r="45" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C45">
+        <v>0.90022031999999996</v>
+      </c>
+      <c r="D45">
+        <v>0.90011015999999999</v>
+      </c>
+    </row>
+    <row r="46" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C46">
+        <v>0.90022080000000004</v>
+      </c>
+      <c r="D46">
+        <v>0.90011039999999998</v>
+      </c>
+    </row>
+    <row r="47" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C47">
+        <v>0.90022031999999996</v>
+      </c>
+      <c r="D47">
+        <v>0.90011015999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C48">
+        <v>0.90022031999999996</v>
+      </c>
+      <c r="D48">
+        <v>0.90011015999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C49">
+        <v>0.60014688000000005</v>
+      </c>
+      <c r="D49">
+        <v>0.60007343999999996</v>
+      </c>
+    </row>
+    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C50">
+        <v>0.60014688000000005</v>
+      </c>
+      <c r="D50">
+        <v>0.60007343999999996</v>
+      </c>
+    </row>
+    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C51">
+        <v>0.90022031999999996</v>
+      </c>
+      <c r="D51">
+        <v>0.90011015999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C52" s="7">
+        <f>AVERAGE(C2:C51)</f>
+        <v>0.85821005760000002</v>
+      </c>
+      <c r="D52" s="7">
+        <f>AVERAGE(D2:D51)</f>
+        <v>0.85210429759999984</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B2ED3A6-0B67-444E-AD81-36D910E53853}">
+  <dimension ref="D5:D54"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="5" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>0.30510000000100002</v>
+      </c>
+    </row>
+    <row r="6" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>0.30510000000100002</v>
+      </c>
+    </row>
+    <row r="7" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>0.30510000000100002</v>
+      </c>
+    </row>
+    <row r="8" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>0.30510000000100002</v>
+      </c>
+    </row>
+    <row r="9" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>0.30510000000100002</v>
+      </c>
+    </row>
+    <row r="10" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>0.30510000000100002</v>
+      </c>
+    </row>
+    <row r="11" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>0.30510000000100002</v>
+      </c>
+    </row>
+    <row r="12" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>0.30510000000100002</v>
+      </c>
+    </row>
+    <row r="13" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <v>0.30510000000100002</v>
+      </c>
+    </row>
+    <row r="14" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>0.30510000000100002</v>
+      </c>
+    </row>
+    <row r="15" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <v>0.30510000000100002</v>
+      </c>
+    </row>
+    <row r="16" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>0.30510000000100002</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>0.30510000000100002</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <v>0.30510000000100002</v>
+      </c>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <v>0.30511111111200001</v>
+      </c>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <v>0.61020000000200003</v>
+      </c>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <v>0.61020000000200003</v>
+      </c>
+    </row>
+    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <v>0.61020000000200003</v>
+      </c>
+    </row>
+    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D23">
+        <v>0.61020000000200003</v>
+      </c>
+    </row>
+    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <v>0.61020000000200003</v>
+      </c>
+    </row>
+    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <v>0.61020000000200003</v>
+      </c>
+    </row>
+    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <v>0.61020000000200003</v>
+      </c>
+    </row>
+    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D27">
+        <v>0.61020000000200003</v>
+      </c>
+    </row>
+    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D28">
+        <v>0.61020000000200003</v>
+      </c>
+    </row>
+    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D29">
+        <v>0.61020000000200003</v>
+      </c>
+    </row>
+    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D30">
+        <v>0.61020000000200003</v>
+      </c>
+    </row>
+    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D31">
+        <v>0.61020000000200003</v>
+      </c>
+    </row>
+    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D32">
+        <v>0.61020000000200003</v>
+      </c>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D33">
+        <v>0.61020000000200003</v>
+      </c>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D34">
+        <v>0.61020000000200003</v>
+      </c>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D35">
+        <v>0.61020000000200003</v>
+      </c>
+    </row>
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D36">
+        <v>0.61020000000200003</v>
+      </c>
+    </row>
+    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D37">
+        <v>0.61293325438599999</v>
+      </c>
+    </row>
+    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D38">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D39">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D40">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D41">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D42">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D43">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D44">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D45">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D46">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D47">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D48">
+        <v>0.91530000000300005</v>
+      </c>
+    </row>
+    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D49">
+        <v>1.2204000000040001</v>
+      </c>
+    </row>
+    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D50">
+        <v>1.2204000000040001</v>
+      </c>
+    </row>
+    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D51">
+        <v>1.2204000000040001</v>
+      </c>
+    </row>
+    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D52">
+        <v>1.2204000000040001</v>
+      </c>
+    </row>
+    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D53">
+        <v>1.2204000000040001</v>
+      </c>
+    </row>
+    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D54">
+        <v>1.2204000000040001</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D5:D54">
+    <sortCondition ref="D5"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated simulation extractor(it can extract multiple decimal detection time)
</commit_message>
<xml_diff>
--- a/Data Collection.xlsx
+++ b/Data Collection.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yoga\Desktop\University\Thesis\TrustChain-Simulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{193BE576-C808-4518-8404-6E0EFE464B83}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64E3C543-061A-47F7-9619-3D83460A81FB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BCACAF04-D4C4-41AE-BAB0-4F6EFB70057E}"/>
+    <workbookView xWindow="3495" yWindow="1320" windowWidth="21600" windowHeight="11385" xr2:uid="{BCACAF04-D4C4-41AE-BAB0-4F6EFB70057E}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Planning" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="29">
   <si>
     <t>Evil Node Sleeping Transactions</t>
   </si>
@@ -122,9 +122,6 @@
   </si>
   <si>
     <t>3 - Transmission speed</t>
-  </si>
-  <si>
-    <t>To compute</t>
   </si>
   <si>
     <t>t student (non normal)</t>
@@ -1324,7 +1321,7 @@
   <dimension ref="A1:P38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1741,7 +1738,7 @@
         <v>50</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -2250,7 +2247,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF874DAA-691A-4835-ACA3-DB30922CFD6B}">
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
@@ -3035,7 +3032,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A8ADDF3-F6DC-49DE-90F6-6F07047D1F12}">
   <dimension ref="A1:D172"/>
   <sheetViews>
-    <sheetView topLeftCell="A136" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D172" sqref="D172"/>
     </sheetView>
   </sheetViews>
@@ -4381,12 +4378,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DB14316-39CC-412C-A762-31F37CE381A2}">
   <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4405,8 +4403,8 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>28</v>
+      <c r="B2">
+        <v>9.0206898844950008</v>
       </c>
       <c r="C2">
         <v>0.60014688000000005</v>
@@ -4416,6 +4414,9 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>8.1138732029790006</v>
+      </c>
       <c r="C3">
         <v>0.90022031999999996</v>
       </c>
@@ -4424,6 +4425,9 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>86.067229126341999</v>
+      </c>
       <c r="C4">
         <v>0.90022031999999996</v>
       </c>
@@ -4432,6 +4436,9 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>54.070096199817002</v>
+      </c>
       <c r="C5">
         <v>0.90022031999999996</v>
       </c>
@@ -4440,6 +4447,9 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>14.367122357386</v>
+      </c>
       <c r="C6">
         <v>0.60014688000000005</v>
       </c>
@@ -4448,6 +4458,9 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>12.070704133185</v>
+      </c>
       <c r="C7">
         <v>0.90022031999999996</v>
       </c>
@@ -4456,6 +4469,9 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>18.447748734832</v>
+      </c>
       <c r="C8">
         <v>0.90022031999999996</v>
       </c>
@@ -4464,6 +4480,9 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>23.197372250868</v>
+      </c>
       <c r="C9">
         <v>0.90022031999999996</v>
       </c>
@@ -4472,6 +4491,9 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>44.948244063537999</v>
+      </c>
       <c r="C10">
         <v>0.90022031999999996</v>
       </c>
@@ -4480,6 +4502,9 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>57.710943001135</v>
+      </c>
       <c r="C11">
         <v>0.60014688000000005</v>
       </c>
@@ -4488,6 +4513,9 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>24.943014619688</v>
+      </c>
       <c r="C12">
         <v>0.90022031999999996</v>
       </c>
@@ -4496,6 +4524,9 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>72.021443379562996</v>
+      </c>
       <c r="C13">
         <v>0.90022031999999996</v>
       </c>
@@ -4504,6 +4535,9 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>13.29247041627</v>
+      </c>
       <c r="C14">
         <v>1.2002937600000001</v>
       </c>
@@ -4512,6 +4546,9 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>49.968599852063001</v>
+      </c>
       <c r="C15">
         <v>0.90022031999999996</v>
       </c>
@@ -4520,6 +4557,9 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>12.860552572982</v>
+      </c>
       <c r="C16">
         <v>0.90022031999999996</v>
       </c>
@@ -4527,7 +4567,10 @@
         <v>0.90011015999999999</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>60.394606775823</v>
+      </c>
       <c r="C17">
         <v>0.90022031999999996</v>
       </c>
@@ -4535,7 +4578,10 @@
         <v>0.90011015999999999</v>
       </c>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>39.426105506888</v>
+      </c>
       <c r="C18">
         <v>1.2002937600000001</v>
       </c>
@@ -4543,7 +4589,10 @@
         <v>1.2001468799999999</v>
       </c>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>3.972</v>
+      </c>
       <c r="C19">
         <v>0.90022031999999996</v>
       </c>
@@ -4551,7 +4600,10 @@
         <v>0.90011015999999999</v>
       </c>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>9.0575738742429994</v>
+      </c>
       <c r="C20">
         <v>0.60014688000000005</v>
       </c>
@@ -4559,7 +4611,10 @@
         <v>0.60007343999999996</v>
       </c>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>13.397505731812</v>
+      </c>
       <c r="C21">
         <v>0.90022031999999996</v>
       </c>
@@ -4567,7 +4622,10 @@
         <v>0.90011015999999999</v>
       </c>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>143.93527849712899</v>
+      </c>
       <c r="C22">
         <v>0.90022080000000004</v>
       </c>
@@ -4575,7 +4633,10 @@
         <v>0.90011039999999998</v>
       </c>
     </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>55.563554033761001</v>
+      </c>
       <c r="C23">
         <v>0.90022031999999996</v>
       </c>
@@ -4583,7 +4644,10 @@
         <v>0.90011015999999999</v>
       </c>
     </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>93.640797061903996</v>
+      </c>
       <c r="C24">
         <v>0.60014688000000005</v>
       </c>
@@ -4591,7 +4655,10 @@
         <v>0.60007343999999996</v>
       </c>
     </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>32.155406817093997</v>
+      </c>
       <c r="C25">
         <v>0.90022031999999996</v>
       </c>
@@ -4599,7 +4666,10 @@
         <v>0.90011015999999999</v>
       </c>
     </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>18.171900619224999</v>
+      </c>
       <c r="C26">
         <v>0.90022031999999996</v>
       </c>
@@ -4607,7 +4677,10 @@
         <v>0.90011015999999999</v>
       </c>
     </row>
-    <row r="27" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>9.5322335704780006</v>
+      </c>
       <c r="C27">
         <v>0.90022031999999996</v>
       </c>
@@ -4615,7 +4688,10 @@
         <v>0.90011015999999999</v>
       </c>
     </row>
-    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>12.720240520995</v>
+      </c>
       <c r="C28">
         <v>0.90022031999999996</v>
       </c>
@@ -4623,7 +4699,10 @@
         <v>0.90011015999999999</v>
       </c>
     </row>
-    <row r="29" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>8.3306891203820008</v>
+      </c>
       <c r="C29">
         <v>1.2002937600000001</v>
       </c>
@@ -4631,7 +4710,10 @@
         <v>1.2001468799999999</v>
       </c>
     </row>
-    <row r="30" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>23.585135122760999</v>
+      </c>
       <c r="C30">
         <v>0.90022031999999996</v>
       </c>
@@ -4639,7 +4721,10 @@
         <v>0.90011015999999999</v>
       </c>
     </row>
-    <row r="31" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>48.680945211054997</v>
+      </c>
       <c r="C31">
         <v>0.90022031999999996</v>
       </c>
@@ -4647,7 +4732,10 @@
         <v>0.90011015999999999</v>
       </c>
     </row>
-    <row r="32" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>14.783931176242</v>
+      </c>
       <c r="C32">
         <v>0.90022031999999996</v>
       </c>
@@ -4655,7 +4743,10 @@
         <v>0.90011015999999999</v>
       </c>
     </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>11.740539271312</v>
+      </c>
       <c r="C33">
         <v>0.90022031999999996</v>
       </c>
@@ -4663,7 +4754,10 @@
         <v>0.90011015999999999</v>
       </c>
     </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>9.730876510621</v>
+      </c>
       <c r="C34">
         <v>0.90022031999999996</v>
       </c>
@@ -4671,7 +4765,10 @@
         <v>0.90011015999999999</v>
       </c>
     </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>13.138436714696001</v>
+      </c>
       <c r="C35">
         <v>0.90022031999999996</v>
       </c>
@@ -4679,7 +4776,10 @@
         <v>0.90011015999999999</v>
       </c>
     </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>16.969290059820999</v>
+      </c>
       <c r="C36">
         <v>0.60014688000000005</v>
       </c>
@@ -4687,7 +4787,10 @@
         <v>0.60007343999999996</v>
       </c>
     </row>
-    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>8.1146932180049998</v>
+      </c>
       <c r="C37">
         <v>0.60014688000000005</v>
       </c>
@@ -4695,7 +4798,10 @@
         <v>0.60007343999999996</v>
       </c>
     </row>
-    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>80.001357786857</v>
+      </c>
       <c r="C38">
         <v>0.90022031999999996</v>
       </c>
@@ -4703,7 +4809,10 @@
         <v>0.90011015999999999</v>
       </c>
     </row>
-    <row r="39" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>58.296201882939002</v>
+      </c>
       <c r="C39">
         <v>0.90022031999999996</v>
       </c>
@@ -4711,7 +4820,10 @@
         <v>0.90011015999999999</v>
       </c>
     </row>
-    <row r="40" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>14.434934680985</v>
+      </c>
       <c r="C40">
         <v>0.90022031999999996</v>
       </c>
@@ -4719,7 +4831,10 @@
         <v>0.90011015999999999</v>
       </c>
     </row>
-    <row r="41" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>8.3342570105539995</v>
+      </c>
       <c r="C41">
         <v>0.90022031999999996</v>
       </c>
@@ -4727,7 +4842,10 @@
         <v>0.90011015999999999</v>
       </c>
     </row>
-    <row r="42" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>26.973621089051999</v>
+      </c>
       <c r="C42">
         <v>0.90022031999999996</v>
       </c>
@@ -4735,7 +4853,10 @@
         <v>0.90011015999999999</v>
       </c>
     </row>
-    <row r="43" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>28.607744638524</v>
+      </c>
       <c r="C43">
         <v>0.90022031999999996</v>
       </c>
@@ -4743,7 +4864,10 @@
         <v>0.90011015999999999</v>
       </c>
     </row>
-    <row r="44" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>12.721196538475001</v>
+      </c>
       <c r="C44">
         <v>0.60014688000000005</v>
       </c>
@@ -4751,7 +4875,10 @@
         <v>0.60007343999999996</v>
       </c>
     </row>
-    <row r="45" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <v>8.1412469709550006</v>
+      </c>
       <c r="C45">
         <v>0.90022031999999996</v>
       </c>
@@ -4759,7 +4886,10 @@
         <v>0.90011015999999999</v>
       </c>
     </row>
-    <row r="46" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <v>23.976391888582999</v>
+      </c>
       <c r="C46">
         <v>0.90022080000000004</v>
       </c>
@@ -4767,7 +4897,10 @@
         <v>0.90011039999999998</v>
       </c>
     </row>
-    <row r="47" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <v>32.661469806021003</v>
+      </c>
       <c r="C47">
         <v>0.90022031999999996</v>
       </c>
@@ -4775,7 +4908,10 @@
         <v>0.90011015999999999</v>
       </c>
     </row>
-    <row r="48" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B48">
+        <v>39.767233249124999</v>
+      </c>
       <c r="C48">
         <v>0.90022031999999996</v>
       </c>
@@ -4783,7 +4919,10 @@
         <v>0.90011015999999999</v>
       </c>
     </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <v>10.544</v>
+      </c>
       <c r="C49">
         <v>0.60014688000000005</v>
       </c>
@@ -4791,7 +4930,10 @@
         <v>0.60007343999999996</v>
       </c>
     </row>
-    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B50">
+        <v>14.722160793601001</v>
+      </c>
       <c r="C50">
         <v>0.60014688000000005</v>
       </c>
@@ -4799,7 +4941,10 @@
         <v>0.60007343999999996</v>
       </c>
     </row>
-    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B51">
+        <v>10.594007882210001</v>
+      </c>
       <c r="C51">
         <v>0.90022031999999996</v>
       </c>
@@ -4807,7 +4952,11 @@
         <v>0.90011015999999999</v>
       </c>
     </row>
-    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B52" s="7">
+        <f>AVERAGE(B3:B51)</f>
+        <v>30.793815868219912</v>
+      </c>
       <c r="C52" s="7">
         <f>AVERAGE(C2:C51)</f>
         <v>0.85821005760000002</v>

</xml_diff>

<commit_message>
code cleaning, data collection
</commit_message>
<xml_diff>
--- a/Data Collection.xlsx
+++ b/Data Collection.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yoga\Desktop\University\Thesis\TrustChain-Simulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA4AE4C-33FB-4C61-B648-DBF19A10D496}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{968F1CBC-7C0B-4570-8C62-809CAE204CE9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{BCACAF04-D4C4-41AE-BAB0-4F6EFB70057E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{BCACAF04-D4C4-41AE-BAB0-4F6EFB70057E}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Planning" sheetId="3" r:id="rId1"/>
@@ -18,18 +18,13 @@
     <sheet name="Set2" sheetId="6" r:id="rId3"/>
     <sheet name="Set3" sheetId="7" r:id="rId4"/>
     <sheet name="Set4" sheetId="5" r:id="rId5"/>
+    <sheet name="Set6" sheetId="8" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'Set4'!$E$4</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'Set4'!$E$5:$E$54</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">'Set4'!$E$61</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'Set4'!$E$62:$E$161</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">'Set4'!$E$4</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">'Set4'!$E$5:$E$54</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'Set4'!$E$61</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'Set4'!$E$62:$E$161</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'Set4'!$E$4</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'Set4'!$E$5:$E$54</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">'Set4'!$E$61</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">'Set4'!$E$62:$E$161</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="54">
   <si>
     <t>Evil Node Sleeping Transactions</t>
   </si>
@@ -112,9 +107,6 @@
     <t>Learn stat tests</t>
   </si>
   <si>
-    <t>()</t>
-  </si>
-  <si>
     <t>Run simulations</t>
   </si>
   <si>
@@ -137,9 +129,6 @@
   </si>
   <si>
     <t>4 - Normalization Test</t>
-  </si>
-  <si>
-    <t>5 - Delay Variation</t>
   </si>
   <si>
     <t>AVG</t>
@@ -189,12 +178,39 @@
   <si>
     <t>SET4.1</t>
   </si>
+  <si>
+    <t>2.5 Min</t>
+  </si>
+  <si>
+    <t>Extra</t>
+  </si>
+  <si>
+    <t>5 - Test execution time</t>
+  </si>
+  <si>
+    <t>6 - Delay variation</t>
+  </si>
+  <si>
+    <t>1ms</t>
+  </si>
+  <si>
+    <t>10ms</t>
+  </si>
+  <si>
+    <t>1000ms</t>
+  </si>
+  <si>
+    <t>10000ms</t>
+  </si>
+  <si>
+    <t>7 - Initial Transaction</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -263,8 +279,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -294,6 +324,17 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
@@ -354,7 +395,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -362,8 +403,10 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -387,8 +430,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="7" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="7"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="8" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
+    <cellStyle name="60% - Accent6" xfId="8" builtinId="52"/>
+    <cellStyle name="Accent1" xfId="7" builtinId="29"/>
     <cellStyle name="Calculation" xfId="4" builtinId="22"/>
     <cellStyle name="Check Cell" xfId="5" builtinId="23"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -1079,12 +1130,12 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-GB" sz="1800" b="0" i="0" baseline="0">
+              <a:rPr lang="en-GB" sz="1400" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
               <a:t>Normal Q-Q Plot</a:t>
             </a:r>
-            <a:endParaRPr lang="en-GB">
+            <a:endParaRPr lang="en-GB" sz="1400">
               <a:effectLst/>
             </a:endParaRPr>
           </a:p>
@@ -1985,7 +2036,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.1</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -2023,7 +2074,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{00000000-BA23-47F0-8325-162A3EB2469F}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.0</cx:f>
+              <cx:f>_xlchart.v1.2</cx:f>
               <cx:v>Standardized </cx:v>
             </cx:txData>
           </cx:tx>
@@ -2051,7 +2102,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.5</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -2089,7 +2140,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{00000000-92AE-4E86-80B1-3A198ACB5431}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.4</cx:f>
+              <cx:f>_xlchart.v1.0</cx:f>
               <cx:v>Standardized </cx:v>
             </cx:txData>
           </cx:tx>
@@ -4852,15 +4903,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4891D42F-3971-43B5-986A-C0853C8465A0}">
-  <dimension ref="A1:P38"/>
+  <dimension ref="A1:S39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B22" sqref="A22:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
@@ -4874,13 +4925,13 @@
     <col min="12" max="12" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="22.28515625" customWidth="1"/>
     <col min="14" max="14" width="28" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="37.7109375" customWidth="1"/>
+    <col min="15" max="15" width="18.7109375" customWidth="1"/>
     <col min="19" max="19" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -4919,12 +4970,15 @@
         <v>11</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
@@ -4965,7 +5019,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="B3" s="4">
         <v>2</v>
@@ -4978,7 +5032,7 @@
         <v>0.13695052585936646</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" ref="E3:E14" si="0">LN(C3)/(C3)</f>
+        <f t="shared" ref="E3:E27" si="0">LN(C3)/(C3)</f>
         <v>0.14978661367769955</v>
       </c>
       <c r="F3" s="1">
@@ -5005,11 +5059,8 @@
       <c r="M3" s="1">
         <v>50</v>
       </c>
-      <c r="O3" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="4">
         <v>3</v>
@@ -5018,7 +5069,7 @@
         <v>50</v>
       </c>
       <c r="D4" s="1">
-        <f t="shared" ref="D4:D14" si="1">2*LOG(C4)/(C4-1)</f>
+        <f t="shared" ref="D4:D27" si="1">2*LOG(C4)/(C4-1)</f>
         <v>6.9345714462694649E-2</v>
       </c>
       <c r="E4" s="1">
@@ -5049,12 +5100,12 @@
       <c r="M4" s="1">
         <v>50</v>
       </c>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1" t="s">
+      <c r="P4" s="1"/>
+      <c r="S4" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="11"/>
       <c r="B5" s="4">
         <v>4</v>
@@ -5094,11 +5145,9 @@
       <c r="M5" s="1">
         <v>50</v>
       </c>
-      <c r="O5" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S5" s="1"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
       <c r="B6" s="4">
         <v>5</v>
@@ -5139,11 +5188,11 @@
       <c r="M6" s="1">
         <v>50</v>
       </c>
-      <c r="O6" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S6" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
       <c r="B7" s="4">
         <v>6</v>
@@ -5181,13 +5230,13 @@
       <c r="M7" s="1">
         <v>50</v>
       </c>
-      <c r="O7" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S7" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" s="5">
         <v>1</v>
@@ -5227,11 +5276,11 @@
       <c r="M8" s="1">
         <v>50</v>
       </c>
-      <c r="O8" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S8" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="B9" s="5">
         <v>2</v>
@@ -5271,11 +5320,11 @@
       <c r="M9" s="1">
         <v>50</v>
       </c>
-      <c r="O9" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S9" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="B10" s="5">
         <v>3</v>
@@ -5315,10 +5364,13 @@
       <c r="M10" s="1">
         <v>50</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S10" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="6">
         <v>1</v>
@@ -5359,7 +5411,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="B12" s="6">
         <v>2</v>
@@ -5400,7 +5452,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6">
         <v>3</v>
@@ -5441,12 +5493,10 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="8">
-        <v>1</v>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="16"/>
+      <c r="B14" s="6">
+        <v>4</v>
       </c>
       <c r="C14" s="1">
         <v>100</v>
@@ -5460,39 +5510,35 @@
         <v>4.6051701859880917E-2</v>
       </c>
       <c r="F14" s="1">
-        <f>E14</f>
+        <v>4.7E-2</v>
+      </c>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+    </row>
+    <row r="15" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="16"/>
+      <c r="B15" s="6">
+        <v>5</v>
+      </c>
+      <c r="C15" s="1">
+        <v>100</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="1"/>
+        <v>4.0404040404040407E-2</v>
+      </c>
+      <c r="E15" s="1">
+        <f t="shared" si="0"/>
         <v>4.6051701859880917E-2</v>
       </c>
-      <c r="G14" s="1">
-        <v>2</v>
-      </c>
-      <c r="H14" s="1">
-        <v>100</v>
-      </c>
-      <c r="I14" s="1">
-        <v>1</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M14" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
+      <c r="F15" s="1">
+        <v>4.7E-2</v>
+      </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
@@ -5501,163 +5547,511 @@
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-    </row>
-    <row r="17" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-    </row>
-    <row r="18" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-    </row>
-    <row r="19" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-    </row>
-    <row r="20" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
-    </row>
-    <row r="21" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-    </row>
-    <row r="22" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-    </row>
-    <row r="23" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-    </row>
-    <row r="24" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
-    </row>
-    <row r="25" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
-    </row>
-    <row r="26" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
-    </row>
-    <row r="27" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
-      <c r="L27" s="1"/>
-      <c r="M27" s="1"/>
-    </row>
-    <row r="28" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="8">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1">
+        <v>100</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="1"/>
+        <v>4.0404040404040407E-2</v>
+      </c>
+      <c r="E16" s="1">
+        <f t="shared" si="0"/>
+        <v>4.6051701859880917E-2</v>
+      </c>
+      <c r="F16" s="1">
+        <f>E16</f>
+        <v>4.6051701859880917E-2</v>
+      </c>
+      <c r="G16" s="1">
+        <v>2</v>
+      </c>
+      <c r="H16" s="1">
+        <v>100</v>
+      </c>
+      <c r="I16" s="1">
+        <v>1</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M16" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1">
+        <v>500</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" si="1"/>
+        <v>1.0817515047438954E-2</v>
+      </c>
+      <c r="E17" s="1">
+        <f t="shared" si="0"/>
+        <v>1.2429216196844383E-2</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1.243E-2</v>
+      </c>
+      <c r="G17" s="1">
+        <v>2</v>
+      </c>
+      <c r="H17" s="1">
+        <v>100</v>
+      </c>
+      <c r="I17" s="1">
+        <v>1</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M17" s="1">
+        <v>1</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="13">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1">
+        <v>100</v>
+      </c>
+      <c r="D18" s="1">
+        <f t="shared" si="1"/>
+        <v>4.0404040404040407E-2</v>
+      </c>
+      <c r="E18" s="1">
+        <f t="shared" si="0"/>
+        <v>4.6051701859880917E-2</v>
+      </c>
+      <c r="F18" s="1">
+        <v>4.7E-2</v>
+      </c>
+      <c r="G18" s="1">
+        <v>2</v>
+      </c>
+      <c r="H18" s="1">
+        <v>100</v>
+      </c>
+      <c r="I18" s="1">
+        <v>1</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M18" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="11"/>
+      <c r="B19" s="14">
+        <v>2</v>
+      </c>
+      <c r="C19" s="1">
+        <v>100</v>
+      </c>
+      <c r="D19" s="1">
+        <f t="shared" si="1"/>
+        <v>4.0404040404040407E-2</v>
+      </c>
+      <c r="E19" s="1">
+        <f t="shared" si="0"/>
+        <v>4.6051701859880917E-2</v>
+      </c>
+      <c r="F19" s="1">
+        <v>4.7E-2</v>
+      </c>
+      <c r="G19" s="1">
+        <v>2</v>
+      </c>
+      <c r="H19" s="1">
+        <v>100</v>
+      </c>
+      <c r="I19" s="1">
+        <v>1</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M19" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="11"/>
+      <c r="B20" s="13">
+        <v>3</v>
+      </c>
+      <c r="C20" s="1">
+        <v>100</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" si="1"/>
+        <v>4.0404040404040407E-2</v>
+      </c>
+      <c r="E20" s="1">
+        <f t="shared" si="0"/>
+        <v>4.6051701859880917E-2</v>
+      </c>
+      <c r="F20" s="1">
+        <v>4.7E-2</v>
+      </c>
+      <c r="G20" s="1">
+        <v>2</v>
+      </c>
+      <c r="H20" s="1">
+        <v>100</v>
+      </c>
+      <c r="I20" s="1">
+        <v>1</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M20" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="11"/>
+      <c r="B21" s="14">
+        <v>4</v>
+      </c>
+      <c r="C21" s="1">
+        <v>100</v>
+      </c>
+      <c r="D21" s="1">
+        <f t="shared" si="1"/>
+        <v>4.0404040404040407E-2</v>
+      </c>
+      <c r="E21" s="1">
+        <f t="shared" si="0"/>
+        <v>4.6051701859880917E-2</v>
+      </c>
+      <c r="F21" s="1">
+        <v>4.7E-2</v>
+      </c>
+      <c r="G21" s="1">
+        <v>2</v>
+      </c>
+      <c r="H21" s="1">
+        <v>100</v>
+      </c>
+      <c r="I21" s="1">
+        <v>1</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M21" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="11"/>
+      <c r="B22" s="13">
+        <v>5</v>
+      </c>
+      <c r="C22" s="1">
+        <v>100</v>
+      </c>
+      <c r="D22" s="1">
+        <f t="shared" si="1"/>
+        <v>4.0404040404040407E-2</v>
+      </c>
+      <c r="E22" s="1">
+        <f t="shared" si="0"/>
+        <v>4.6051701859880917E-2</v>
+      </c>
+      <c r="F22" s="1">
+        <v>4.7E-2</v>
+      </c>
+      <c r="G22" s="1">
+        <v>2</v>
+      </c>
+      <c r="H22" s="1">
+        <v>100</v>
+      </c>
+      <c r="I22" s="1">
+        <v>1</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M22" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" s="15">
+        <v>1</v>
+      </c>
+      <c r="C23" s="1">
+        <v>100</v>
+      </c>
+      <c r="D23" s="1">
+        <f>2*LOG(C23)/(C23-1)</f>
+        <v>4.0404040404040407E-2</v>
+      </c>
+      <c r="E23" s="1">
+        <f t="shared" si="0"/>
+        <v>4.6051701859880917E-2</v>
+      </c>
+      <c r="F23" s="1">
+        <v>4.7E-2</v>
+      </c>
+      <c r="G23" s="1">
+        <v>2</v>
+      </c>
+      <c r="H23" s="1">
+        <v>100</v>
+      </c>
+      <c r="I23" s="1">
+        <v>1</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M23" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="11"/>
+      <c r="B24" s="15">
+        <v>2</v>
+      </c>
+      <c r="C24" s="1">
+        <v>100</v>
+      </c>
+      <c r="D24" s="1">
+        <f t="shared" si="1"/>
+        <v>4.0404040404040407E-2</v>
+      </c>
+      <c r="E24" s="1">
+        <f t="shared" si="0"/>
+        <v>4.6051701859880917E-2</v>
+      </c>
+      <c r="F24" s="1">
+        <v>4.7E-2</v>
+      </c>
+      <c r="G24" s="1">
+        <v>4</v>
+      </c>
+      <c r="H24" s="1">
+        <v>100</v>
+      </c>
+      <c r="I24" s="1">
+        <v>1</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M24" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="11"/>
+      <c r="B25" s="15">
+        <v>3</v>
+      </c>
+      <c r="C25" s="1">
+        <v>100</v>
+      </c>
+      <c r="D25" s="1">
+        <f t="shared" si="1"/>
+        <v>4.0404040404040407E-2</v>
+      </c>
+      <c r="E25" s="1">
+        <f t="shared" si="0"/>
+        <v>4.6051701859880917E-2</v>
+      </c>
+      <c r="F25" s="1">
+        <v>4.7E-2</v>
+      </c>
+      <c r="G25" s="1">
+        <v>8</v>
+      </c>
+      <c r="H25" s="1">
+        <v>100</v>
+      </c>
+      <c r="I25" s="1">
+        <v>1</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M25" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="11"/>
+      <c r="B26" s="15">
+        <v>4</v>
+      </c>
+      <c r="C26" s="1">
+        <v>100</v>
+      </c>
+      <c r="D26" s="1">
+        <f t="shared" si="1"/>
+        <v>4.0404040404040407E-2</v>
+      </c>
+      <c r="E26" s="1">
+        <f t="shared" si="0"/>
+        <v>4.6051701859880917E-2</v>
+      </c>
+      <c r="F26" s="1">
+        <v>4.7E-2</v>
+      </c>
+      <c r="G26" s="1">
+        <v>16</v>
+      </c>
+      <c r="H26" s="1">
+        <v>100</v>
+      </c>
+      <c r="I26" s="1">
+        <v>1</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M26" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="11"/>
+      <c r="B27" s="15">
+        <v>5</v>
+      </c>
+      <c r="C27" s="1">
+        <v>100</v>
+      </c>
+      <c r="D27" s="1">
+        <f t="shared" si="1"/>
+        <v>4.0404040404040407E-2</v>
+      </c>
+      <c r="E27" s="1">
+        <f t="shared" si="0"/>
+        <v>4.6051701859880917E-2</v>
+      </c>
+      <c r="F27" s="1">
+        <v>4.7E-2</v>
+      </c>
+      <c r="G27" s="1">
+        <v>32</v>
+      </c>
+      <c r="H27" s="1">
+        <v>100</v>
+      </c>
+      <c r="I27" s="1">
+        <v>1</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M27" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -5670,7 +6064,7 @@
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
     </row>
-    <row r="29" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -5683,7 +6077,7 @@
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
     </row>
-    <row r="30" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
@@ -5696,7 +6090,7 @@
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
     </row>
-    <row r="31" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
@@ -5709,7 +6103,7 @@
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
     </row>
-    <row r="32" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -5800,11 +6194,26 @@
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
     </row>
+    <row r="39" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
+      <c r="L39" s="1"/>
+      <c r="M39" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A18:A22"/>
+    <mergeCell ref="A23:A27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5815,7 +6224,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF874DAA-691A-4835-ACA3-DB30922CFD6B}">
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
@@ -7944,10 +8353,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DB14316-39CC-412C-A762-31F37CE381A2}">
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7956,7 +8365,7 @@
     <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -7969,8 +8378,14 @@
       <c r="D1" s="5">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="5">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>9.0206898844950008</v>
       </c>
@@ -7981,7 +8396,7 @@
         <v>0.60007343999999996</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>8.1138732029790006</v>
       </c>
@@ -7992,7 +8407,7 @@
         <v>0.90011015999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>86.067229126341999</v>
       </c>
@@ -8003,7 +8418,7 @@
         <v>0.90011015999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>54.070096199817002</v>
       </c>
@@ -8014,7 +8429,7 @@
         <v>0.90011015999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>14.367122357386</v>
       </c>
@@ -8025,7 +8440,7 @@
         <v>0.60007343999999996</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>12.070704133185</v>
       </c>
@@ -8036,7 +8451,7 @@
         <v>0.90011015999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>18.447748734832</v>
       </c>
@@ -8047,7 +8462,7 @@
         <v>0.90011015999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>23.197372250868</v>
       </c>
@@ -8058,7 +8473,7 @@
         <v>0.90011015999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>44.948244063537999</v>
       </c>
@@ -8069,7 +8484,7 @@
         <v>0.90011015999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>57.710943001135</v>
       </c>
@@ -8080,7 +8495,7 @@
         <v>0.60007343999999996</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>24.943014619688</v>
       </c>
@@ -8091,7 +8506,7 @@
         <v>0.90011015999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>72.021443379562996</v>
       </c>
@@ -8102,7 +8517,7 @@
         <v>0.60007359999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>13.29247041627</v>
       </c>
@@ -8113,7 +8528,7 @@
         <v>1.2001468799999999</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>49.968599852063001</v>
       </c>
@@ -8124,7 +8539,7 @@
         <v>0.90011015999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>12.860552572982</v>
       </c>
@@ -8543,8 +8958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B2ED3A6-0B67-444E-AD81-36D910E53853}">
   <dimension ref="A1:S164"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D164" sqref="D164"/>
+    <sheetView topLeftCell="G4" workbookViewId="0">
+      <selection activeCell="W53" sqref="W53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8561,49 +8976,49 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B1" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B2" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="O2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" t="s">
         <v>31</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>32</v>
       </c>
-      <c r="D4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" t="s">
-        <v>34</v>
-      </c>
       <c r="O4" t="s">
+        <v>36</v>
+      </c>
+      <c r="P4" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>37</v>
+      </c>
+      <c r="R4" t="s">
         <v>38</v>
       </c>
-      <c r="P4" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q4" t="s">
+      <c r="S4" t="s">
         <v>39</v>
-      </c>
-      <c r="R4" t="s">
-        <v>40</v>
-      </c>
-      <c r="S4" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -8707,7 +9122,7 @@
         <v>-1.6448536269514726</v>
       </c>
       <c r="S7">
-        <f t="shared" ref="S7:S54" si="4">(P7-$P$55)/$P$56</f>
+        <f t="shared" ref="S7:S53" si="4">(P7-$P$55)/$P$56</f>
         <v>-2.3247457307844104</v>
       </c>
     </row>
@@ -10358,14 +10773,14 @@
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C55" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D55" s="7">
         <f>AVERAGE(D5:D54)</f>
         <v>0.91610186017854023</v>
       </c>
       <c r="O55" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="P55" s="7">
         <f>AVERAGE(P5:P54)</f>
@@ -10374,14 +10789,14 @@
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C56" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D56">
         <f>STDEV(D5:D54)</f>
         <v>0.26282524238527133</v>
       </c>
       <c r="O56" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="P56">
         <f>_xlfn.STDEV.S(P5:P54)</f>
@@ -10390,7 +10805,7 @@
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C57" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D57">
         <f>SKEW(D5:D54)</f>
@@ -10399,30 +10814,30 @@
     </row>
     <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D61" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E61" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="O61" t="s">
+        <v>36</v>
+      </c>
+      <c r="P61" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q61" t="s">
+        <v>37</v>
+      </c>
+      <c r="R61" t="s">
         <v>38</v>
       </c>
-      <c r="P61" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q61" t="s">
+      <c r="S61" t="s">
         <v>39</v>
-      </c>
-      <c r="R61" t="s">
-        <v>40</v>
-      </c>
-      <c r="S61" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
@@ -12195,15 +12610,15 @@
         <v>0.91570407199600001</v>
       </c>
       <c r="Q127">
-        <f t="shared" ref="Q127:Q163" si="11">(O127-0.5)/100</f>
+        <f t="shared" ref="Q127:Q160" si="11">(O127-0.5)/100</f>
         <v>0.65500000000000003</v>
       </c>
       <c r="R127">
-        <f t="shared" ref="R127:R163" si="12">_xlfn.NORM.S.INV(Q127)</f>
+        <f t="shared" ref="R127:R160" si="12">_xlfn.NORM.S.INV(Q127)</f>
         <v>0.39885506564233691</v>
       </c>
       <c r="S127">
-        <f t="shared" ref="S127:S163" si="13">STANDARDIZE(P127,$P$162,$P$163)</f>
+        <f t="shared" ref="S127:S160" si="13">STANDARDIZE(P127,$P$162,$P$163)</f>
         <v>4.1311977670285036E-2</v>
       </c>
     </row>
@@ -13127,14 +13542,14 @@
     </row>
     <row r="162" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C162" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D162" s="7">
         <f>AVERAGE(D62:D161)</f>
         <v>0.90449402464180051</v>
       </c>
       <c r="O162" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="P162" s="7">
         <f>AVERAGE(P62:P161)</f>
@@ -13143,14 +13558,14 @@
     </row>
     <row r="163" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C163" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D163">
         <f>STDEV(D62:D161)</f>
         <v>0.27135102181909121</v>
       </c>
       <c r="O163" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="P163">
         <f>STDEV(P62:P161)</f>
@@ -13159,7 +13574,7 @@
     </row>
     <row r="164" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C164" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D164">
         <f>SKEW(D62:D161)</f>
@@ -13177,4 +13592,1736 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BEB8E32-D847-46DD-A9C2-FCA6CC8CF645}">
+  <dimension ref="C1:G101"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C1" s="5">
+        <v>1</v>
+      </c>
+      <c r="D1" s="5">
+        <v>2</v>
+      </c>
+      <c r="E1" s="5">
+        <v>3</v>
+      </c>
+      <c r="F1" s="5">
+        <v>4</v>
+      </c>
+      <c r="G1" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>2.4300000003000002E-2</v>
+      </c>
+      <c r="D2">
+        <v>0.10696251452199999</v>
+      </c>
+      <c r="E2">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="F2">
+        <v>9.0153000000030001</v>
+      </c>
+      <c r="G2">
+        <v>90.015300000002995</v>
+      </c>
+    </row>
+    <row r="3" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>2.4644617290999999E-2</v>
+      </c>
+      <c r="D3">
+        <v>7.0200000001999996E-2</v>
+      </c>
+      <c r="E3">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="F3">
+        <v>6.0102000000020004</v>
+      </c>
+      <c r="G3">
+        <v>60.010200000002001</v>
+      </c>
+    </row>
+    <row r="4" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>1.6200000002E-2</v>
+      </c>
+      <c r="D4">
+        <v>0.14040000000399999</v>
+      </c>
+      <c r="E4">
+        <v>1.2204000000040001</v>
+      </c>
+      <c r="F4">
+        <v>6.0102000000020004</v>
+      </c>
+      <c r="G4">
+        <v>120.020444444448</v>
+      </c>
+    </row>
+    <row r="5" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>2.4300000003000002E-2</v>
+      </c>
+      <c r="D5">
+        <v>0.106950502157</v>
+      </c>
+      <c r="E5">
+        <v>0.61020000000200003</v>
+      </c>
+      <c r="F5">
+        <v>9.0153000000030001</v>
+      </c>
+      <c r="G5">
+        <v>120.020400000004</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>2.4300000003000002E-2</v>
+      </c>
+      <c r="D6">
+        <v>9.3533333336000002E-2</v>
+      </c>
+      <c r="E6">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="F6">
+        <v>9.0153000000030001</v>
+      </c>
+      <c r="G6">
+        <v>30.005100000001001</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>2.4300000003000002E-2</v>
+      </c>
+      <c r="D7">
+        <v>0.10530000000299999</v>
+      </c>
+      <c r="E7">
+        <v>0.30510000000100002</v>
+      </c>
+      <c r="F7">
+        <v>9.0168154843719996</v>
+      </c>
+      <c r="G7">
+        <v>60.010200000002001</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>3.2795122231E-2</v>
+      </c>
+      <c r="D8">
+        <v>0.14040000000399999</v>
+      </c>
+      <c r="E8">
+        <v>1.5506994742060001</v>
+      </c>
+      <c r="F8">
+        <v>12.020400000004001</v>
+      </c>
+      <c r="G8">
+        <v>90.015300000002995</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>3.2400000004E-2</v>
+      </c>
+      <c r="D9">
+        <v>0.10530000000299999</v>
+      </c>
+      <c r="E9">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="F9">
+        <v>12.020400000004001</v>
+      </c>
+      <c r="G9">
+        <v>90.015300000002995</v>
+      </c>
+    </row>
+    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>2.9633333336999999E-2</v>
+      </c>
+      <c r="D10">
+        <v>0.14040000000399999</v>
+      </c>
+      <c r="E10">
+        <v>0.61020000000200003</v>
+      </c>
+      <c r="F10">
+        <v>12.020400000004001</v>
+      </c>
+      <c r="G10">
+        <v>90.015300000002995</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>2.4300000003000002E-2</v>
+      </c>
+      <c r="D11">
+        <v>0.10530000000299999</v>
+      </c>
+      <c r="E11">
+        <v>0.91610358299899997</v>
+      </c>
+      <c r="F11">
+        <v>9.0153000000030001</v>
+      </c>
+      <c r="G11">
+        <v>90.015300000002995</v>
+      </c>
+    </row>
+    <row r="12" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>2.4300000003000002E-2</v>
+      </c>
+      <c r="D12">
+        <v>0.10530000000299999</v>
+      </c>
+      <c r="E12">
+        <v>1.221610090177</v>
+      </c>
+      <c r="F12">
+        <v>6.0102000000020004</v>
+      </c>
+      <c r="G12">
+        <v>60.010200000002001</v>
+      </c>
+    </row>
+    <row r="13" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>2.4300000003000002E-2</v>
+      </c>
+      <c r="D13">
+        <v>0.14040000000399999</v>
+      </c>
+      <c r="E13">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="F13">
+        <v>9.0153000000030001</v>
+      </c>
+      <c r="G13">
+        <v>90.015300000002995</v>
+      </c>
+    </row>
+    <row r="14" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>2.4300000003000002E-2</v>
+      </c>
+      <c r="D14">
+        <v>0.10530000000299999</v>
+      </c>
+      <c r="E14">
+        <v>0.91621382376299998</v>
+      </c>
+      <c r="F14">
+        <v>9.0153000000030001</v>
+      </c>
+      <c r="G14">
+        <v>90.015300000002995</v>
+      </c>
+    </row>
+    <row r="15" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>2.4300000003000002E-2</v>
+      </c>
+      <c r="D15">
+        <v>7.0200000001999996E-2</v>
+      </c>
+      <c r="E15">
+        <v>0.92268943506099999</v>
+      </c>
+      <c r="F15">
+        <v>12.020400000004001</v>
+      </c>
+      <c r="G15">
+        <v>120.020400000004</v>
+      </c>
+    </row>
+    <row r="16" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>2.5733333340000001E-2</v>
+      </c>
+      <c r="D16">
+        <v>0.14273731846599999</v>
+      </c>
+      <c r="E16">
+        <v>0.61020000000200003</v>
+      </c>
+      <c r="F16">
+        <v>6.0102000000020004</v>
+      </c>
+      <c r="G16">
+        <v>120.020400000004</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>2.4526741179999999E-2</v>
+      </c>
+      <c r="D17">
+        <v>0.10530000000299999</v>
+      </c>
+      <c r="E17">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="F17">
+        <v>9.0153000000030001</v>
+      </c>
+      <c r="G17">
+        <v>120.020400000004</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>2.696666667E-2</v>
+      </c>
+      <c r="D18">
+        <v>0.17580000001500001</v>
+      </c>
+      <c r="E18">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="F18">
+        <v>6.0102000000020004</v>
+      </c>
+      <c r="G18">
+        <v>90.015300000002995</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>1.6200000002E-2</v>
+      </c>
+      <c r="D19">
+        <v>0.14591726123400001</v>
+      </c>
+      <c r="E19">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="F19">
+        <v>9.0153333333360006</v>
+      </c>
+      <c r="G19">
+        <v>120.020400000004</v>
+      </c>
+    </row>
+    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>3.0300000003999999E-2</v>
+      </c>
+      <c r="D20">
+        <v>0.128088256648</v>
+      </c>
+      <c r="E20">
+        <v>1.2204000000040001</v>
+      </c>
+      <c r="F20">
+        <v>6.0102000000020004</v>
+      </c>
+      <c r="G20">
+        <v>60.010200000002001</v>
+      </c>
+    </row>
+    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>3.2400000004E-2</v>
+      </c>
+      <c r="D21">
+        <v>0.14040000000399999</v>
+      </c>
+      <c r="E21">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="F21">
+        <v>12.020444444448</v>
+      </c>
+      <c r="G21">
+        <v>90.015300000002995</v>
+      </c>
+    </row>
+    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>2.7000000002999999E-2</v>
+      </c>
+      <c r="D22">
+        <v>0.10530000000299999</v>
+      </c>
+      <c r="E22">
+        <v>0.30510000000100002</v>
+      </c>
+      <c r="F22">
+        <v>9.0153000000030001</v>
+      </c>
+      <c r="G22">
+        <v>90.015300000002995</v>
+      </c>
+    </row>
+    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <v>2.5933333342999999E-2</v>
+      </c>
+      <c r="D23">
+        <v>0.105471172073</v>
+      </c>
+      <c r="E23">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="F23">
+        <v>6.0102000000020004</v>
+      </c>
+      <c r="G23">
+        <v>90.015300000002995</v>
+      </c>
+    </row>
+    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <v>1.7533333341000001E-2</v>
+      </c>
+      <c r="D24">
+        <v>0.14044987923899999</v>
+      </c>
+      <c r="E24">
+        <v>1.2204000000040001</v>
+      </c>
+      <c r="F24">
+        <v>6.0102000000020004</v>
+      </c>
+      <c r="G24">
+        <v>90.015300000002995</v>
+      </c>
+    </row>
+    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <v>1.6200000002E-2</v>
+      </c>
+      <c r="D25">
+        <v>7.0200000001999996E-2</v>
+      </c>
+      <c r="E25">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="F25">
+        <v>9.0466619928219991</v>
+      </c>
+      <c r="G25">
+        <v>90.015300000002995</v>
+      </c>
+    </row>
+    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>2.4333333336000001E-2</v>
+      </c>
+      <c r="D26">
+        <v>0.140416466209</v>
+      </c>
+      <c r="E26">
+        <v>0.91572428847099996</v>
+      </c>
+      <c r="F26">
+        <v>9.0153000000030001</v>
+      </c>
+      <c r="G26">
+        <v>90.015300000002995</v>
+      </c>
+    </row>
+    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <v>2.4300000003000002E-2</v>
+      </c>
+      <c r="D27">
+        <v>0.14040000000399999</v>
+      </c>
+      <c r="E27">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="F27">
+        <v>12.020400000004001</v>
+      </c>
+      <c r="G27">
+        <v>60.010200000002001</v>
+      </c>
+    </row>
+    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <v>2.4300000003000002E-2</v>
+      </c>
+      <c r="D28">
+        <v>0.10530000000299999</v>
+      </c>
+      <c r="E28">
+        <v>0.91580119928699999</v>
+      </c>
+      <c r="F28">
+        <v>12.020400000004001</v>
+      </c>
+      <c r="G28">
+        <v>90.015300000002995</v>
+      </c>
+    </row>
+    <row r="29" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <v>1.8866666668999998E-2</v>
+      </c>
+      <c r="D29">
+        <v>7.0200000001999996E-2</v>
+      </c>
+      <c r="E29">
+        <v>1.220789647273</v>
+      </c>
+      <c r="F29">
+        <v>9.0153000000030001</v>
+      </c>
+      <c r="G29">
+        <v>90.015300000002995</v>
+      </c>
+    </row>
+    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <v>2.4300000003000002E-2</v>
+      </c>
+      <c r="D30">
+        <v>0.10530000000299999</v>
+      </c>
+      <c r="E30">
+        <v>1.2204000000040001</v>
+      </c>
+      <c r="F30">
+        <v>9.0153000000030001</v>
+      </c>
+      <c r="G30">
+        <v>90.015300000002995</v>
+      </c>
+    </row>
+    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <v>8.100000001E-3</v>
+      </c>
+      <c r="D31">
+        <v>0.10533333333600001</v>
+      </c>
+      <c r="E31">
+        <v>0.61020000000200003</v>
+      </c>
+      <c r="F31">
+        <v>9.0153000000030001</v>
+      </c>
+      <c r="G31">
+        <v>120.020400000004</v>
+      </c>
+    </row>
+    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C32">
+        <v>2.4754959478999999E-2</v>
+      </c>
+      <c r="D32">
+        <v>0.10530000000299999</v>
+      </c>
+      <c r="E32">
+        <v>0.91639452465600002</v>
+      </c>
+      <c r="F32">
+        <v>3.0051000000010002</v>
+      </c>
+      <c r="G32">
+        <v>120.020400000004</v>
+      </c>
+    </row>
+    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C33">
+        <v>3.1300000004000003E-2</v>
+      </c>
+      <c r="D33">
+        <v>0.10530000000299999</v>
+      </c>
+      <c r="E33">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="F33">
+        <v>12.020400000004001</v>
+      </c>
+      <c r="G33">
+        <v>120.020400000004</v>
+      </c>
+    </row>
+    <row r="34" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C34">
+        <v>2.4300000003000002E-2</v>
+      </c>
+      <c r="D34">
+        <v>0.10530000000299999</v>
+      </c>
+      <c r="E34">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="F34">
+        <v>9.0153000000030001</v>
+      </c>
+      <c r="G34">
+        <v>60.010200000002001</v>
+      </c>
+    </row>
+    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C35">
+        <v>1.6200000002E-2</v>
+      </c>
+      <c r="D35">
+        <v>7.0200000001999996E-2</v>
+      </c>
+      <c r="E35">
+        <v>0.91533333333599998</v>
+      </c>
+      <c r="F35">
+        <v>6.0102222222239998</v>
+      </c>
+      <c r="G35">
+        <v>60.010200000002001</v>
+      </c>
+    </row>
+    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C36">
+        <v>3.2300000003999997E-2</v>
+      </c>
+      <c r="D36">
+        <v>7.0200000001999996E-2</v>
+      </c>
+      <c r="E36">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="F36">
+        <v>9.0153000000030001</v>
+      </c>
+      <c r="G36">
+        <v>150.025500000005</v>
+      </c>
+    </row>
+    <row r="37" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C37">
+        <v>3.3600000009E-2</v>
+      </c>
+      <c r="D37">
+        <v>0.14070000001399999</v>
+      </c>
+      <c r="E37">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="F37">
+        <v>9.0153000000030001</v>
+      </c>
+      <c r="G37">
+        <v>90.015300000002995</v>
+      </c>
+    </row>
+    <row r="38" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C38">
+        <v>2.5833333340999999E-2</v>
+      </c>
+      <c r="D38">
+        <v>0.10530000000299999</v>
+      </c>
+      <c r="E38">
+        <v>0.61020000000200003</v>
+      </c>
+      <c r="F38">
+        <v>3.0051000000010002</v>
+      </c>
+      <c r="G38">
+        <v>90.015300000002995</v>
+      </c>
+    </row>
+    <row r="39" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C39">
+        <v>5.2442095458999999E-2</v>
+      </c>
+      <c r="D39">
+        <v>7.0200000001999996E-2</v>
+      </c>
+      <c r="E39">
+        <v>0.915326595774</v>
+      </c>
+      <c r="F39">
+        <v>3.0051000000010002</v>
+      </c>
+      <c r="G39">
+        <v>120.020400000004</v>
+      </c>
+    </row>
+    <row r="40" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C40">
+        <v>3.2400000004E-2</v>
+      </c>
+      <c r="D40">
+        <v>0.14145486296400001</v>
+      </c>
+      <c r="E40">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="F40">
+        <v>6.0102000000020004</v>
+      </c>
+      <c r="G40">
+        <v>60.010200000002001</v>
+      </c>
+    </row>
+    <row r="41" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C41">
+        <v>3.5800000011999997E-2</v>
+      </c>
+      <c r="D41">
+        <v>3.5100000000999998E-2</v>
+      </c>
+      <c r="E41">
+        <v>0.61020000000200003</v>
+      </c>
+      <c r="F41">
+        <v>9.0153000000030001</v>
+      </c>
+      <c r="G41">
+        <v>90.015300000002995</v>
+      </c>
+    </row>
+    <row r="42" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C42">
+        <v>3.5633333337999999E-2</v>
+      </c>
+      <c r="D42">
+        <v>0.10530000000299999</v>
+      </c>
+      <c r="E42">
+        <v>1.222507013815</v>
+      </c>
+      <c r="F42">
+        <v>9.0153000000030001</v>
+      </c>
+      <c r="G42">
+        <v>60.010200000002001</v>
+      </c>
+    </row>
+    <row r="43" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C43">
+        <v>1.7733333340000001E-2</v>
+      </c>
+      <c r="D43">
+        <v>7.0200000001999996E-2</v>
+      </c>
+      <c r="E43">
+        <v>1.2204000000040001</v>
+      </c>
+      <c r="F43">
+        <v>9.0153333333360006</v>
+      </c>
+      <c r="G43">
+        <v>120.020400000004</v>
+      </c>
+    </row>
+    <row r="44" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C44">
+        <v>2.6986828327000001E-2</v>
+      </c>
+      <c r="D44">
+        <v>0.19794260142299999</v>
+      </c>
+      <c r="E44">
+        <v>1.5255000000050001</v>
+      </c>
+      <c r="F44">
+        <v>9.0153000000030001</v>
+      </c>
+      <c r="G44">
+        <v>120.020400000004</v>
+      </c>
+    </row>
+    <row r="45" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C45">
+        <v>3.0202053311E-2</v>
+      </c>
+      <c r="D45">
+        <v>7.0200000001999996E-2</v>
+      </c>
+      <c r="E45">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="F45">
+        <v>9.0153000000030001</v>
+      </c>
+      <c r="G45">
+        <v>60.010200000002001</v>
+      </c>
+    </row>
+    <row r="46" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C46">
+        <v>3.4856977349999999E-2</v>
+      </c>
+      <c r="D46">
+        <v>3.5100000000999998E-2</v>
+      </c>
+      <c r="E46">
+        <v>1.2204000000040001</v>
+      </c>
+      <c r="F46">
+        <v>9.0153000000030001</v>
+      </c>
+      <c r="G46">
+        <v>60.010200000002001</v>
+      </c>
+    </row>
+    <row r="47" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C47">
+        <v>2.8633333338E-2</v>
+      </c>
+      <c r="D47">
+        <v>7.0200000001999996E-2</v>
+      </c>
+      <c r="E47">
+        <v>0.61020000000200003</v>
+      </c>
+      <c r="F47">
+        <v>9.0153000000030001</v>
+      </c>
+      <c r="G47">
+        <v>60.010200000002001</v>
+      </c>
+    </row>
+    <row r="48" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C48">
+        <v>2.4300000003000002E-2</v>
+      </c>
+      <c r="D48">
+        <v>7.0200000001999996E-2</v>
+      </c>
+      <c r="E48">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="F48">
+        <v>6.0102222222239998</v>
+      </c>
+      <c r="G48">
+        <v>90.015300000002995</v>
+      </c>
+    </row>
+    <row r="49" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C49">
+        <v>2.9739232094999998E-2</v>
+      </c>
+      <c r="D49">
+        <v>0.10530000000299999</v>
+      </c>
+      <c r="E49">
+        <v>0.30510000000100002</v>
+      </c>
+      <c r="F49">
+        <v>6.0102000000020004</v>
+      </c>
+      <c r="G49">
+        <v>150.025500000005</v>
+      </c>
+    </row>
+    <row r="50" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C50">
+        <v>3.0014655859000001E-2</v>
+      </c>
+      <c r="D50">
+        <v>0.106647814236</v>
+      </c>
+      <c r="E50">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="F50">
+        <v>6.0102000000020004</v>
+      </c>
+      <c r="G50">
+        <v>30.005111111112001</v>
+      </c>
+    </row>
+    <row r="51" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C51">
+        <v>1.6200000002E-2</v>
+      </c>
+      <c r="D51">
+        <v>0.105765365869</v>
+      </c>
+      <c r="E51">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="F51">
+        <v>9.0153000000030001</v>
+      </c>
+      <c r="G51">
+        <v>60.010200000002001</v>
+      </c>
+    </row>
+    <row r="52" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C52">
+        <v>3.2400000004E-2</v>
+      </c>
+      <c r="D52">
+        <v>0.10530000000299999</v>
+      </c>
+      <c r="E52">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="F52">
+        <v>9.0153000000030001</v>
+      </c>
+      <c r="G52">
+        <v>90.015300000002995</v>
+      </c>
+    </row>
+    <row r="53" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C53">
+        <v>4.0500000005000002E-2</v>
+      </c>
+      <c r="D53">
+        <v>7.0200000001999996E-2</v>
+      </c>
+      <c r="E53">
+        <v>1.2204000000040001</v>
+      </c>
+      <c r="F53">
+        <v>12.020400000004001</v>
+      </c>
+      <c r="G53">
+        <v>90.015300000002995</v>
+      </c>
+    </row>
+    <row r="54" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C54">
+        <v>4.8500000012E-2</v>
+      </c>
+      <c r="D54">
+        <v>0.105527794733</v>
+      </c>
+      <c r="E54">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="F54">
+        <v>9.0153000000030001</v>
+      </c>
+      <c r="G54">
+        <v>60.010200000002001</v>
+      </c>
+    </row>
+    <row r="55" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C55">
+        <v>2.4300000003000002E-2</v>
+      </c>
+      <c r="D55">
+        <v>0.10648743881099999</v>
+      </c>
+      <c r="E55">
+        <v>0.61020000000200003</v>
+      </c>
+      <c r="F55">
+        <v>9.0153000000030001</v>
+      </c>
+      <c r="G55">
+        <v>90.015300000002995</v>
+      </c>
+    </row>
+    <row r="56" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C56">
+        <v>3.2400000004E-2</v>
+      </c>
+      <c r="D56">
+        <v>0.10648178686</v>
+      </c>
+      <c r="E56">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="F56">
+        <v>9.0153000000030001</v>
+      </c>
+      <c r="G56">
+        <v>90.015300000002995</v>
+      </c>
+    </row>
+    <row r="57" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C57">
+        <v>1.6200000002E-2</v>
+      </c>
+      <c r="D57">
+        <v>0.10530000000299999</v>
+      </c>
+      <c r="E57">
+        <v>0.30510000000100002</v>
+      </c>
+      <c r="F57">
+        <v>9.0153000000030001</v>
+      </c>
+      <c r="G57">
+        <v>90.015300000002995</v>
+      </c>
+    </row>
+    <row r="58" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C58">
+        <v>3.4583902894999997E-2</v>
+      </c>
+      <c r="D58">
+        <v>0.14040000000399999</v>
+      </c>
+      <c r="E58">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="F58">
+        <v>9.0153000000030001</v>
+      </c>
+      <c r="G58">
+        <v>120.020400000004</v>
+      </c>
+    </row>
+    <row r="59" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C59">
+        <v>2.4300000003000002E-2</v>
+      </c>
+      <c r="D59">
+        <v>0.10530000000299999</v>
+      </c>
+      <c r="E59">
+        <v>0.61020000000200003</v>
+      </c>
+      <c r="F59">
+        <v>3.0051000000010002</v>
+      </c>
+      <c r="G59">
+        <v>90.015300000002995</v>
+      </c>
+    </row>
+    <row r="60" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C60">
+        <v>1.6200000002E-2</v>
+      </c>
+      <c r="D60">
+        <v>4.8433333335000002E-2</v>
+      </c>
+      <c r="E60">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="F60">
+        <v>12.020400000004001</v>
+      </c>
+      <c r="G60">
+        <v>60.010200000002001</v>
+      </c>
+    </row>
+    <row r="61" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C61">
+        <v>5.6833333340999999E-2</v>
+      </c>
+      <c r="D61">
+        <v>7.0200000001999996E-2</v>
+      </c>
+      <c r="E61">
+        <v>1.2204000000040001</v>
+      </c>
+      <c r="F61">
+        <v>6.0102000000020004</v>
+      </c>
+      <c r="G61">
+        <v>120.020400000004</v>
+      </c>
+    </row>
+    <row r="62" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C62">
+        <v>2.696666667E-2</v>
+      </c>
+      <c r="D62">
+        <v>0.10530000000299999</v>
+      </c>
+      <c r="E62">
+        <v>0.61020000000200003</v>
+      </c>
+      <c r="F62">
+        <v>9.0153000000030001</v>
+      </c>
+      <c r="G62">
+        <v>90.015300000002995</v>
+      </c>
+    </row>
+    <row r="63" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C63">
+        <v>2.5400000012000001E-2</v>
+      </c>
+      <c r="D63">
+        <v>0.10530000000299999</v>
+      </c>
+      <c r="E63">
+        <v>0.61020000000200003</v>
+      </c>
+      <c r="F63">
+        <v>12.020400000004001</v>
+      </c>
+      <c r="G63">
+        <v>90.015300000002995</v>
+      </c>
+    </row>
+    <row r="64" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C64">
+        <v>2.4300000003000002E-2</v>
+      </c>
+      <c r="D64">
+        <v>0.10631527459499999</v>
+      </c>
+      <c r="E64">
+        <v>1.2204000000040001</v>
+      </c>
+      <c r="F64">
+        <v>9.0153000000030001</v>
+      </c>
+      <c r="G64">
+        <v>90.015300000002995</v>
+      </c>
+    </row>
+    <row r="65" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C65">
+        <v>4.0500000005000002E-2</v>
+      </c>
+      <c r="D65">
+        <v>0.14040000000399999</v>
+      </c>
+      <c r="E65">
+        <v>0.64430279008400004</v>
+      </c>
+      <c r="F65">
+        <v>12.020400000004001</v>
+      </c>
+      <c r="G65">
+        <v>60.010200000002001</v>
+      </c>
+    </row>
+    <row r="66" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C66">
+        <v>2.6633333344000001E-2</v>
+      </c>
+      <c r="D66">
+        <v>7.6966666675999995E-2</v>
+      </c>
+      <c r="E66">
+        <v>1.2204000000040001</v>
+      </c>
+      <c r="F66">
+        <v>9.0153000000030001</v>
+      </c>
+      <c r="G66">
+        <v>90.015300000002995</v>
+      </c>
+    </row>
+    <row r="67" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C67">
+        <v>3.2400000004E-2</v>
+      </c>
+      <c r="D67">
+        <v>0.10530000000299999</v>
+      </c>
+      <c r="E67">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="F67">
+        <v>6.0102000000020004</v>
+      </c>
+      <c r="G67">
+        <v>90.015300000002995</v>
+      </c>
+    </row>
+    <row r="68" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C68">
+        <v>1.6200000002E-2</v>
+      </c>
+      <c r="D68">
+        <v>0.17550000000499999</v>
+      </c>
+      <c r="E68">
+        <v>0.93772873219300001</v>
+      </c>
+      <c r="F68">
+        <v>6.0102000000020004</v>
+      </c>
+      <c r="G68">
+        <v>90.015300000002995</v>
+      </c>
+    </row>
+    <row r="69" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C69">
+        <v>2.4300000003000002E-2</v>
+      </c>
+      <c r="D69">
+        <v>0.14040000000399999</v>
+      </c>
+      <c r="E69">
+        <v>1.2205257633519999</v>
+      </c>
+      <c r="F69">
+        <v>9.0153000000030001</v>
+      </c>
+      <c r="G69">
+        <v>90.015300000002995</v>
+      </c>
+    </row>
+    <row r="70" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C70">
+        <v>3.2300000003999997E-2</v>
+      </c>
+      <c r="D70">
+        <v>0.10530000000299999</v>
+      </c>
+      <c r="E70">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="F70">
+        <v>9.0153000000030001</v>
+      </c>
+      <c r="G70">
+        <v>120.020400000004</v>
+      </c>
+    </row>
+    <row r="71" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C71">
+        <v>0.12069403091600001</v>
+      </c>
+      <c r="D71">
+        <v>0.106848746386</v>
+      </c>
+      <c r="E71">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="F71">
+        <v>9.0153000000030001</v>
+      </c>
+      <c r="G71">
+        <v>120.020444444448</v>
+      </c>
+    </row>
+    <row r="72" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C72">
+        <v>2.5700000011E-2</v>
+      </c>
+      <c r="D72">
+        <v>7.0200000001999996E-2</v>
+      </c>
+      <c r="E72">
+        <v>0.91570407199600001</v>
+      </c>
+      <c r="F72">
+        <v>9.0153000000030001</v>
+      </c>
+      <c r="G72">
+        <v>90.015300000002995</v>
+      </c>
+    </row>
+    <row r="73" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C73">
+        <v>1.2433333335E-2</v>
+      </c>
+      <c r="D73">
+        <v>0.105600000017</v>
+      </c>
+      <c r="E73">
+        <v>0.61020000000200003</v>
+      </c>
+      <c r="F73">
+        <v>9.0153000000030001</v>
+      </c>
+      <c r="G73">
+        <v>90.015300000002995</v>
+      </c>
+    </row>
+    <row r="74" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C74">
+        <v>1.7733333342000002E-2</v>
+      </c>
+      <c r="D74">
+        <v>0.10530000000299999</v>
+      </c>
+      <c r="E74">
+        <v>0.30510000000100002</v>
+      </c>
+      <c r="F74">
+        <v>9.0153000000030001</v>
+      </c>
+      <c r="G74">
+        <v>120.020400000004</v>
+      </c>
+    </row>
+    <row r="75" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C75">
+        <v>1.6200000002E-2</v>
+      </c>
+      <c r="D75">
+        <v>7.0200000001999996E-2</v>
+      </c>
+      <c r="E75">
+        <v>1.2208513528260001</v>
+      </c>
+      <c r="F75">
+        <v>9.0153000000030001</v>
+      </c>
+      <c r="G75">
+        <v>90.015300000002995</v>
+      </c>
+    </row>
+    <row r="76" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C76">
+        <v>3.2400000004E-2</v>
+      </c>
+      <c r="D76">
+        <v>0.10530000000299999</v>
+      </c>
+      <c r="E76">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="F76">
+        <v>6.0102000000020004</v>
+      </c>
+      <c r="G76">
+        <v>60.010200000002001</v>
+      </c>
+    </row>
+    <row r="77" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C77">
+        <v>2.5833333340999999E-2</v>
+      </c>
+      <c r="D77">
+        <v>7.0200000001999996E-2</v>
+      </c>
+      <c r="E77">
+        <v>1.2204000000040001</v>
+      </c>
+      <c r="F77">
+        <v>9.0153000000030001</v>
+      </c>
+      <c r="G77">
+        <v>90.015300000002995</v>
+      </c>
+    </row>
+    <row r="78" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C78">
+        <v>2.696666667E-2</v>
+      </c>
+      <c r="D78">
+        <v>0.10530000000299999</v>
+      </c>
+      <c r="E78">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="F78">
+        <v>9.0153000000030001</v>
+      </c>
+      <c r="G78">
+        <v>90.015300000002995</v>
+      </c>
+    </row>
+    <row r="79" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C79">
+        <v>2.4300000003000002E-2</v>
+      </c>
+      <c r="D79">
+        <v>0.10530000000299999</v>
+      </c>
+      <c r="E79">
+        <v>0.30510000000100002</v>
+      </c>
+      <c r="F79">
+        <v>12.020400000004001</v>
+      </c>
+      <c r="G79">
+        <v>90.015300000002995</v>
+      </c>
+    </row>
+    <row r="80" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C80">
+        <v>3.2400000004E-2</v>
+      </c>
+      <c r="D80">
+        <v>7.0200000001999996E-2</v>
+      </c>
+      <c r="E80">
+        <v>1.2214467787800001</v>
+      </c>
+      <c r="F80">
+        <v>9.0153333333360006</v>
+      </c>
+      <c r="G80">
+        <v>90.015300000002995</v>
+      </c>
+    </row>
+    <row r="81" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C81">
+        <v>3.2300000003999997E-2</v>
+      </c>
+      <c r="D81">
+        <v>0.10557824439000001</v>
+      </c>
+      <c r="E81">
+        <v>1.2204000000040001</v>
+      </c>
+      <c r="F81">
+        <v>9.0153000000030001</v>
+      </c>
+      <c r="G81">
+        <v>60.010200000002001</v>
+      </c>
+    </row>
+    <row r="82" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C82">
+        <v>2.8633333337000001E-2</v>
+      </c>
+      <c r="D82">
+        <v>0.105720322921</v>
+      </c>
+      <c r="E82">
+        <v>0.61020000000200003</v>
+      </c>
+      <c r="F82">
+        <v>6.0102000000020004</v>
+      </c>
+      <c r="G82">
+        <v>90.015300000002995</v>
+      </c>
+    </row>
+    <row r="83" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C83">
+        <v>3.2400000004E-2</v>
+      </c>
+      <c r="D83">
+        <v>7.1639761361000004E-2</v>
+      </c>
+      <c r="E83">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="F83">
+        <v>6.0503963230490001</v>
+      </c>
+      <c r="G83">
+        <v>90.015333333336002</v>
+      </c>
+    </row>
+    <row r="84" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C84">
+        <v>2.696666667E-2</v>
+      </c>
+      <c r="D84">
+        <v>0.10530000000299999</v>
+      </c>
+      <c r="E84">
+        <v>0.61020000000200003</v>
+      </c>
+      <c r="F84">
+        <v>6.0102000000020004</v>
+      </c>
+      <c r="G84">
+        <v>60.010200000002001</v>
+      </c>
+    </row>
+    <row r="85" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C85">
+        <v>2.696666667E-2</v>
+      </c>
+      <c r="D85">
+        <v>3.5444444459000003E-2</v>
+      </c>
+      <c r="E85">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="F85">
+        <v>12.020400000004001</v>
+      </c>
+      <c r="G85">
+        <v>90.015300000002995</v>
+      </c>
+    </row>
+    <row r="86" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C86">
+        <v>3.1218777297999999E-2</v>
+      </c>
+      <c r="D86">
+        <v>7.0400000010000005E-2</v>
+      </c>
+      <c r="E86">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="F86">
+        <v>6.0102000000020004</v>
+      </c>
+      <c r="G86">
+        <v>60.010200000002001</v>
+      </c>
+    </row>
+    <row r="87" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C87">
+        <v>2.3200000003000001E-2</v>
+      </c>
+      <c r="D87">
+        <v>0.10530000000299999</v>
+      </c>
+      <c r="E87">
+        <v>1.2204000000040001</v>
+      </c>
+      <c r="F87">
+        <v>9.0153000000030001</v>
+      </c>
+      <c r="G87">
+        <v>90.015300000002995</v>
+      </c>
+    </row>
+    <row r="88" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C88">
+        <v>1.6200000002E-2</v>
+      </c>
+      <c r="D88">
+        <v>0.106335568012</v>
+      </c>
+      <c r="E88">
+        <v>0.61020000000200003</v>
+      </c>
+      <c r="F88">
+        <v>6.0102000000020004</v>
+      </c>
+      <c r="G88">
+        <v>120.020400000004</v>
+      </c>
+    </row>
+    <row r="89" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C89">
+        <v>2.1533333336E-2</v>
+      </c>
+      <c r="D89">
+        <v>0.14040000000399999</v>
+      </c>
+      <c r="E89">
+        <v>1.2204000000040001</v>
+      </c>
+      <c r="F89">
+        <v>12.028629794889</v>
+      </c>
+      <c r="G89">
+        <v>90.015300000002995</v>
+      </c>
+    </row>
+    <row r="90" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C90">
+        <v>4.2064791759999998E-2</v>
+      </c>
+      <c r="D90">
+        <v>3.8633333346999997E-2</v>
+      </c>
+      <c r="E90">
+        <v>1.221454586945</v>
+      </c>
+      <c r="F90">
+        <v>6.0102000000020004</v>
+      </c>
+      <c r="G90">
+        <v>90.015300000002995</v>
+      </c>
+    </row>
+    <row r="91" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C91">
+        <v>8.100000001E-3</v>
+      </c>
+      <c r="D91">
+        <v>0.14040000000399999</v>
+      </c>
+      <c r="E91">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="F91">
+        <v>6.0102000000020004</v>
+      </c>
+      <c r="G91">
+        <v>60.010200000002001</v>
+      </c>
+    </row>
+    <row r="92" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C92">
+        <v>2.4300000003000002E-2</v>
+      </c>
+      <c r="D92">
+        <v>0.14040000000399999</v>
+      </c>
+      <c r="E92">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="F92">
+        <v>12.020400000004001</v>
+      </c>
+      <c r="G92">
+        <v>90.015300000002995</v>
+      </c>
+    </row>
+    <row r="93" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C93">
+        <v>3.2400000004E-2</v>
+      </c>
+      <c r="D93">
+        <v>0.14040000000399999</v>
+      </c>
+      <c r="E93">
+        <v>0.61020000000200003</v>
+      </c>
+      <c r="F93">
+        <v>9.0153000000030001</v>
+      </c>
+      <c r="G93">
+        <v>120.020400000004</v>
+      </c>
+    </row>
+    <row r="94" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C94">
+        <v>3.1300000004000003E-2</v>
+      </c>
+      <c r="D94">
+        <v>0.14040000000399999</v>
+      </c>
+      <c r="E94">
+        <v>0.30510000000100002</v>
+      </c>
+      <c r="F94">
+        <v>9.0153000000030001</v>
+      </c>
+      <c r="G94">
+        <v>60.010200000002001</v>
+      </c>
+    </row>
+    <row r="95" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C95">
+        <v>2.4300000003000002E-2</v>
+      </c>
+      <c r="D95">
+        <v>0.10530000000299999</v>
+      </c>
+      <c r="E95">
+        <v>1.25854821737</v>
+      </c>
+      <c r="F95">
+        <v>12.020400000004001</v>
+      </c>
+      <c r="G95">
+        <v>90.015300000002995</v>
+      </c>
+    </row>
+    <row r="96" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C96">
+        <v>3.3951164999E-2</v>
+      </c>
+      <c r="D96">
+        <v>0.10530000000299999</v>
+      </c>
+      <c r="E96">
+        <v>1.2204000000040001</v>
+      </c>
+      <c r="F96">
+        <v>6.0102000000020004</v>
+      </c>
+      <c r="G96">
+        <v>90.015300000002995</v>
+      </c>
+    </row>
+    <row r="97" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C97">
+        <v>1.6200000002E-2</v>
+      </c>
+      <c r="D97">
+        <v>7.0200000001999996E-2</v>
+      </c>
+      <c r="E97">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="F97">
+        <v>9.0153000000030001</v>
+      </c>
+      <c r="G97">
+        <v>90.015300000002995</v>
+      </c>
+    </row>
+    <row r="98" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C98">
+        <v>4.1600000009999999E-2</v>
+      </c>
+      <c r="D98">
+        <v>7.0200000001999996E-2</v>
+      </c>
+      <c r="E98">
+        <v>0.91647944517299995</v>
+      </c>
+      <c r="F98">
+        <v>6.0102000000020004</v>
+      </c>
+      <c r="G98">
+        <v>90.015300000002995</v>
+      </c>
+    </row>
+    <row r="99" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C99">
+        <v>2.3200000003000001E-2</v>
+      </c>
+      <c r="D99">
+        <v>0.140444444448</v>
+      </c>
+      <c r="E99">
+        <v>0.61096771642100001</v>
+      </c>
+      <c r="F99">
+        <v>9.0153000000030001</v>
+      </c>
+      <c r="G99">
+        <v>90.016600273750996</v>
+      </c>
+    </row>
+    <row r="100" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C100">
+        <v>1.6200000002E-2</v>
+      </c>
+      <c r="D100">
+        <v>7.0200000001999996E-2</v>
+      </c>
+      <c r="E100">
+        <v>1.2204000000040001</v>
+      </c>
+      <c r="F100">
+        <v>9.0153000000030001</v>
+      </c>
+      <c r="G100">
+        <v>60.010200000002001</v>
+      </c>
+    </row>
+    <row r="101" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C101">
+        <v>1.7966666676000002E-2</v>
+      </c>
+      <c r="D101">
+        <v>7.0200000001999996E-2</v>
+      </c>
+      <c r="E101">
+        <v>0.91530000000300005</v>
+      </c>
+      <c r="F101">
+        <v>6.0102000000020004</v>
+      </c>
+      <c r="G101">
+        <v>90.015300000002995</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
implemented new test cases
</commit_message>
<xml_diff>
--- a/Data Collection.xlsx
+++ b/Data Collection.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yoga\Desktop\University\Thesis\TrustChain-Simulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA1DC4F0-D606-43FB-AAA0-124041F17500}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DDB4FBC-55FC-4FFF-AC8C-DE62208D0B27}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10680" yWindow="1425" windowWidth="14340" windowHeight="13950" activeTab="1" xr2:uid="{BCACAF04-D4C4-41AE-BAB0-4F6EFB70057E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="28440" xr2:uid="{BCACAF04-D4C4-41AE-BAB0-4F6EFB70057E}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Planning" sheetId="3" r:id="rId1"/>
@@ -21,12 +21,13 @@
     <sheet name="Set6" sheetId="8" r:id="rId6"/>
     <sheet name="Set7" sheetId="9" r:id="rId7"/>
     <sheet name="Set8" sheetId="10" r:id="rId8"/>
+    <sheet name="Set9" sheetId="11" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'Set4'!$E$4</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'Set4'!$E$5:$E$54</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'Set4'!$E$61</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'Set4'!$E$62:$E$161</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">'Set4'!$E$61</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'Set4'!$E$62:$E$161</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'Set4'!$E$4</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'Set4'!$E$5:$E$54</definedName>
     <definedName name="solver_eng" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_num" localSheetId="3" hidden="1">0</definedName>
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="115">
   <si>
     <t>Evil Node Sleeping Transactions</t>
   </si>
@@ -385,6 +386,18 @@
   <si>
     <t>Nodes</t>
   </si>
+  <si>
+    <t>9 - Average Path Length</t>
+  </si>
+  <si>
+    <t>Path Length</t>
+  </si>
+  <si>
+    <t>8 -  Average Path Length</t>
+  </si>
+  <si>
+    <t>dissemination + direct connection after the first message</t>
+  </si>
 </sst>
 </file>
 
@@ -503,7 +516,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -555,6 +568,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
@@ -650,7 +669,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="12">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -663,8 +682,9 @@
     <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -697,10 +717,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="7" xfId="10"/>
     <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="11"/>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="11" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -716,8 +739,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="12" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="12">
+  <cellStyles count="13">
+    <cellStyle name="60% - Accent1" xfId="12" builtinId="32"/>
     <cellStyle name="60% - Accent4" xfId="9" builtinId="44"/>
     <cellStyle name="60% - Accent6" xfId="8" builtinId="52"/>
     <cellStyle name="Accent1" xfId="7" builtinId="29"/>
@@ -6435,7 +6460,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.1</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -6473,7 +6498,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{00000000-BA23-47F0-8325-162A3EB2469F}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.0</cx:f>
+              <cx:f>_xlchart.v1.2</cx:f>
               <cx:v>Standardized </cx:v>
             </cx:txData>
           </cx:tx>
@@ -6501,7 +6526,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -6539,7 +6564,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{00000000-92AE-4E86-80B1-3A198ACB5431}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.2</cx:f>
+              <cx:f>_xlchart.v1.0</cx:f>
               <cx:v>Standardized </cx:v>
             </cx:txData>
           </cx:tx>
@@ -15788,33 +15813,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4891D42F-3971-43B5-986A-C0853C8465A0}">
-  <dimension ref="A1:S49"/>
+  <dimension ref="A1:T49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.5703125" style="13" customWidth="1"/>
     <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="15.28515625" customWidth="1"/>
     <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="38" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.28515625" customWidth="1"/>
-    <col min="14" max="14" width="28" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.140625" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="38" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.28515625" customWidth="1"/>
+    <col min="15" max="15" width="28" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>23</v>
       </c>
@@ -15834,35 +15860,38 @@
         <v>13</v>
       </c>
       <c r="G1" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="26" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="4">
@@ -15882,30 +15911,31 @@
       <c r="F2" s="1">
         <v>0.23</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="24"/>
+      <c r="H2" s="1">
         <v>10</v>
       </c>
-      <c r="H2" s="1">
+      <c r="I2" s="1">
         <v>100</v>
       </c>
-      <c r="I2" s="1">
+      <c r="J2" s="1">
         <v>1</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="1">
+      <c r="N2" s="1">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="24"/>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="25"/>
       <c r="B3" s="4">
         <v>2</v>
       </c>
@@ -15917,36 +15947,37 @@
         <v>0.13695052585936646</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" ref="E3:E35" si="0">LN(C3)/(C3)</f>
+        <f t="shared" ref="E3:E39" si="0">LN(C3)/(C3)</f>
         <v>0.14978661367769955</v>
       </c>
       <c r="F3" s="1">
         <v>0.15</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="24"/>
+      <c r="H3" s="1">
         <v>10</v>
       </c>
-      <c r="H3" s="1">
+      <c r="I3" s="1">
         <v>100</v>
       </c>
-      <c r="I3" s="1">
+      <c r="J3" s="1">
         <v>1</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="1">
+      <c r="N3" s="1">
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="24"/>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" s="25"/>
       <c r="B4" s="4">
         <v>3</v>
       </c>
@@ -15964,34 +15995,35 @@
       <c r="F4" s="1">
         <v>7.9000000000000001E-2</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="24"/>
+      <c r="H4" s="1">
         <v>10</v>
       </c>
-      <c r="H4" s="1">
+      <c r="I4" s="1">
         <v>100</v>
       </c>
-      <c r="I4" s="1">
+      <c r="J4" s="1">
         <v>1</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M4" s="1">
+      <c r="N4" s="1">
         <v>50</v>
       </c>
-      <c r="P4" s="1"/>
-      <c r="S4" s="1" t="s">
+      <c r="Q4" s="1"/>
+      <c r="T4" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" s="25"/>
       <c r="B5" s="4">
         <v>4</v>
       </c>
@@ -16009,31 +16041,32 @@
       <c r="F5" s="1">
         <v>4.7E-2</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="24"/>
+      <c r="H5" s="1">
         <v>10</v>
       </c>
-      <c r="H5" s="1">
+      <c r="I5" s="1">
         <v>100</v>
       </c>
-      <c r="I5" s="1">
+      <c r="J5" s="1">
         <v>1</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="M5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M5" s="1">
+      <c r="N5" s="1">
         <v>50</v>
       </c>
-      <c r="S5" s="1"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="24"/>
+      <c r="T5" s="1"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" s="25"/>
       <c r="B6" s="4">
         <v>5</v>
       </c>
@@ -16052,33 +16085,34 @@
         <f>E6</f>
         <v>6.9077552789821367E-3</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="24"/>
+      <c r="H6" s="1">
         <v>10</v>
       </c>
-      <c r="H6" s="1">
+      <c r="I6" s="1">
         <v>100</v>
       </c>
-      <c r="I6" s="1">
+      <c r="J6" s="1">
         <v>1</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="M6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M6" s="1">
+      <c r="N6" s="1">
         <v>50</v>
       </c>
-      <c r="S6" s="1" t="s">
+      <c r="T6" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="24"/>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" s="25"/>
       <c r="B7" s="4">
         <v>6</v>
       </c>
@@ -16094,33 +16128,34 @@
         <v>9.210340371976184E-4</v>
       </c>
       <c r="F7" s="1"/>
-      <c r="G7" s="1">
+      <c r="G7" s="24"/>
+      <c r="H7" s="1">
         <v>10</v>
       </c>
-      <c r="H7" s="1">
+      <c r="I7" s="1">
         <v>100</v>
       </c>
-      <c r="I7" s="1">
+      <c r="J7" s="1">
         <v>1</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="M7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M7" s="1">
+      <c r="N7" s="1">
         <v>50</v>
       </c>
-      <c r="S7" s="1" t="s">
+      <c r="T7" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" s="27" t="s">
         <v>25</v>
       </c>
       <c r="B8" s="5">
@@ -16140,33 +16175,34 @@
       <c r="F8" s="1">
         <v>4.7E-2</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="24"/>
+      <c r="H8" s="1">
         <v>10</v>
       </c>
-      <c r="H8" s="1">
+      <c r="I8" s="1">
         <v>100</v>
       </c>
-      <c r="I8" s="1">
+      <c r="J8" s="1">
         <v>1</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="K8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="L8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="M8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M8" s="1">
+      <c r="N8" s="1">
         <v>50</v>
       </c>
-      <c r="S8" s="1" t="s">
+      <c r="T8" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="26"/>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" s="27"/>
       <c r="B9" s="5">
         <v>2</v>
       </c>
@@ -16184,33 +16220,34 @@
       <c r="F9" s="1">
         <v>4.7E-2</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="24"/>
+      <c r="H9" s="1">
         <v>10</v>
       </c>
-      <c r="H9" s="1">
+      <c r="I9" s="1">
         <v>100</v>
       </c>
-      <c r="I9" s="1">
+      <c r="J9" s="1">
         <v>2</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="K9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="L9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="M9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M9" s="1">
+      <c r="N9" s="1">
         <v>50</v>
       </c>
-      <c r="S9" s="1" t="s">
+      <c r="T9" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="26"/>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" s="27"/>
       <c r="B10" s="5">
         <v>3</v>
       </c>
@@ -16228,33 +16265,34 @@
       <c r="F10" s="1">
         <v>4.7E-2</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="24"/>
+      <c r="H10" s="1">
         <v>10</v>
       </c>
-      <c r="H10" s="1">
+      <c r="I10" s="1">
         <v>100</v>
       </c>
-      <c r="I10" s="1">
+      <c r="J10" s="1">
         <v>10</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="K10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="L10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="M10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M10" s="1">
+      <c r="N10" s="1">
         <v>50</v>
       </c>
-      <c r="S10" s="1" t="s">
+      <c r="T10" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="26" t="s">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" s="27" t="s">
         <v>26</v>
       </c>
       <c r="B11" s="6">
@@ -16274,30 +16312,31 @@
       <c r="F11" s="1">
         <v>4.7E-2</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11" s="24"/>
+      <c r="H11" s="1">
         <v>10</v>
       </c>
-      <c r="H11" s="1">
+      <c r="I11" s="1">
         <v>100</v>
       </c>
-      <c r="I11" s="1">
+      <c r="J11" s="1">
         <v>1</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="K11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="L11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L11" s="1" t="s">
+      <c r="M11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M11" s="1">
+      <c r="N11" s="1">
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="26"/>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" s="27"/>
       <c r="B12" s="6">
         <v>2</v>
       </c>
@@ -16315,30 +16354,31 @@
       <c r="F12" s="1">
         <v>4.7E-2</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12" s="24"/>
+      <c r="H12" s="1">
         <v>10</v>
       </c>
-      <c r="H12" s="1">
+      <c r="I12" s="1">
         <v>100</v>
       </c>
-      <c r="I12" s="1">
+      <c r="J12" s="1">
         <v>1</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="K12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="L12" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="L12" s="1" t="s">
+      <c r="M12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M12" s="1">
+      <c r="N12" s="1">
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="26"/>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" s="27"/>
       <c r="B13" s="6">
         <v>3</v>
       </c>
@@ -16356,30 +16396,31 @@
       <c r="F13" s="1">
         <v>4.7E-2</v>
       </c>
-      <c r="G13" s="1">
+      <c r="G13" s="24"/>
+      <c r="H13" s="1">
         <v>10</v>
       </c>
-      <c r="H13" s="1">
+      <c r="I13" s="1">
         <v>100</v>
       </c>
-      <c r="I13" s="1">
+      <c r="J13" s="1">
         <v>1</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="K13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K13" s="1" t="s">
+      <c r="L13" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="L13" s="1" t="s">
+      <c r="M13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M13" s="1">
+      <c r="N13" s="1">
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="26"/>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" s="27"/>
       <c r="B14" s="6">
         <v>4</v>
       </c>
@@ -16397,30 +16438,31 @@
       <c r="F14" s="1">
         <v>4.7E-2</v>
       </c>
-      <c r="G14" s="1">
+      <c r="G14" s="24"/>
+      <c r="H14" s="1">
         <v>10</v>
       </c>
-      <c r="H14" s="1">
+      <c r="I14" s="1">
         <v>100</v>
       </c>
-      <c r="I14" s="1">
+      <c r="J14" s="1">
         <v>1</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="K14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K14" s="1" t="s">
+      <c r="L14" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="L14" s="1" t="s">
+      <c r="M14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M14" s="1">
+      <c r="N14" s="1">
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="26"/>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" s="27"/>
       <c r="B15" s="6">
         <v>5</v>
       </c>
@@ -16438,30 +16480,31 @@
       <c r="F15" s="1">
         <v>4.7E-2</v>
       </c>
-      <c r="G15" s="1">
+      <c r="G15" s="24"/>
+      <c r="H15" s="1">
         <v>10</v>
       </c>
-      <c r="H15" s="1">
+      <c r="I15" s="1">
         <v>100</v>
       </c>
-      <c r="I15" s="1">
+      <c r="J15" s="1">
         <v>1</v>
       </c>
-      <c r="J15" s="1" t="s">
+      <c r="K15" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K15" s="1" t="s">
+      <c r="L15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L15" s="1" t="s">
+      <c r="M15" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M15" s="1">
+      <c r="N15" s="1">
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="26"/>
+    <row r="16" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="27"/>
       <c r="B16" s="6">
         <v>6</v>
       </c>
@@ -16479,29 +16522,30 @@
       <c r="F16" s="1">
         <v>4.7E-2</v>
       </c>
-      <c r="G16" s="1">
+      <c r="G16" s="24"/>
+      <c r="H16" s="1">
         <v>10</v>
       </c>
-      <c r="H16" s="1">
+      <c r="I16" s="1">
         <v>100</v>
       </c>
-      <c r="I16" s="1">
+      <c r="J16" s="1">
         <v>1</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="K16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K16" s="1" t="s">
+      <c r="L16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="L16" s="1" t="s">
+      <c r="M16" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M16" s="1">
+      <c r="N16" s="1">
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
         <v>28</v>
       </c>
@@ -16523,29 +16567,30 @@
         <f>E17</f>
         <v>4.6051701859880917E-2</v>
       </c>
-      <c r="G17" s="1">
+      <c r="G17" s="24"/>
+      <c r="H17" s="1">
         <v>10</v>
       </c>
-      <c r="H17" s="1">
+      <c r="I17" s="1">
         <v>100</v>
       </c>
-      <c r="I17" s="1">
+      <c r="J17" s="1">
         <v>1</v>
       </c>
-      <c r="J17" s="1" t="s">
+      <c r="K17" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="L17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L17" s="1" t="s">
+      <c r="M17" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M17" s="1">
+      <c r="N17" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>46</v>
       </c>
@@ -16566,32 +16611,33 @@
       <c r="F18" s="1">
         <v>1.243E-2</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G18" s="24"/>
+      <c r="H18" s="1">
         <v>10</v>
       </c>
-      <c r="H18" s="1">
+      <c r="I18" s="1">
         <v>100</v>
       </c>
-      <c r="I18" s="1">
+      <c r="J18" s="1">
         <v>1</v>
       </c>
-      <c r="J18" s="1" t="s">
+      <c r="K18" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K18" s="1" t="s">
+      <c r="L18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L18" s="1" t="s">
+      <c r="M18" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M18" s="1">
+      <c r="N18" s="1">
         <v>1</v>
       </c>
-      <c r="O18" s="1" t="s">
+      <c r="P18" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B19" s="20">
         <v>2</v>
       </c>
@@ -16609,33 +16655,34 @@
       <c r="F19" s="1">
         <v>1.243E-2</v>
       </c>
-      <c r="G19" s="1">
+      <c r="G19" s="24"/>
+      <c r="H19" s="1">
         <v>2</v>
       </c>
-      <c r="H19" s="1">
+      <c r="I19" s="1">
         <v>100</v>
       </c>
-      <c r="I19" s="1">
+      <c r="J19" s="1">
         <v>1</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="K19" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K19" s="1" t="s">
+      <c r="L19" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L19" s="1" t="s">
+      <c r="M19" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M19" s="1">
+      <c r="N19" s="1">
         <v>1</v>
       </c>
-      <c r="O19" s="1" t="s">
+      <c r="P19" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="24" t="s">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20" s="25" t="s">
         <v>47</v>
       </c>
       <c r="B20" s="10">
@@ -16655,30 +16702,31 @@
       <c r="F20" s="1">
         <v>4.7E-2</v>
       </c>
-      <c r="G20" s="1">
+      <c r="G20" s="24"/>
+      <c r="H20" s="1">
         <v>10</v>
       </c>
-      <c r="H20" s="1">
+      <c r="I20" s="1">
         <v>100</v>
       </c>
-      <c r="I20" s="1">
+      <c r="J20" s="1">
         <v>1</v>
       </c>
-      <c r="J20" s="1" t="s">
+      <c r="K20" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="K20" s="1" t="s">
+      <c r="L20" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L20" s="1" t="s">
+      <c r="M20" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M20" s="1">
+      <c r="N20" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="24"/>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" s="25"/>
       <c r="B21" s="11">
         <v>2</v>
       </c>
@@ -16696,30 +16744,31 @@
       <c r="F21" s="1">
         <v>4.7E-2</v>
       </c>
-      <c r="G21" s="1">
+      <c r="G21" s="24"/>
+      <c r="H21" s="1">
         <v>10</v>
       </c>
-      <c r="H21" s="1">
+      <c r="I21" s="1">
         <v>100</v>
       </c>
-      <c r="I21" s="1">
+      <c r="J21" s="1">
         <v>1</v>
       </c>
-      <c r="J21" s="1" t="s">
+      <c r="K21" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="K21" s="1" t="s">
+      <c r="L21" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L21" s="1" t="s">
+      <c r="M21" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M21" s="1">
+      <c r="N21" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="24"/>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A22" s="25"/>
       <c r="B22" s="10">
         <v>3</v>
       </c>
@@ -16737,30 +16786,31 @@
       <c r="F22" s="1">
         <v>4.7E-2</v>
       </c>
-      <c r="G22" s="1">
+      <c r="G22" s="24"/>
+      <c r="H22" s="1">
         <v>10</v>
       </c>
-      <c r="H22" s="1">
+      <c r="I22" s="1">
         <v>100</v>
       </c>
-      <c r="I22" s="1">
+      <c r="J22" s="1">
         <v>1</v>
       </c>
-      <c r="J22" s="1" t="s">
+      <c r="K22" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K22" s="1" t="s">
+      <c r="L22" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L22" s="1" t="s">
+      <c r="M22" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M22" s="1">
+      <c r="N22" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="24"/>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A23" s="25"/>
       <c r="B23" s="11">
         <v>4</v>
       </c>
@@ -16778,30 +16828,31 @@
       <c r="F23" s="1">
         <v>4.7E-2</v>
       </c>
-      <c r="G23" s="1">
+      <c r="G23" s="24"/>
+      <c r="H23" s="1">
         <v>10</v>
       </c>
-      <c r="H23" s="1">
+      <c r="I23" s="1">
         <v>100</v>
       </c>
-      <c r="I23" s="1">
+      <c r="J23" s="1">
         <v>1</v>
       </c>
-      <c r="J23" s="1" t="s">
+      <c r="K23" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="K23" s="1" t="s">
+      <c r="L23" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L23" s="1" t="s">
+      <c r="M23" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M23" s="1">
+      <c r="N23" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="24"/>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24" s="25"/>
       <c r="B24" s="10">
         <v>5</v>
       </c>
@@ -16819,30 +16870,31 @@
       <c r="F24" s="1">
         <v>4.7E-2</v>
       </c>
-      <c r="G24" s="1">
+      <c r="G24" s="24"/>
+      <c r="H24" s="1">
         <v>10</v>
       </c>
-      <c r="H24" s="1">
+      <c r="I24" s="1">
         <v>100</v>
       </c>
-      <c r="I24" s="1">
+      <c r="J24" s="1">
         <v>1</v>
       </c>
-      <c r="J24" s="1" t="s">
+      <c r="K24" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="K24" s="1" t="s">
+      <c r="L24" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L24" s="1" t="s">
+      <c r="M24" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M24" s="1">
+      <c r="N24" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="27" t="s">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A25" s="28" t="s">
         <v>57</v>
       </c>
       <c r="B25" s="12">
@@ -16862,33 +16914,34 @@
       <c r="F25" s="1">
         <v>4.7E-2</v>
       </c>
-      <c r="G25" s="1">
+      <c r="G25" s="24"/>
+      <c r="H25" s="1">
         <v>1</v>
       </c>
-      <c r="H25" s="1">
+      <c r="I25" s="1">
         <v>100</v>
       </c>
-      <c r="I25" s="1">
+      <c r="J25" s="1">
         <v>1</v>
       </c>
-      <c r="J25" s="1" t="s">
+      <c r="K25" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K25" s="1" t="s">
+      <c r="L25" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L25" s="1" t="s">
+      <c r="M25" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M25" s="1">
+      <c r="N25" s="1">
         <v>100</v>
       </c>
-      <c r="O25" s="1" t="s">
+      <c r="P25" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="27"/>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A26" s="28"/>
       <c r="B26" s="12">
         <v>2</v>
       </c>
@@ -16906,30 +16959,31 @@
       <c r="F26" s="1">
         <v>4.7E-2</v>
       </c>
-      <c r="G26" s="1">
+      <c r="G26" s="24"/>
+      <c r="H26" s="1">
         <v>2</v>
       </c>
-      <c r="H26" s="1">
+      <c r="I26" s="1">
         <v>100</v>
       </c>
-      <c r="I26" s="1">
+      <c r="J26" s="1">
         <v>1</v>
       </c>
-      <c r="J26" s="1" t="s">
+      <c r="K26" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K26" s="1" t="s">
+      <c r="L26" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L26" s="1" t="s">
+      <c r="M26" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M26" s="1">
+      <c r="N26" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="27"/>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A27" s="28"/>
       <c r="B27" s="12">
         <v>3</v>
       </c>
@@ -16947,30 +17001,31 @@
       <c r="F27" s="1">
         <v>4.7E-2</v>
       </c>
-      <c r="G27" s="1">
+      <c r="G27" s="24"/>
+      <c r="H27" s="1">
         <v>4</v>
       </c>
-      <c r="H27" s="1">
+      <c r="I27" s="1">
         <v>100</v>
       </c>
-      <c r="I27" s="1">
+      <c r="J27" s="1">
         <v>1</v>
       </c>
-      <c r="J27" s="1" t="s">
+      <c r="K27" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K27" s="1" t="s">
+      <c r="L27" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L27" s="1" t="s">
+      <c r="M27" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M27" s="1">
+      <c r="N27" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="27"/>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" s="28"/>
       <c r="B28" s="12">
         <v>4</v>
       </c>
@@ -16988,30 +17043,31 @@
       <c r="F28" s="1">
         <v>4.7E-2</v>
       </c>
-      <c r="G28" s="1">
+      <c r="G28" s="24"/>
+      <c r="H28" s="1">
         <v>8</v>
       </c>
-      <c r="H28" s="1">
+      <c r="I28" s="1">
         <v>100</v>
       </c>
-      <c r="I28" s="1">
+      <c r="J28" s="1">
         <v>1</v>
       </c>
-      <c r="J28" s="1" t="s">
+      <c r="K28" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K28" s="1" t="s">
+      <c r="L28" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L28" s="1" t="s">
+      <c r="M28" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M28" s="1">
+      <c r="N28" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="27"/>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" s="28"/>
       <c r="B29" s="12">
         <v>5</v>
       </c>
@@ -17029,30 +17085,31 @@
       <c r="F29" s="1">
         <v>4.7E-2</v>
       </c>
-      <c r="G29" s="1">
+      <c r="G29" s="24"/>
+      <c r="H29" s="1">
         <v>16</v>
       </c>
-      <c r="H29" s="1">
+      <c r="I29" s="1">
         <v>100</v>
       </c>
-      <c r="I29" s="1">
+      <c r="J29" s="1">
         <v>1</v>
       </c>
-      <c r="J29" s="1" t="s">
+      <c r="K29" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K29" s="1" t="s">
+      <c r="L29" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L29" s="1" t="s">
+      <c r="M29" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M29" s="1">
+      <c r="N29" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="27"/>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30" s="28"/>
       <c r="B30" s="12">
         <v>6</v>
       </c>
@@ -17070,30 +17127,31 @@
       <c r="F30" s="1">
         <v>4.7E-2</v>
       </c>
-      <c r="G30" s="1">
+      <c r="G30" s="24"/>
+      <c r="H30" s="1">
         <v>32</v>
       </c>
-      <c r="H30" s="1">
+      <c r="I30" s="1">
         <v>100</v>
       </c>
-      <c r="I30" s="1">
+      <c r="J30" s="1">
         <v>1</v>
       </c>
-      <c r="J30" s="1" t="s">
+      <c r="K30" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K30" s="1" t="s">
+      <c r="L30" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L30" s="1" t="s">
+      <c r="M30" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M30" s="1">
+      <c r="N30" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="24" t="s">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A31" s="25" t="s">
         <v>58</v>
       </c>
       <c r="B31" s="14">
@@ -17113,30 +17171,31 @@
       <c r="F31" s="1">
         <v>4.7E-2</v>
       </c>
-      <c r="G31" s="1">
+      <c r="G31" s="24"/>
+      <c r="H31" s="1">
         <v>2</v>
       </c>
-      <c r="H31" s="1">
+      <c r="I31" s="1">
         <v>100</v>
       </c>
-      <c r="I31" s="1">
+      <c r="J31" s="1">
         <v>1</v>
       </c>
-      <c r="J31" s="1" t="s">
+      <c r="K31" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K31" s="1" t="s">
+      <c r="L31" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L31" s="1" t="s">
+      <c r="M31" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="M31" s="1">
+      <c r="N31" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="24"/>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32" s="25"/>
       <c r="B32" s="14">
         <v>2</v>
       </c>
@@ -17154,30 +17213,31 @@
       <c r="F32" s="1">
         <v>4.7E-2</v>
       </c>
-      <c r="G32" s="1">
+      <c r="G32" s="24"/>
+      <c r="H32" s="1">
         <v>2</v>
       </c>
-      <c r="H32" s="1">
+      <c r="I32" s="1">
         <v>100</v>
       </c>
-      <c r="I32" s="1">
+      <c r="J32" s="1">
         <v>1</v>
       </c>
-      <c r="J32" s="1" t="s">
+      <c r="K32" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K32" s="1" t="s">
+      <c r="L32" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L32" s="1" t="s">
+      <c r="M32" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="M32" s="1">
+      <c r="N32" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" s="24"/>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33" s="25"/>
       <c r="B33" s="14">
         <v>3</v>
       </c>
@@ -17195,30 +17255,31 @@
       <c r="F33" s="1">
         <v>4.7E-2</v>
       </c>
-      <c r="G33" s="1">
+      <c r="G33" s="24"/>
+      <c r="H33" s="1">
         <v>2</v>
       </c>
-      <c r="H33" s="1">
+      <c r="I33" s="1">
         <v>100</v>
       </c>
-      <c r="I33" s="1">
+      <c r="J33" s="1">
         <v>1</v>
       </c>
-      <c r="J33" s="1" t="s">
+      <c r="K33" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K33" s="1" t="s">
+      <c r="L33" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L33" s="1" t="s">
+      <c r="M33" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="M33" s="1">
+      <c r="N33" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="24"/>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34" s="25"/>
       <c r="B34" s="14">
         <v>4</v>
       </c>
@@ -17236,30 +17297,31 @@
       <c r="F34" s="1">
         <v>4.7E-2</v>
       </c>
-      <c r="G34" s="1">
+      <c r="G34" s="24"/>
+      <c r="H34" s="1">
         <v>2</v>
       </c>
-      <c r="H34" s="1">
+      <c r="I34" s="1">
         <v>100</v>
       </c>
-      <c r="I34" s="1">
+      <c r="J34" s="1">
         <v>1</v>
       </c>
-      <c r="J34" s="1" t="s">
+      <c r="K34" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K34" s="1" t="s">
+      <c r="L34" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L34" s="1" t="s">
+      <c r="M34" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="M34" s="1">
+      <c r="N34" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" s="24"/>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A35" s="25"/>
       <c r="B35" s="14">
         <v>5</v>
       </c>
@@ -17277,125 +17339,273 @@
       <c r="F35" s="1">
         <v>4.7E-2</v>
       </c>
-      <c r="G35" s="1">
+      <c r="G35" s="24"/>
+      <c r="H35" s="1">
         <v>2</v>
       </c>
-      <c r="H35" s="1">
+      <c r="I35" s="1">
         <v>100</v>
       </c>
-      <c r="I35" s="1">
+      <c r="J35" s="1">
         <v>1</v>
       </c>
-      <c r="J35" s="1" t="s">
+      <c r="K35" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K35" s="1" t="s">
+      <c r="L35" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L35" s="1" t="s">
+      <c r="M35" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="M35" s="1">
+      <c r="N35" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="22" t="s">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="B36" s="30">
+        <v>1</v>
+      </c>
+      <c r="C36" s="1">
+        <v>500</v>
+      </c>
+      <c r="D36" s="1"/>
+      <c r="E36" s="24">
+        <f t="shared" si="0"/>
+        <v>1.2429216196844383E-2</v>
+      </c>
+      <c r="F36" s="1"/>
+      <c r="G36" s="24">
+        <v>1</v>
+      </c>
+      <c r="H36" s="1">
+        <v>2</v>
+      </c>
+      <c r="I36" s="24">
+        <v>100</v>
+      </c>
+      <c r="J36" s="24">
+        <v>1</v>
+      </c>
+      <c r="K36" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="L36" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="M36" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="N36" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B37" s="30">
+        <v>2</v>
+      </c>
+      <c r="C37" s="24">
+        <v>500</v>
+      </c>
+      <c r="D37" s="1"/>
+      <c r="E37" s="24">
+        <f t="shared" si="0"/>
+        <v>1.2429216196844383E-2</v>
+      </c>
+      <c r="F37" s="1"/>
+      <c r="G37" s="24">
+        <v>2</v>
+      </c>
+      <c r="H37" s="24">
+        <v>2</v>
+      </c>
+      <c r="I37" s="24">
+        <v>100</v>
+      </c>
+      <c r="J37" s="24">
+        <v>1</v>
+      </c>
+      <c r="K37" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="L37" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="M37" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="N37" s="24">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B38" s="30">
+        <v>3</v>
+      </c>
+      <c r="C38" s="24">
+        <v>500</v>
+      </c>
+      <c r="D38" s="1"/>
+      <c r="E38" s="24">
+        <f t="shared" si="0"/>
+        <v>1.2429216196844383E-2</v>
+      </c>
+      <c r="F38" s="1"/>
+      <c r="G38" s="24">
+        <v>5</v>
+      </c>
+      <c r="H38" s="24">
+        <v>2</v>
+      </c>
+      <c r="I38" s="24">
+        <v>100</v>
+      </c>
+      <c r="J38" s="24">
+        <v>1</v>
+      </c>
+      <c r="K38" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="L38" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="M38" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="N38" s="24">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B39" s="30">
+        <v>4</v>
+      </c>
+      <c r="C39" s="24">
+        <v>500</v>
+      </c>
+      <c r="D39" s="1"/>
+      <c r="E39" s="24">
+        <f t="shared" si="0"/>
+        <v>1.2429216196844383E-2</v>
+      </c>
+      <c r="F39" s="1"/>
+      <c r="G39" s="24">
+        <v>10</v>
+      </c>
+      <c r="H39" s="24">
+        <v>2</v>
+      </c>
+      <c r="I39" s="24">
+        <v>100</v>
+      </c>
+      <c r="J39" s="24">
+        <v>1</v>
+      </c>
+      <c r="K39" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="L39" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="M39" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="N39" s="24">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A40" s="23"/>
+      <c r="B40" s="30">
+        <v>5</v>
+      </c>
+      <c r="C40" s="24">
+        <v>500</v>
+      </c>
+      <c r="D40" s="24"/>
+      <c r="E40" s="24">
+        <f t="shared" ref="E40" si="2">LN(C40)/(C40)</f>
+        <v>1.2429216196844383E-2</v>
+      </c>
+      <c r="F40" s="24"/>
+      <c r="G40" s="24">
+        <v>100</v>
+      </c>
+      <c r="H40" s="24">
+        <v>2</v>
+      </c>
+      <c r="I40" s="24">
+        <v>100</v>
+      </c>
+      <c r="J40" s="24">
+        <v>1</v>
+      </c>
+      <c r="K40" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="L40" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="M40" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="N40" s="24">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A41" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
-      <c r="K36" s="1"/>
-      <c r="L36" s="1"/>
-      <c r="M36" s="1"/>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-      <c r="K37" s="1"/>
-      <c r="L37" s="1"/>
-      <c r="M37" s="1"/>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
-      <c r="K38" s="1"/>
-      <c r="L38" s="1"/>
-      <c r="M38" s="1"/>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
-      <c r="K39" s="1"/>
-      <c r="L39" s="1"/>
-      <c r="M39" s="1"/>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-      <c r="J40" s="1"/>
-      <c r="K40" s="1"/>
-      <c r="L40" s="1"/>
-      <c r="M40" s="1"/>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
+      <c r="G41" s="24"/>
       <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
-      <c r="K41" s="1"/>
-      <c r="L41" s="1"/>
-      <c r="M41" s="1"/>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I41" s="24"/>
+      <c r="J41" s="24">
+        <v>1</v>
+      </c>
+      <c r="K41" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="L41" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="M41" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="N41" s="24">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
+      <c r="G42" s="24"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
-    </row>
-    <row r="49" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="N42" s="1"/>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A43" s="13" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="49" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C49" s="7"/>
       <c r="F49" s="7"/>
+      <c r="G49" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -17415,7 +17625,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF874DAA-691A-4835-ACA3-DB30922CFD6B}">
   <dimension ref="A1:W52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
@@ -18513,15 +18723,15 @@
       <c r="E40">
         <v>0.91530000000300005</v>
       </c>
-      <c r="I40" s="27" t="s">
+      <c r="I40" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="J40" s="27"/>
-      <c r="K40" s="27"/>
-      <c r="L40" s="27"/>
-      <c r="M40" s="27"/>
-      <c r="N40" s="27"/>
-      <c r="O40" s="27"/>
+      <c r="J40" s="28"/>
+      <c r="K40" s="28"/>
+      <c r="L40" s="28"/>
+      <c r="M40" s="28"/>
+      <c r="N40" s="28"/>
+      <c r="O40" s="28"/>
     </row>
     <row r="41" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B41">
@@ -18539,18 +18749,18 @@
       <c r="I41" t="s">
         <v>110</v>
       </c>
-      <c r="J41" s="28" t="s">
+      <c r="J41" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="K41" s="28"/>
-      <c r="L41" s="28" t="s">
+      <c r="K41" s="29"/>
+      <c r="L41" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="M41" s="28"/>
-      <c r="N41" s="28" t="s">
+      <c r="M41" s="29"/>
+      <c r="N41" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="O41" s="28"/>
+      <c r="O41" s="29"/>
     </row>
     <row r="42" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B42">
@@ -18571,18 +18781,18 @@
       <c r="I42">
         <v>10</v>
       </c>
-      <c r="J42" s="28">
+      <c r="J42" s="29">
         <v>1.2</v>
       </c>
-      <c r="K42" s="28"/>
-      <c r="L42" s="28">
+      <c r="K42" s="29"/>
+      <c r="L42" s="29">
         <v>3</v>
       </c>
-      <c r="M42" s="28"/>
-      <c r="N42" s="28">
+      <c r="M42" s="29"/>
+      <c r="N42" s="29">
         <v>1.7929999999999999</v>
       </c>
-      <c r="O42" s="28"/>
+      <c r="O42" s="29"/>
     </row>
     <row r="43" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B43">
@@ -18603,18 +18813,18 @@
       <c r="I43">
         <v>20</v>
       </c>
-      <c r="J43" s="28">
+      <c r="J43" s="29">
         <v>1.3</v>
       </c>
-      <c r="K43" s="28"/>
-      <c r="L43" s="28">
+      <c r="K43" s="29"/>
+      <c r="L43" s="29">
         <v>4</v>
       </c>
-      <c r="M43" s="28"/>
-      <c r="N43" s="28">
+      <c r="M43" s="29"/>
+      <c r="N43" s="29">
         <v>1.8839999999999999</v>
       </c>
-      <c r="O43" s="28"/>
+      <c r="O43" s="29"/>
     </row>
     <row r="44" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B44">
@@ -18635,18 +18845,18 @@
       <c r="I44">
         <v>50</v>
       </c>
-      <c r="J44" s="28">
+      <c r="J44" s="29">
         <v>2.36</v>
       </c>
-      <c r="K44" s="28"/>
-      <c r="L44" s="28">
+      <c r="K44" s="29"/>
+      <c r="L44" s="29">
         <v>6</v>
       </c>
-      <c r="M44" s="28"/>
-      <c r="N44" s="28">
+      <c r="M44" s="29"/>
+      <c r="N44" s="29">
         <v>2.2669999999999999</v>
       </c>
-      <c r="O44" s="28"/>
+      <c r="O44" s="29"/>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45">
@@ -18667,18 +18877,18 @@
       <c r="I45">
         <v>100</v>
       </c>
-      <c r="J45" s="28">
+      <c r="J45" s="29">
         <v>2.5499999999999998</v>
       </c>
-      <c r="K45" s="28"/>
-      <c r="L45" s="28">
+      <c r="K45" s="29"/>
+      <c r="L45" s="29">
         <v>8</v>
       </c>
-      <c r="M45" s="28"/>
-      <c r="N45" s="28">
+      <c r="M45" s="29"/>
+      <c r="N45" s="29">
         <v>2.8820000000000001</v>
       </c>
-      <c r="O45" s="28"/>
+      <c r="O45" s="29"/>
     </row>
     <row r="46" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B46">
@@ -18699,18 +18909,18 @@
       <c r="I46">
         <v>1000</v>
       </c>
-      <c r="J46" s="28">
+      <c r="J46" s="29">
         <v>3.55</v>
       </c>
-      <c r="K46" s="28"/>
-      <c r="L46" s="28">
+      <c r="K46" s="29"/>
+      <c r="L46" s="29">
         <v>12</v>
       </c>
-      <c r="M46" s="28"/>
-      <c r="N46" s="28">
+      <c r="M46" s="29"/>
+      <c r="N46" s="29">
         <v>4.1079999999999997</v>
       </c>
-      <c r="O46" s="28"/>
+      <c r="O46" s="29"/>
     </row>
     <row r="47" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B47">
@@ -18810,13 +19020,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="J42:K42"/>
-    <mergeCell ref="L42:M42"/>
-    <mergeCell ref="N42:O42"/>
-    <mergeCell ref="N46:O46"/>
-    <mergeCell ref="N45:O45"/>
-    <mergeCell ref="N44:O44"/>
-    <mergeCell ref="N43:O43"/>
     <mergeCell ref="I40:O40"/>
     <mergeCell ref="J43:K43"/>
     <mergeCell ref="J44:K44"/>
@@ -18829,6 +19032,13 @@
     <mergeCell ref="J41:K41"/>
     <mergeCell ref="L41:M41"/>
     <mergeCell ref="N41:O41"/>
+    <mergeCell ref="J42:K42"/>
+    <mergeCell ref="L42:M42"/>
+    <mergeCell ref="N42:O42"/>
+    <mergeCell ref="N46:O46"/>
+    <mergeCell ref="N45:O45"/>
+    <mergeCell ref="N44:O44"/>
+    <mergeCell ref="N43:O43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -18840,7 +19050,7 @@
   <dimension ref="A1:O172"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O29" sqref="O29"/>
+      <selection activeCell="O31" sqref="O31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22153,8 +22363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B2ED3A6-0B67-444E-AD81-36D910E53853}">
   <dimension ref="A1:AW164"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AC3" sqref="AC3"/>
+    <sheetView topLeftCell="AB2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AC7" sqref="AC7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22358,7 +22568,7 @@
         <f>STANDARDIZE(AO5,$AM$6,$AM$7)</f>
         <v>-2.3247457307844104</v>
       </c>
-      <c r="AS5" s="23">
+      <c r="AS5" s="22">
         <f>NORMSDIST(AR5)</f>
         <v>1.0042780206055512E-2</v>
       </c>
@@ -22451,7 +22661,7 @@
         <f t="shared" ref="AR6:AR54" si="7">STANDARDIZE(AO6,$AM$6,$AM$7)</f>
         <v>-2.3247457307844104</v>
       </c>
-      <c r="AS6" s="23">
+      <c r="AS6" s="22">
         <f t="shared" ref="AS6:AS54" si="8">NORMSDIST(AR6)</f>
         <v>1.0042780206055512E-2</v>
       </c>
@@ -22544,7 +22754,7 @@
         <f t="shared" si="7"/>
         <v>-2.3247457307844104</v>
       </c>
-      <c r="AS7" s="23">
+      <c r="AS7" s="22">
         <f t="shared" si="8"/>
         <v>1.0042780206055512E-2</v>
       </c>
@@ -22644,7 +22854,7 @@
         <f t="shared" si="7"/>
         <v>-1.1638983280309203</v>
       </c>
-      <c r="AS8" s="23">
+      <c r="AS8" s="22">
         <f t="shared" si="8"/>
         <v>0.12223260863025018</v>
       </c>
@@ -22737,7 +22947,7 @@
         <f t="shared" si="7"/>
         <v>-1.1638983280309203</v>
       </c>
-      <c r="AS9" s="23">
+      <c r="AS9" s="22">
         <f t="shared" si="8"/>
         <v>0.12223260863025018</v>
       </c>
@@ -22830,7 +23040,7 @@
         <f t="shared" si="7"/>
         <v>-1.1638983280309203</v>
       </c>
-      <c r="AS10" s="23">
+      <c r="AS10" s="22">
         <f t="shared" si="8"/>
         <v>0.12223260863025018</v>
       </c>
@@ -22916,7 +23126,7 @@
         <f t="shared" si="7"/>
         <v>-1.1638983280309203</v>
       </c>
-      <c r="AS11" s="23">
+      <c r="AS11" s="22">
         <f t="shared" si="8"/>
         <v>0.12223260863025018</v>
       </c>
@@ -23002,7 +23212,7 @@
         <f t="shared" si="7"/>
         <v>-1.1638983280309203</v>
       </c>
-      <c r="AS12" s="23">
+      <c r="AS12" s="22">
         <f t="shared" si="8"/>
         <v>0.12223260863025018</v>
       </c>
@@ -23088,7 +23298,7 @@
         <f t="shared" si="7"/>
         <v>-1.1638983280309203</v>
       </c>
-      <c r="AS13" s="23">
+      <c r="AS13" s="22">
         <f t="shared" si="8"/>
         <v>0.12223260863025018</v>
       </c>
@@ -23174,7 +23384,7 @@
         <f t="shared" si="7"/>
         <v>-1.1638983280309203</v>
       </c>
-      <c r="AS14" s="23">
+      <c r="AS14" s="22">
         <f t="shared" si="8"/>
         <v>0.12223260863025018</v>
       </c>
@@ -23260,7 +23470,7 @@
         <f t="shared" si="7"/>
         <v>-3.0509252774302462E-3</v>
       </c>
-      <c r="AS15" s="23">
+      <c r="AS15" s="22">
         <f t="shared" si="8"/>
         <v>0.49878285880070905</v>
       </c>
@@ -23346,7 +23556,7 @@
         <f t="shared" si="7"/>
         <v>-3.0509252774302462E-3</v>
       </c>
-      <c r="AS16" s="23">
+      <c r="AS16" s="22">
         <f t="shared" si="8"/>
         <v>0.49878285880070905</v>
       </c>
@@ -23432,7 +23642,7 @@
         <f t="shared" si="7"/>
         <v>-3.0509252774302462E-3</v>
       </c>
-      <c r="AS17" s="23">
+      <c r="AS17" s="22">
         <f t="shared" si="8"/>
         <v>0.49878285880070905</v>
       </c>
@@ -23518,7 +23728,7 @@
         <f t="shared" si="7"/>
         <v>-3.0509252774302462E-3</v>
       </c>
-      <c r="AS18" s="23">
+      <c r="AS18" s="22">
         <f t="shared" si="8"/>
         <v>0.49878285880070905</v>
       </c>
@@ -23604,7 +23814,7 @@
         <f t="shared" si="7"/>
         <v>-3.0509252774302462E-3</v>
       </c>
-      <c r="AS19" s="23">
+      <c r="AS19" s="22">
         <f t="shared" si="8"/>
         <v>0.49878285880070905</v>
       </c>
@@ -23690,7 +23900,7 @@
         <f t="shared" si="7"/>
         <v>-3.0509252774302462E-3</v>
       </c>
-      <c r="AS20" s="23">
+      <c r="AS20" s="22">
         <f t="shared" si="8"/>
         <v>0.49878285880070905</v>
       </c>
@@ -23776,7 +23986,7 @@
         <f t="shared" si="7"/>
         <v>-3.0509252774302462E-3</v>
       </c>
-      <c r="AS21" s="23">
+      <c r="AS21" s="22">
         <f t="shared" si="8"/>
         <v>0.49878285880070905</v>
       </c>
@@ -23862,7 +24072,7 @@
         <f t="shared" si="7"/>
         <v>-3.0509252774302462E-3</v>
       </c>
-      <c r="AS22" s="23">
+      <c r="AS22" s="22">
         <f t="shared" si="8"/>
         <v>0.49878285880070905</v>
       </c>
@@ -23948,7 +24158,7 @@
         <f t="shared" si="7"/>
         <v>-3.0509252774302462E-3</v>
       </c>
-      <c r="AS23" s="23">
+      <c r="AS23" s="22">
         <f t="shared" si="8"/>
         <v>0.49878285880070905</v>
       </c>
@@ -24034,7 +24244,7 @@
         <f t="shared" si="7"/>
         <v>-3.0509252774302462E-3</v>
       </c>
-      <c r="AS24" s="23">
+      <c r="AS24" s="22">
         <f t="shared" si="8"/>
         <v>0.49878285880070905</v>
       </c>
@@ -24120,7 +24330,7 @@
         <f t="shared" si="7"/>
         <v>-3.0509252774302462E-3</v>
       </c>
-      <c r="AS25" s="23">
+      <c r="AS25" s="22">
         <f t="shared" si="8"/>
         <v>0.49878285880070905</v>
       </c>
@@ -24206,7 +24416,7 @@
         <f t="shared" si="7"/>
         <v>-3.0509252774302462E-3</v>
       </c>
-      <c r="AS26" s="23">
+      <c r="AS26" s="22">
         <f t="shared" si="8"/>
         <v>0.49878285880070905</v>
       </c>
@@ -24292,7 +24502,7 @@
         <f t="shared" si="7"/>
         <v>-3.0509252774302462E-3</v>
       </c>
-      <c r="AS27" s="23">
+      <c r="AS27" s="22">
         <f t="shared" si="8"/>
         <v>0.49878285880070905</v>
       </c>
@@ -24378,7 +24588,7 @@
         <f t="shared" si="7"/>
         <v>-3.0509252774302462E-3</v>
       </c>
-      <c r="AS28" s="23">
+      <c r="AS28" s="22">
         <f t="shared" si="8"/>
         <v>0.49878285880070905</v>
       </c>
@@ -24464,7 +24674,7 @@
         <f t="shared" si="7"/>
         <v>-3.0509252774302462E-3</v>
       </c>
-      <c r="AS29" s="23">
+      <c r="AS29" s="22">
         <f t="shared" si="8"/>
         <v>0.49878285880070905</v>
       </c>
@@ -24550,7 +24760,7 @@
         <f t="shared" si="7"/>
         <v>-3.0509252774302462E-3</v>
       </c>
-      <c r="AS30" s="23">
+      <c r="AS30" s="22">
         <f t="shared" si="8"/>
         <v>0.49878285880070905</v>
       </c>
@@ -24636,7 +24846,7 @@
         <f t="shared" si="7"/>
         <v>-3.0509252774302462E-3</v>
       </c>
-      <c r="AS31" s="23">
+      <c r="AS31" s="22">
         <f t="shared" si="8"/>
         <v>0.49878285880070905</v>
       </c>
@@ -24722,7 +24932,7 @@
         <f t="shared" si="7"/>
         <v>-3.0509252774302462E-3</v>
       </c>
-      <c r="AS32" s="23">
+      <c r="AS32" s="22">
         <f t="shared" si="8"/>
         <v>0.49878285880070905</v>
       </c>
@@ -24808,7 +25018,7 @@
         <f t="shared" si="7"/>
         <v>-3.0509252774302462E-3</v>
       </c>
-      <c r="AS33" s="23">
+      <c r="AS33" s="22">
         <f t="shared" si="8"/>
         <v>0.49878285880070905</v>
       </c>
@@ -24894,7 +25104,7 @@
         <f t="shared" si="7"/>
         <v>-3.0509252774302462E-3</v>
       </c>
-      <c r="AS34" s="23">
+      <c r="AS34" s="22">
         <f t="shared" si="8"/>
         <v>0.49878285880070905</v>
       </c>
@@ -24980,7 +25190,7 @@
         <f t="shared" si="7"/>
         <v>-3.0509252774302462E-3</v>
       </c>
-      <c r="AS35" s="23">
+      <c r="AS35" s="22">
         <f t="shared" si="8"/>
         <v>0.49878285880070905</v>
       </c>
@@ -25066,7 +25276,7 @@
         <f t="shared" si="7"/>
         <v>-2.949733433151597E-3</v>
       </c>
-      <c r="AS36" s="23">
+      <c r="AS36" s="22">
         <f t="shared" si="8"/>
         <v>0.4988232283241032</v>
       </c>
@@ -25152,7 +25362,7 @@
         <f t="shared" si="7"/>
         <v>-2.9240982927106174E-3</v>
       </c>
-      <c r="AS37" s="23">
+      <c r="AS37" s="22">
         <f t="shared" si="8"/>
         <v>0.49883345522138284</v>
       </c>
@@ -25238,7 +25448,7 @@
         <f t="shared" si="7"/>
         <v>-1.4365884498512879E-3</v>
       </c>
-      <c r="AS38" s="23">
+      <c r="AS38" s="22">
         <f t="shared" si="8"/>
         <v>0.49942688432494936</v>
       </c>
@@ -25324,7 +25534,7 @@
         <f t="shared" si="7"/>
         <v>-1.1439574403560573E-3</v>
       </c>
-      <c r="AS39" s="23">
+      <c r="AS39" s="22">
         <f t="shared" si="8"/>
         <v>0.49954362710960004</v>
       </c>
@@ -25410,7 +25620,7 @@
         <f t="shared" si="7"/>
         <v>6.5550037900623962E-6</v>
       </c>
-      <c r="AS40" s="23">
+      <c r="AS40" s="22">
         <f t="shared" si="8"/>
         <v>0.50000261506816002</v>
       </c>
@@ -25496,7 +25706,7 @@
         <f t="shared" si="7"/>
         <v>4.260001187246962E-4</v>
       </c>
-      <c r="AS41" s="23">
+      <c r="AS41" s="22">
         <f t="shared" si="8"/>
         <v>0.5001699494536751</v>
       </c>
@@ -25582,7 +25792,7 @@
         <f t="shared" si="7"/>
         <v>1.1135326074616554E-3</v>
       </c>
-      <c r="AS42" s="23">
+      <c r="AS42" s="22">
         <f t="shared" si="8"/>
         <v>0.50044423514591685</v>
       </c>
@@ -25668,7 +25878,7 @@
         <f t="shared" si="7"/>
         <v>2.5064468019412419E-2</v>
       </c>
-      <c r="AS43" s="23">
+      <c r="AS43" s="22">
         <f t="shared" si="8"/>
         <v>0.50999822915724069</v>
       </c>
@@ -25754,7 +25964,7 @@
         <f t="shared" si="7"/>
         <v>1.1577964774760598</v>
       </c>
-      <c r="AS44" s="23">
+      <c r="AS44" s="22">
         <f t="shared" si="8"/>
         <v>0.87652644938718871</v>
       </c>
@@ -25840,7 +26050,7 @@
         <f t="shared" si="7"/>
         <v>1.1577964774760598</v>
       </c>
-      <c r="AS45" s="23">
+      <c r="AS45" s="22">
         <f t="shared" si="8"/>
         <v>0.87652644938718871</v>
       </c>
@@ -25926,7 +26136,7 @@
         <f t="shared" si="7"/>
         <v>1.1577964774760598</v>
       </c>
-      <c r="AS46" s="23">
+      <c r="AS46" s="22">
         <f t="shared" si="8"/>
         <v>0.87652644938718871</v>
       </c>
@@ -26012,7 +26222,7 @@
         <f t="shared" si="7"/>
         <v>1.1577964774760598</v>
       </c>
-      <c r="AS47" s="23">
+      <c r="AS47" s="22">
         <f t="shared" si="8"/>
         <v>0.87652644938718871</v>
       </c>
@@ -26098,7 +26308,7 @@
         <f t="shared" si="7"/>
         <v>1.1577964774760598</v>
       </c>
-      <c r="AS48" s="23">
+      <c r="AS48" s="22">
         <f t="shared" si="8"/>
         <v>0.87652644938718871</v>
       </c>
@@ -26184,7 +26394,7 @@
         <f t="shared" si="7"/>
         <v>1.1577964774760598</v>
       </c>
-      <c r="AS49" s="23">
+      <c r="AS49" s="22">
         <f t="shared" si="8"/>
         <v>0.87652644938718871</v>
       </c>
@@ -26270,7 +26480,7 @@
         <f t="shared" si="7"/>
         <v>1.1592790111378333</v>
       </c>
-      <c r="AS50" s="23">
+      <c r="AS50" s="22">
         <f t="shared" si="8"/>
         <v>0.87682876286419187</v>
       </c>
@@ -26356,7 +26566,7 @@
         <f t="shared" si="7"/>
         <v>1.1624006401585241</v>
       </c>
-      <c r="AS51" s="23">
+      <c r="AS51" s="22">
         <f t="shared" si="8"/>
         <v>0.87746361830713249</v>
       </c>
@@ -26442,7 +26652,7 @@
         <f t="shared" si="7"/>
         <v>1.165813263808597</v>
       </c>
-      <c r="AS52" s="23">
+      <c r="AS52" s="22">
         <f t="shared" si="8"/>
         <v>0.87815502334545448</v>
       </c>
@@ -26528,7 +26738,7 @@
         <f t="shared" si="7"/>
         <v>2.3186438802295499</v>
       </c>
-      <c r="AS53" s="23">
+      <c r="AS53" s="22">
         <f t="shared" si="8"/>
         <v>0.9897928231174431</v>
       </c>
@@ -26614,7 +26824,7 @@
         <f t="shared" si="7"/>
         <v>2.4145230810715312</v>
       </c>
-      <c r="AS54" s="23">
+      <c r="AS54" s="22">
         <f t="shared" si="8"/>
         <v>0.99212208765952326</v>
       </c>
@@ -32420,8 +32630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BEB8E32-D847-46DD-A9C2-FCA6CC8CF645}">
   <dimension ref="A1:U102"/>
   <sheetViews>
-    <sheetView topLeftCell="B16" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34677,7 +34887,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CE560BB-010F-4538-8606-72D35C2079F1}">
   <dimension ref="A1:Z102"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T27" sqref="T27"/>
     </sheetView>
   </sheetViews>
@@ -37339,8 +37549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB00259A-76EF-42CC-A63F-F0BB8151E029}">
   <dimension ref="A1:V102"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39590,4 +39800,42 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6DE4954-B822-463F-AF49-CD5C62D3DBE0}">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" s="5">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated data collection excel with new testing
</commit_message>
<xml_diff>
--- a/Data Collection.xlsx
+++ b/Data Collection.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yoga\Desktop\University\Thesis\TrustChain-Simulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DDB4FBC-55FC-4FFF-AC8C-DE62208D0B27}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7AD2171-4C2C-4B90-9EFA-BA7B4A9BA3F4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="28440" xr2:uid="{BCACAF04-D4C4-41AE-BAB0-4F6EFB70057E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BCACAF04-D4C4-41AE-BAB0-4F6EFB70057E}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Planning" sheetId="3" r:id="rId1"/>
@@ -24,10 +24,10 @@
     <sheet name="Set9" sheetId="11" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'Set4'!$E$61</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'Set4'!$E$62:$E$161</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'Set4'!$E$4</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'Set4'!$E$5:$E$54</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">'Set4'!$E$4</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'Set4'!$E$5:$E$54</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'Set4'!$E$61</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'Set4'!$E$62:$E$161</definedName>
     <definedName name="solver_eng" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_num" localSheetId="3" hidden="1">0</definedName>
@@ -315,9 +315,6 @@
     <t>Exection time: 14 s</t>
   </si>
   <si>
-    <t>Creaft network with same number of node but higer dist (watts - strogatz)</t>
-  </si>
-  <si>
     <t>Do one more set with 20 evil</t>
   </si>
   <si>
@@ -387,9 +384,6 @@
     <t>Nodes</t>
   </si>
   <si>
-    <t>9 - Average Path Length</t>
-  </si>
-  <si>
     <t>Path Length</t>
   </si>
   <si>
@@ -397,6 +391,13 @@
   </si>
   <si>
     <t>dissemination + direct connection after the first message</t>
+  </si>
+  <si>
+    <t>9 - Average Path Length
+(WattsStrogatz)</t>
+  </si>
+  <si>
+    <t>simulation with many evil node</t>
   </si>
 </sst>
 </file>
@@ -684,7 +685,7 @@
     <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -724,6 +725,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="12" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -739,7 +741,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="12" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="60% - Accent1" xfId="12" builtinId="32"/>
@@ -6460,7 +6464,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -6498,7 +6502,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{00000000-BA23-47F0-8325-162A3EB2469F}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.2</cx:f>
+              <cx:f>_xlchart.v1.0</cx:f>
               <cx:v>Standardized </cx:v>
             </cx:txData>
           </cx:tx>
@@ -6526,7 +6530,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.1</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -6564,7 +6568,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{00000000-92AE-4E86-80B1-3A198ACB5431}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.0</cx:f>
+              <cx:f>_xlchart.v1.2</cx:f>
               <cx:v>Standardized </cx:v>
             </cx:txData>
           </cx:tx>
@@ -15815,8 +15819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4891D42F-3971-43B5-986A-C0853C8465A0}">
   <dimension ref="A1:T49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15860,7 +15864,7 @@
         <v>13</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>0</v>
@@ -15891,7 +15895,7 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="27" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="4">
@@ -15935,7 +15939,7 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="25"/>
+      <c r="A3" s="26"/>
       <c r="B3" s="4">
         <v>2</v>
       </c>
@@ -15977,7 +15981,7 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="25"/>
+      <c r="A4" s="26"/>
       <c r="B4" s="4">
         <v>3</v>
       </c>
@@ -16023,7 +16027,7 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="25"/>
+      <c r="A5" s="26"/>
       <c r="B5" s="4">
         <v>4</v>
       </c>
@@ -16066,7 +16070,7 @@
       <c r="T5" s="1"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="25"/>
+      <c r="A6" s="26"/>
       <c r="B6" s="4">
         <v>5</v>
       </c>
@@ -16112,7 +16116,7 @@
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="25"/>
+      <c r="A7" s="26"/>
       <c r="B7" s="4">
         <v>6</v>
       </c>
@@ -16155,7 +16159,7 @@
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="28" t="s">
         <v>25</v>
       </c>
       <c r="B8" s="5">
@@ -16202,7 +16206,7 @@
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="27"/>
+      <c r="A9" s="28"/>
       <c r="B9" s="5">
         <v>2</v>
       </c>
@@ -16247,7 +16251,7 @@
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="27"/>
+      <c r="A10" s="28"/>
       <c r="B10" s="5">
         <v>3</v>
       </c>
@@ -16292,7 +16296,7 @@
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="27" t="s">
+      <c r="A11" s="28" t="s">
         <v>26</v>
       </c>
       <c r="B11" s="6">
@@ -16336,7 +16340,7 @@
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="27"/>
+      <c r="A12" s="28"/>
       <c r="B12" s="6">
         <v>2</v>
       </c>
@@ -16378,7 +16382,7 @@
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
+      <c r="A13" s="28"/>
       <c r="B13" s="6">
         <v>3</v>
       </c>
@@ -16420,7 +16424,7 @@
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="27"/>
+      <c r="A14" s="28"/>
       <c r="B14" s="6">
         <v>4</v>
       </c>
@@ -16462,7 +16466,7 @@
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="27"/>
+      <c r="A15" s="28"/>
       <c r="B15" s="6">
         <v>5</v>
       </c>
@@ -16504,7 +16508,7 @@
       </c>
     </row>
     <row r="16" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="27"/>
+      <c r="A16" s="28"/>
       <c r="B16" s="6">
         <v>6</v>
       </c>
@@ -16682,7 +16686,7 @@
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="25" t="s">
+      <c r="A20" s="26" t="s">
         <v>47</v>
       </c>
       <c r="B20" s="10">
@@ -16726,7 +16730,7 @@
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="25"/>
+      <c r="A21" s="26"/>
       <c r="B21" s="11">
         <v>2</v>
       </c>
@@ -16768,7 +16772,7 @@
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="25"/>
+      <c r="A22" s="26"/>
       <c r="B22" s="10">
         <v>3</v>
       </c>
@@ -16810,7 +16814,7 @@
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="25"/>
+      <c r="A23" s="26"/>
       <c r="B23" s="11">
         <v>4</v>
       </c>
@@ -16852,7 +16856,7 @@
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="25"/>
+      <c r="A24" s="26"/>
       <c r="B24" s="10">
         <v>5</v>
       </c>
@@ -16894,7 +16898,7 @@
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25" s="28" t="s">
+      <c r="A25" s="29" t="s">
         <v>57</v>
       </c>
       <c r="B25" s="12">
@@ -16941,7 +16945,7 @@
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A26" s="28"/>
+      <c r="A26" s="29"/>
       <c r="B26" s="12">
         <v>2</v>
       </c>
@@ -16983,7 +16987,7 @@
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" s="28"/>
+      <c r="A27" s="29"/>
       <c r="B27" s="12">
         <v>3</v>
       </c>
@@ -17025,7 +17029,7 @@
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A28" s="28"/>
+      <c r="A28" s="29"/>
       <c r="B28" s="12">
         <v>4</v>
       </c>
@@ -17067,7 +17071,7 @@
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A29" s="28"/>
+      <c r="A29" s="29"/>
       <c r="B29" s="12">
         <v>5</v>
       </c>
@@ -17109,7 +17113,7 @@
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A30" s="28"/>
+      <c r="A30" s="29"/>
       <c r="B30" s="12">
         <v>6</v>
       </c>
@@ -17151,7 +17155,7 @@
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A31" s="25" t="s">
+      <c r="A31" s="26" t="s">
         <v>58</v>
       </c>
       <c r="B31" s="14">
@@ -17195,7 +17199,7 @@
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A32" s="25"/>
+      <c r="A32" s="26"/>
       <c r="B32" s="14">
         <v>2</v>
       </c>
@@ -17237,7 +17241,7 @@
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" s="25"/>
+      <c r="A33" s="26"/>
       <c r="B33" s="14">
         <v>3</v>
       </c>
@@ -17279,7 +17283,7 @@
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="25"/>
+      <c r="A34" s="26"/>
       <c r="B34" s="14">
         <v>4</v>
       </c>
@@ -17321,7 +17325,7 @@
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" s="25"/>
+      <c r="A35" s="26"/>
       <c r="B35" s="14">
         <v>5</v>
       </c>
@@ -17363,10 +17367,10 @@
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="B36" s="30">
+      <c r="A36" s="31" t="s">
+        <v>113</v>
+      </c>
+      <c r="B36" s="25">
         <v>1</v>
       </c>
       <c r="C36" s="1">
@@ -17404,7 +17408,8 @@
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B37" s="30">
+      <c r="A37" s="29"/>
+      <c r="B37" s="25">
         <v>2</v>
       </c>
       <c r="C37" s="24">
@@ -17442,7 +17447,8 @@
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B38" s="30">
+      <c r="A38" s="29"/>
+      <c r="B38" s="25">
         <v>3</v>
       </c>
       <c r="C38" s="24">
@@ -17480,7 +17486,8 @@
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B39" s="30">
+      <c r="A39" s="29"/>
+      <c r="B39" s="25">
         <v>4</v>
       </c>
       <c r="C39" s="24">
@@ -17518,8 +17525,8 @@
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A40" s="23"/>
-      <c r="B40" s="30">
+      <c r="A40" s="29"/>
+      <c r="B40" s="25">
         <v>5</v>
       </c>
       <c r="C40" s="24">
@@ -17558,7 +17565,7 @@
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
@@ -17584,6 +17591,9 @@
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A42" s="13" t="s">
+        <v>114</v>
+      </c>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
@@ -17599,7 +17609,7 @@
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="49" spans="3:7" x14ac:dyDescent="0.25">
@@ -17608,7 +17618,8 @@
       <c r="G49" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="A36:A40"/>
     <mergeCell ref="A31:A35"/>
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="A8:A10"/>
@@ -17625,8 +17636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF874DAA-691A-4835-ACA3-DB30922CFD6B}">
   <dimension ref="A1:W52"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F59" sqref="F59"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18580,9 +18591,6 @@
       <c r="E30">
         <v>1.2204000000040001</v>
       </c>
-      <c r="S30" s="21" t="s">
-        <v>87</v>
-      </c>
     </row>
     <row r="31" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B31">
@@ -18723,15 +18731,15 @@
       <c r="E40">
         <v>0.91530000000300005</v>
       </c>
-      <c r="I40" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="J40" s="28"/>
-      <c r="K40" s="28"/>
-      <c r="L40" s="28"/>
-      <c r="M40" s="28"/>
-      <c r="N40" s="28"/>
-      <c r="O40" s="28"/>
+      <c r="I40" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="J40" s="29"/>
+      <c r="K40" s="29"/>
+      <c r="L40" s="29"/>
+      <c r="M40" s="29"/>
+      <c r="N40" s="29"/>
+      <c r="O40" s="29"/>
     </row>
     <row r="41" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B41">
@@ -18747,20 +18755,20 @@
         <v>0.61020000000200003</v>
       </c>
       <c r="I41" t="s">
-        <v>110</v>
-      </c>
-      <c r="J41" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="J41" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="K41" s="30"/>
+      <c r="L41" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="K41" s="29"/>
-      <c r="L41" s="29" t="s">
+      <c r="M41" s="30"/>
+      <c r="N41" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="M41" s="29"/>
-      <c r="N41" s="29" t="s">
-        <v>109</v>
-      </c>
-      <c r="O41" s="29"/>
+      <c r="O41" s="30"/>
     </row>
     <row r="42" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B42">
@@ -18781,18 +18789,18 @@
       <c r="I42">
         <v>10</v>
       </c>
-      <c r="J42" s="29">
+      <c r="J42" s="30">
         <v>1.2</v>
       </c>
-      <c r="K42" s="29"/>
-      <c r="L42" s="29">
+      <c r="K42" s="30"/>
+      <c r="L42" s="30">
         <v>3</v>
       </c>
-      <c r="M42" s="29"/>
-      <c r="N42" s="29">
+      <c r="M42" s="30"/>
+      <c r="N42" s="30">
         <v>1.7929999999999999</v>
       </c>
-      <c r="O42" s="29"/>
+      <c r="O42" s="30"/>
     </row>
     <row r="43" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B43">
@@ -18813,18 +18821,18 @@
       <c r="I43">
         <v>20</v>
       </c>
-      <c r="J43" s="29">
+      <c r="J43" s="30">
         <v>1.3</v>
       </c>
-      <c r="K43" s="29"/>
-      <c r="L43" s="29">
+      <c r="K43" s="30"/>
+      <c r="L43" s="30">
         <v>4</v>
       </c>
-      <c r="M43" s="29"/>
-      <c r="N43" s="29">
+      <c r="M43" s="30"/>
+      <c r="N43" s="30">
         <v>1.8839999999999999</v>
       </c>
-      <c r="O43" s="29"/>
+      <c r="O43" s="30"/>
     </row>
     <row r="44" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B44">
@@ -18845,18 +18853,18 @@
       <c r="I44">
         <v>50</v>
       </c>
-      <c r="J44" s="29">
+      <c r="J44" s="30">
         <v>2.36</v>
       </c>
-      <c r="K44" s="29"/>
-      <c r="L44" s="29">
+      <c r="K44" s="30"/>
+      <c r="L44" s="30">
         <v>6</v>
       </c>
-      <c r="M44" s="29"/>
-      <c r="N44" s="29">
+      <c r="M44" s="30"/>
+      <c r="N44" s="30">
         <v>2.2669999999999999</v>
       </c>
-      <c r="O44" s="29"/>
+      <c r="O44" s="30"/>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45">
@@ -18877,18 +18885,18 @@
       <c r="I45">
         <v>100</v>
       </c>
-      <c r="J45" s="29">
+      <c r="J45" s="30">
         <v>2.5499999999999998</v>
       </c>
-      <c r="K45" s="29"/>
-      <c r="L45" s="29">
+      <c r="K45" s="30"/>
+      <c r="L45" s="30">
         <v>8</v>
       </c>
-      <c r="M45" s="29"/>
-      <c r="N45" s="29">
+      <c r="M45" s="30"/>
+      <c r="N45" s="30">
         <v>2.8820000000000001</v>
       </c>
-      <c r="O45" s="29"/>
+      <c r="O45" s="30"/>
     </row>
     <row r="46" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B46">
@@ -18909,18 +18917,18 @@
       <c r="I46">
         <v>1000</v>
       </c>
-      <c r="J46" s="29">
+      <c r="J46" s="30">
         <v>3.55</v>
       </c>
-      <c r="K46" s="29"/>
-      <c r="L46" s="29">
+      <c r="K46" s="30"/>
+      <c r="L46" s="30">
         <v>12</v>
       </c>
-      <c r="M46" s="29"/>
-      <c r="N46" s="29">
+      <c r="M46" s="30"/>
+      <c r="N46" s="30">
         <v>4.1079999999999997</v>
       </c>
-      <c r="O46" s="29"/>
+      <c r="O46" s="30"/>
     </row>
     <row r="47" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B47">
@@ -19020,6 +19028,9 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="N45:O45"/>
+    <mergeCell ref="N44:O44"/>
+    <mergeCell ref="N43:O43"/>
     <mergeCell ref="I40:O40"/>
     <mergeCell ref="J43:K43"/>
     <mergeCell ref="J44:K44"/>
@@ -19036,9 +19047,6 @@
     <mergeCell ref="L42:M42"/>
     <mergeCell ref="N42:O42"/>
     <mergeCell ref="N46:O46"/>
-    <mergeCell ref="N45:O45"/>
-    <mergeCell ref="N44:O44"/>
-    <mergeCell ref="N43:O43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -19050,7 +19058,7 @@
   <dimension ref="A1:O172"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O31" sqref="O31"/>
+      <selection activeCell="P31" sqref="P31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19681,7 +19689,7 @@
         <v>0.92352396971999995</v>
       </c>
       <c r="O29" s="21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.25">
@@ -22363,7 +22371,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B2ED3A6-0B67-444E-AD81-36D910E53853}">
   <dimension ref="A1:AW164"/>
   <sheetViews>
-    <sheetView topLeftCell="AB2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AC7" sqref="AC7"/>
     </sheetView>
   </sheetViews>
@@ -22410,7 +22418,7 @@
         <v>43</v>
       </c>
       <c r="AC3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:49" x14ac:dyDescent="0.25">
@@ -22445,43 +22453,43 @@
         <v>31</v>
       </c>
       <c r="AD4" t="s">
+        <v>89</v>
+      </c>
+      <c r="AE4" t="s">
         <v>90</v>
       </c>
-      <c r="AE4" t="s">
-        <v>91</v>
-      </c>
       <c r="AF4" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>92</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>93</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>94</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>95</v>
+      </c>
+      <c r="AO4" t="s">
+        <v>89</v>
+      </c>
+      <c r="AP4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AQ4" t="s">
+        <v>100</v>
+      </c>
+      <c r="AR4" t="s">
         <v>101</v>
       </c>
-      <c r="AG4" t="s">
-        <v>93</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>94</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>95</v>
-      </c>
-      <c r="AJ4" t="s">
-        <v>96</v>
-      </c>
-      <c r="AO4" t="s">
-        <v>90</v>
-      </c>
-      <c r="AP4" t="s">
-        <v>91</v>
-      </c>
-      <c r="AQ4" t="s">
-        <v>101</v>
-      </c>
-      <c r="AR4" t="s">
+      <c r="AS4" t="s">
         <v>102</v>
       </c>
-      <c r="AS4" t="s">
+      <c r="AT4" t="s">
         <v>103</v>
-      </c>
-      <c r="AT4" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:49" ht="15.75" x14ac:dyDescent="0.25">
@@ -22734,7 +22742,7 @@
         <v>2.9957219793944487E-2</v>
       </c>
       <c r="AL7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AM7">
         <f>_xlfn.STDEV.S(AD5:AD54)</f>
@@ -22763,7 +22771,7 @@
         <v>4.9957219793944484E-2</v>
       </c>
       <c r="AV7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AW7">
         <f>MAX(AT5:AT54)</f>
@@ -22863,7 +22871,7 @@
         <v>4.2232608630250176E-2</v>
       </c>
       <c r="AV8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AW8">
         <f>0.18845</f>
@@ -23020,7 +23028,7 @@
         <v>2.2232608630250172E-2</v>
       </c>
       <c r="AL10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AM10">
         <f>0.18845</f>
@@ -26879,10 +26887,10 @@
         <v>44</v>
       </c>
       <c r="O60" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AC60" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="61" spans="1:46" x14ac:dyDescent="0.25">
@@ -26911,25 +26919,25 @@
         <v>31</v>
       </c>
       <c r="AD61" t="s">
+        <v>89</v>
+      </c>
+      <c r="AE61" t="s">
         <v>90</v>
       </c>
-      <c r="AE61" t="s">
+      <c r="AF61" t="s">
         <v>91</v>
       </c>
-      <c r="AF61" t="s">
+      <c r="AG61" t="s">
         <v>92</v>
       </c>
-      <c r="AG61" t="s">
+      <c r="AH61" t="s">
         <v>93</v>
       </c>
-      <c r="AH61" t="s">
+      <c r="AI61" t="s">
         <v>94</v>
       </c>
-      <c r="AI61" t="s">
+      <c r="AJ61" t="s">
         <v>95</v>
-      </c>
-      <c r="AJ61" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="62" spans="1:46" x14ac:dyDescent="0.25">
@@ -27114,7 +27122,7 @@
         <v>6.410067001008506E-3</v>
       </c>
       <c r="AL64" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AM64">
         <f>_xlfn.STDEV.S(AD62:AD161)</f>
@@ -27296,7 +27304,7 @@
         <v>3.641006700100851E-2</v>
       </c>
       <c r="AL67" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AM67">
         <f>1.3581/SQRT(AM62)</f>
@@ -37550,7 +37558,7 @@
   <dimension ref="A1:V102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39806,8 +39814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6DE4954-B822-463F-AF49-CD5C62D3DBE0}">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39817,7 +39825,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B1" s="5">
         <v>1</v>

</xml_diff>

<commit_message>
implemtend randomization on evil node id
</commit_message>
<xml_diff>
--- a/Data Collection.xlsx
+++ b/Data Collection.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yoga\Desktop\University\Thesis\TrustChain-Simulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7AD2171-4C2C-4B90-9EFA-BA7B4A9BA3F4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{767513A8-1E84-4CF1-A0C8-911C3C2F6894}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BCACAF04-D4C4-41AE-BAB0-4F6EFB70057E}"/>
+    <workbookView xWindow="6435" yWindow="495" windowWidth="16215" windowHeight="15240" xr2:uid="{BCACAF04-D4C4-41AE-BAB0-4F6EFB70057E}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Planning" sheetId="3" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="115">
   <si>
     <t>Evil Node Sleeping Transactions</t>
   </si>
@@ -318,9 +318,6 @@
     <t>Do one more set with 20 evil</t>
   </si>
   <si>
-    <t>7.2 try with a slower than 7.2 mb</t>
-  </si>
-  <si>
     <t>Data Ordered</t>
   </si>
   <si>
@@ -398,6 +395,9 @@
   </si>
   <si>
     <t>simulation with many evil node</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.2 - Initial transactions (slow speed) </t>
   </si>
 </sst>
 </file>
@@ -517,7 +517,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -577,8 +577,14 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -669,8 +675,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -684,8 +699,9 @@
     <xf numFmtId="0" fontId="12" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -720,20 +736,17 @@
     <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="11"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="12" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -741,12 +754,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="13" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="14">
     <cellStyle name="60% - Accent1" xfId="12" builtinId="32"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
     <cellStyle name="60% - Accent4" xfId="9" builtinId="44"/>
     <cellStyle name="60% - Accent6" xfId="8" builtinId="52"/>
     <cellStyle name="Accent1" xfId="7" builtinId="29"/>
@@ -15817,15 +15838,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4891D42F-3971-43B5-986A-C0853C8465A0}">
-  <dimension ref="A1:T49"/>
+  <dimension ref="A1:T52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N41" sqref="N41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" style="13" customWidth="1"/>
+    <col min="1" max="1" width="31.28515625" style="13" customWidth="1"/>
     <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" hidden="1" customWidth="1"/>
@@ -15864,7 +15886,7 @@
         <v>13</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>0</v>
@@ -15895,7 +15917,7 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="30" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="4">
@@ -15915,7 +15937,7 @@
       <c r="F2" s="1">
         <v>0.23</v>
       </c>
-      <c r="G2" s="24"/>
+      <c r="G2" s="23"/>
       <c r="H2" s="1">
         <v>10</v>
       </c>
@@ -15939,7 +15961,7 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="26"/>
+      <c r="A3" s="27"/>
       <c r="B3" s="4">
         <v>2</v>
       </c>
@@ -15957,7 +15979,7 @@
       <c r="F3" s="1">
         <v>0.15</v>
       </c>
-      <c r="G3" s="24"/>
+      <c r="G3" s="23"/>
       <c r="H3" s="1">
         <v>10</v>
       </c>
@@ -15981,7 +16003,7 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
+      <c r="A4" s="27"/>
       <c r="B4" s="4">
         <v>3</v>
       </c>
@@ -15999,7 +16021,7 @@
       <c r="F4" s="1">
         <v>7.9000000000000001E-2</v>
       </c>
-      <c r="G4" s="24"/>
+      <c r="G4" s="23"/>
       <c r="H4" s="1">
         <v>10</v>
       </c>
@@ -16027,7 +16049,7 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="26"/>
+      <c r="A5" s="27"/>
       <c r="B5" s="4">
         <v>4</v>
       </c>
@@ -16045,7 +16067,7 @@
       <c r="F5" s="1">
         <v>4.7E-2</v>
       </c>
-      <c r="G5" s="24"/>
+      <c r="G5" s="23"/>
       <c r="H5" s="1">
         <v>10</v>
       </c>
@@ -16070,7 +16092,7 @@
       <c r="T5" s="1"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="26"/>
+      <c r="A6" s="27"/>
       <c r="B6" s="4">
         <v>5</v>
       </c>
@@ -16089,7 +16111,7 @@
         <f>E6</f>
         <v>6.9077552789821367E-3</v>
       </c>
-      <c r="G6" s="24"/>
+      <c r="G6" s="23"/>
       <c r="H6" s="1">
         <v>10</v>
       </c>
@@ -16116,7 +16138,7 @@
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
+      <c r="A7" s="27"/>
       <c r="B7" s="4">
         <v>6</v>
       </c>
@@ -16132,7 +16154,7 @@
         <v>9.210340371976184E-4</v>
       </c>
       <c r="F7" s="1"/>
-      <c r="G7" s="24"/>
+      <c r="G7" s="23"/>
       <c r="H7" s="1">
         <v>10</v>
       </c>
@@ -16159,7 +16181,7 @@
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="31" t="s">
         <v>25</v>
       </c>
       <c r="B8" s="5">
@@ -16179,7 +16201,7 @@
       <c r="F8" s="1">
         <v>4.7E-2</v>
       </c>
-      <c r="G8" s="24"/>
+      <c r="G8" s="23"/>
       <c r="H8" s="1">
         <v>10</v>
       </c>
@@ -16206,7 +16228,7 @@
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="28"/>
+      <c r="A9" s="31"/>
       <c r="B9" s="5">
         <v>2</v>
       </c>
@@ -16224,7 +16246,7 @@
       <c r="F9" s="1">
         <v>4.7E-2</v>
       </c>
-      <c r="G9" s="24"/>
+      <c r="G9" s="23"/>
       <c r="H9" s="1">
         <v>10</v>
       </c>
@@ -16251,7 +16273,7 @@
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
+      <c r="A10" s="31"/>
       <c r="B10" s="5">
         <v>3</v>
       </c>
@@ -16269,7 +16291,7 @@
       <c r="F10" s="1">
         <v>4.7E-2</v>
       </c>
-      <c r="G10" s="24"/>
+      <c r="G10" s="23"/>
       <c r="H10" s="1">
         <v>10</v>
       </c>
@@ -16296,7 +16318,7 @@
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="31" t="s">
         <v>26</v>
       </c>
       <c r="B11" s="6">
@@ -16316,7 +16338,7 @@
       <c r="F11" s="1">
         <v>4.7E-2</v>
       </c>
-      <c r="G11" s="24"/>
+      <c r="G11" s="23"/>
       <c r="H11" s="1">
         <v>10</v>
       </c>
@@ -16340,7 +16362,7 @@
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="28"/>
+      <c r="A12" s="31"/>
       <c r="B12" s="6">
         <v>2</v>
       </c>
@@ -16358,7 +16380,7 @@
       <c r="F12" s="1">
         <v>4.7E-2</v>
       </c>
-      <c r="G12" s="24"/>
+      <c r="G12" s="23"/>
       <c r="H12" s="1">
         <v>10</v>
       </c>
@@ -16382,7 +16404,7 @@
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="28"/>
+      <c r="A13" s="31"/>
       <c r="B13" s="6">
         <v>3</v>
       </c>
@@ -16400,7 +16422,7 @@
       <c r="F13" s="1">
         <v>4.7E-2</v>
       </c>
-      <c r="G13" s="24"/>
+      <c r="G13" s="23"/>
       <c r="H13" s="1">
         <v>10</v>
       </c>
@@ -16424,7 +16446,7 @@
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="28"/>
+      <c r="A14" s="31"/>
       <c r="B14" s="6">
         <v>4</v>
       </c>
@@ -16442,7 +16464,7 @@
       <c r="F14" s="1">
         <v>4.7E-2</v>
       </c>
-      <c r="G14" s="24"/>
+      <c r="G14" s="23"/>
       <c r="H14" s="1">
         <v>10</v>
       </c>
@@ -16466,7 +16488,7 @@
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="28"/>
+      <c r="A15" s="31"/>
       <c r="B15" s="6">
         <v>5</v>
       </c>
@@ -16484,7 +16506,7 @@
       <c r="F15" s="1">
         <v>4.7E-2</v>
       </c>
-      <c r="G15" s="24"/>
+      <c r="G15" s="23"/>
       <c r="H15" s="1">
         <v>10</v>
       </c>
@@ -16508,7 +16530,7 @@
       </c>
     </row>
     <row r="16" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="28"/>
+      <c r="A16" s="31"/>
       <c r="B16" s="6">
         <v>6</v>
       </c>
@@ -16526,7 +16548,7 @@
       <c r="F16" s="1">
         <v>4.7E-2</v>
       </c>
-      <c r="G16" s="24"/>
+      <c r="G16" s="23"/>
       <c r="H16" s="1">
         <v>10</v>
       </c>
@@ -16550,7 +16572,7 @@
       </c>
     </row>
     <row r="17" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="26" t="s">
         <v>28</v>
       </c>
       <c r="B17" s="8">
@@ -16571,7 +16593,7 @@
         <f>E17</f>
         <v>4.6051701859880917E-2</v>
       </c>
-      <c r="G17" s="24"/>
+      <c r="G17" s="23"/>
       <c r="H17" s="1">
         <v>10</v>
       </c>
@@ -16595,7 +16617,7 @@
       </c>
     </row>
     <row r="18" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="32" t="s">
         <v>46</v>
       </c>
       <c r="B18" s="20">
@@ -16615,7 +16637,7 @@
       <c r="F18" s="1">
         <v>1.243E-2</v>
       </c>
-      <c r="G18" s="24"/>
+      <c r="G18" s="23"/>
       <c r="H18" s="1">
         <v>10</v>
       </c>
@@ -16642,6 +16664,7 @@
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" s="32"/>
       <c r="B19" s="20">
         <v>2</v>
       </c>
@@ -16659,7 +16682,7 @@
       <c r="F19" s="1">
         <v>1.243E-2</v>
       </c>
-      <c r="G19" s="24"/>
+      <c r="G19" s="23"/>
       <c r="H19" s="1">
         <v>2</v>
       </c>
@@ -16686,7 +16709,7 @@
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="26" t="s">
+      <c r="A20" s="27" t="s">
         <v>47</v>
       </c>
       <c r="B20" s="10">
@@ -16706,7 +16729,7 @@
       <c r="F20" s="1">
         <v>4.7E-2</v>
       </c>
-      <c r="G20" s="24"/>
+      <c r="G20" s="23"/>
       <c r="H20" s="1">
         <v>10</v>
       </c>
@@ -16730,7 +16753,7 @@
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="26"/>
+      <c r="A21" s="27"/>
       <c r="B21" s="11">
         <v>2</v>
       </c>
@@ -16748,7 +16771,7 @@
       <c r="F21" s="1">
         <v>4.7E-2</v>
       </c>
-      <c r="G21" s="24"/>
+      <c r="G21" s="23"/>
       <c r="H21" s="1">
         <v>10</v>
       </c>
@@ -16772,7 +16795,7 @@
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="26"/>
+      <c r="A22" s="27"/>
       <c r="B22" s="10">
         <v>3</v>
       </c>
@@ -16790,7 +16813,7 @@
       <c r="F22" s="1">
         <v>4.7E-2</v>
       </c>
-      <c r="G22" s="24"/>
+      <c r="G22" s="23"/>
       <c r="H22" s="1">
         <v>10</v>
       </c>
@@ -16814,7 +16837,7 @@
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="26"/>
+      <c r="A23" s="27"/>
       <c r="B23" s="11">
         <v>4</v>
       </c>
@@ -16832,7 +16855,7 @@
       <c r="F23" s="1">
         <v>4.7E-2</v>
       </c>
-      <c r="G23" s="24"/>
+      <c r="G23" s="23"/>
       <c r="H23" s="1">
         <v>10</v>
       </c>
@@ -16856,7 +16879,7 @@
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="26"/>
+      <c r="A24" s="27"/>
       <c r="B24" s="10">
         <v>5</v>
       </c>
@@ -16874,7 +16897,7 @@
       <c r="F24" s="1">
         <v>4.7E-2</v>
       </c>
-      <c r="G24" s="24"/>
+      <c r="G24" s="23"/>
       <c r="H24" s="1">
         <v>10</v>
       </c>
@@ -16898,7 +16921,7 @@
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25" s="29" t="s">
+      <c r="A25" s="27" t="s">
         <v>57</v>
       </c>
       <c r="B25" s="12">
@@ -16918,7 +16941,7 @@
       <c r="F25" s="1">
         <v>4.7E-2</v>
       </c>
-      <c r="G25" s="24"/>
+      <c r="G25" s="23"/>
       <c r="H25" s="1">
         <v>1</v>
       </c>
@@ -16945,7 +16968,7 @@
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A26" s="29"/>
+      <c r="A26" s="27"/>
       <c r="B26" s="12">
         <v>2</v>
       </c>
@@ -16963,7 +16986,7 @@
       <c r="F26" s="1">
         <v>4.7E-2</v>
       </c>
-      <c r="G26" s="24"/>
+      <c r="G26" s="23"/>
       <c r="H26" s="1">
         <v>2</v>
       </c>
@@ -16987,7 +17010,7 @@
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" s="29"/>
+      <c r="A27" s="27"/>
       <c r="B27" s="12">
         <v>3</v>
       </c>
@@ -17005,7 +17028,7 @@
       <c r="F27" s="1">
         <v>4.7E-2</v>
       </c>
-      <c r="G27" s="24"/>
+      <c r="G27" s="23"/>
       <c r="H27" s="1">
         <v>4</v>
       </c>
@@ -17029,7 +17052,7 @@
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A28" s="29"/>
+      <c r="A28" s="27"/>
       <c r="B28" s="12">
         <v>4</v>
       </c>
@@ -17047,7 +17070,7 @@
       <c r="F28" s="1">
         <v>4.7E-2</v>
       </c>
-      <c r="G28" s="24"/>
+      <c r="G28" s="23"/>
       <c r="H28" s="1">
         <v>8</v>
       </c>
@@ -17071,7 +17094,7 @@
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A29" s="29"/>
+      <c r="A29" s="27"/>
       <c r="B29" s="12">
         <v>5</v>
       </c>
@@ -17089,7 +17112,7 @@
       <c r="F29" s="1">
         <v>4.7E-2</v>
       </c>
-      <c r="G29" s="24"/>
+      <c r="G29" s="23"/>
       <c r="H29" s="1">
         <v>16</v>
       </c>
@@ -17113,7 +17136,7 @@
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A30" s="29"/>
+      <c r="A30" s="27"/>
       <c r="B30" s="12">
         <v>6</v>
       </c>
@@ -17131,7 +17154,7 @@
       <c r="F30" s="1">
         <v>4.7E-2</v>
       </c>
-      <c r="G30" s="24"/>
+      <c r="G30" s="23"/>
       <c r="H30" s="1">
         <v>32</v>
       </c>
@@ -17155,7 +17178,7 @@
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A31" s="26" t="s">
+      <c r="A31" s="27" t="s">
         <v>58</v>
       </c>
       <c r="B31" s="14">
@@ -17175,7 +17198,7 @@
       <c r="F31" s="1">
         <v>4.7E-2</v>
       </c>
-      <c r="G31" s="24"/>
+      <c r="G31" s="23"/>
       <c r="H31" s="1">
         <v>2</v>
       </c>
@@ -17199,7 +17222,7 @@
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A32" s="26"/>
+      <c r="A32" s="27"/>
       <c r="B32" s="14">
         <v>2</v>
       </c>
@@ -17217,7 +17240,7 @@
       <c r="F32" s="1">
         <v>4.7E-2</v>
       </c>
-      <c r="G32" s="24"/>
+      <c r="G32" s="23"/>
       <c r="H32" s="1">
         <v>2</v>
       </c>
@@ -17241,7 +17264,7 @@
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" s="26"/>
+      <c r="A33" s="27"/>
       <c r="B33" s="14">
         <v>3</v>
       </c>
@@ -17259,7 +17282,7 @@
       <c r="F33" s="1">
         <v>4.7E-2</v>
       </c>
-      <c r="G33" s="24"/>
+      <c r="G33" s="23"/>
       <c r="H33" s="1">
         <v>2</v>
       </c>
@@ -17283,7 +17306,7 @@
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="26"/>
+      <c r="A34" s="27"/>
       <c r="B34" s="14">
         <v>4</v>
       </c>
@@ -17301,7 +17324,7 @@
       <c r="F34" s="1">
         <v>4.7E-2</v>
       </c>
-      <c r="G34" s="24"/>
+      <c r="G34" s="23"/>
       <c r="H34" s="1">
         <v>2</v>
       </c>
@@ -17325,7 +17348,7 @@
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" s="26"/>
+      <c r="A35" s="27"/>
       <c r="B35" s="14">
         <v>5</v>
       </c>
@@ -17343,7 +17366,7 @@
       <c r="F35" s="1">
         <v>4.7E-2</v>
       </c>
-      <c r="G35" s="24"/>
+      <c r="G35" s="23"/>
       <c r="H35" s="1">
         <v>2</v>
       </c>
@@ -17367,40 +17390,40 @@
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" s="31" t="s">
-        <v>113</v>
-      </c>
-      <c r="B36" s="25">
+      <c r="A36" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="B36" s="24">
         <v>1</v>
       </c>
       <c r="C36" s="1">
         <v>500</v>
       </c>
       <c r="D36" s="1"/>
-      <c r="E36" s="24">
+      <c r="E36" s="23">
         <f t="shared" si="0"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F36" s="1"/>
-      <c r="G36" s="24">
+      <c r="G36" s="23">
         <v>1</v>
       </c>
       <c r="H36" s="1">
         <v>2</v>
       </c>
-      <c r="I36" s="24">
+      <c r="I36" s="23">
         <v>100</v>
       </c>
-      <c r="J36" s="24">
+      <c r="J36" s="23">
         <v>1</v>
       </c>
-      <c r="K36" s="24" t="s">
+      <c r="K36" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="L36" s="24" t="s">
+      <c r="L36" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="M36" s="24" t="s">
+      <c r="M36" s="23" t="s">
         <v>63</v>
       </c>
       <c r="N36" s="1">
@@ -17408,217 +17431,361 @@
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" s="29"/>
-      <c r="B37" s="25">
+      <c r="A37" s="27"/>
+      <c r="B37" s="24">
         <v>2</v>
       </c>
-      <c r="C37" s="24">
+      <c r="C37" s="23">
         <v>500</v>
       </c>
       <c r="D37" s="1"/>
-      <c r="E37" s="24">
+      <c r="E37" s="23">
         <f t="shared" si="0"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F37" s="1"/>
-      <c r="G37" s="24">
+      <c r="G37" s="23">
         <v>2</v>
       </c>
-      <c r="H37" s="24">
+      <c r="H37" s="23">
         <v>2</v>
       </c>
-      <c r="I37" s="24">
+      <c r="I37" s="23">
         <v>100</v>
       </c>
-      <c r="J37" s="24">
+      <c r="J37" s="23">
         <v>1</v>
       </c>
-      <c r="K37" s="24" t="s">
+      <c r="K37" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="L37" s="24" t="s">
+      <c r="L37" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="M37" s="24" t="s">
+      <c r="M37" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="N37" s="24">
+      <c r="N37" s="23">
         <v>50</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" s="29"/>
-      <c r="B38" s="25">
+      <c r="A38" s="27"/>
+      <c r="B38" s="24">
         <v>3</v>
       </c>
-      <c r="C38" s="24">
+      <c r="C38" s="23">
         <v>500</v>
       </c>
       <c r="D38" s="1"/>
-      <c r="E38" s="24">
+      <c r="E38" s="23">
         <f t="shared" si="0"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F38" s="1"/>
-      <c r="G38" s="24">
+      <c r="G38" s="23">
         <v>5</v>
       </c>
-      <c r="H38" s="24">
+      <c r="H38" s="23">
         <v>2</v>
       </c>
-      <c r="I38" s="24">
+      <c r="I38" s="23">
         <v>100</v>
       </c>
-      <c r="J38" s="24">
+      <c r="J38" s="23">
         <v>1</v>
       </c>
-      <c r="K38" s="24" t="s">
+      <c r="K38" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="L38" s="24" t="s">
+      <c r="L38" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="M38" s="24" t="s">
+      <c r="M38" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="N38" s="24">
+      <c r="N38" s="23">
         <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" s="29"/>
-      <c r="B39" s="25">
+      <c r="A39" s="27"/>
+      <c r="B39" s="24">
         <v>4</v>
       </c>
-      <c r="C39" s="24">
+      <c r="C39" s="23">
         <v>500</v>
       </c>
       <c r="D39" s="1"/>
-      <c r="E39" s="24">
+      <c r="E39" s="23">
         <f t="shared" si="0"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F39" s="1"/>
-      <c r="G39" s="24">
+      <c r="G39" s="23">
         <v>10</v>
       </c>
-      <c r="H39" s="24">
+      <c r="H39" s="23">
         <v>2</v>
       </c>
-      <c r="I39" s="24">
+      <c r="I39" s="23">
         <v>100</v>
       </c>
-      <c r="J39" s="24">
+      <c r="J39" s="23">
         <v>1</v>
       </c>
-      <c r="K39" s="24" t="s">
+      <c r="K39" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="L39" s="24" t="s">
+      <c r="L39" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="M39" s="24" t="s">
+      <c r="M39" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="N39" s="24">
+      <c r="N39" s="23">
         <v>50</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A40" s="29"/>
-      <c r="B40" s="25">
+      <c r="A40" s="27"/>
+      <c r="B40" s="24">
         <v>5</v>
       </c>
-      <c r="C40" s="24">
+      <c r="C40" s="23">
         <v>500</v>
       </c>
-      <c r="D40" s="24"/>
-      <c r="E40" s="24">
-        <f t="shared" ref="E40" si="2">LN(C40)/(C40)</f>
+      <c r="D40" s="23"/>
+      <c r="E40" s="23">
+        <f t="shared" ref="E40:E44" si="2">LN(C40)/(C40)</f>
         <v>1.2429216196844383E-2</v>
       </c>
-      <c r="F40" s="24"/>
-      <c r="G40" s="24">
+      <c r="F40" s="23"/>
+      <c r="G40" s="23">
         <v>100</v>
       </c>
-      <c r="H40" s="24">
+      <c r="H40" s="23">
         <v>2</v>
       </c>
-      <c r="I40" s="24">
+      <c r="I40" s="23">
         <v>100</v>
       </c>
-      <c r="J40" s="24">
+      <c r="J40" s="23">
         <v>1</v>
       </c>
-      <c r="K40" s="24" t="s">
+      <c r="K40" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="L40" s="24" t="s">
+      <c r="L40" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="M40" s="24" t="s">
+      <c r="M40" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="N40" s="24">
+      <c r="N40" s="23">
         <v>50</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A41" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="24"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="24"/>
-      <c r="J41" s="24">
+      <c r="A41" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="B41" s="33">
         <v>1</v>
       </c>
-      <c r="K41" s="24" t="s">
+      <c r="C41" s="25">
+        <v>100</v>
+      </c>
+      <c r="D41" s="25">
+        <f>2*LOG(C41)/(C41-1)</f>
+        <v>4.0404040404040407E-2</v>
+      </c>
+      <c r="E41" s="25">
+        <f t="shared" si="2"/>
+        <v>4.6051701859880917E-2</v>
+      </c>
+      <c r="F41" s="25">
+        <v>4.7E-2</v>
+      </c>
+      <c r="G41" s="25"/>
+      <c r="H41" s="25">
+        <v>1</v>
+      </c>
+      <c r="I41" s="25">
+        <v>100</v>
+      </c>
+      <c r="J41" s="25">
+        <v>1</v>
+      </c>
+      <c r="K41" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="L41" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="M41" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="N41" s="24">
+      <c r="L41" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="M41" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="N41" s="25">
         <v>50</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A42" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="24"/>
-      <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
-      <c r="K42" s="1"/>
-      <c r="L42" s="1"/>
-      <c r="M42" s="1"/>
-      <c r="N42" s="1"/>
+      <c r="A42" s="27"/>
+      <c r="B42" s="33">
+        <v>2</v>
+      </c>
+      <c r="C42" s="25">
+        <v>100</v>
+      </c>
+      <c r="D42" s="25">
+        <f>2*LOG(C42)/(C42-1)</f>
+        <v>4.0404040404040407E-2</v>
+      </c>
+      <c r="E42" s="25">
+        <f t="shared" si="2"/>
+        <v>4.6051701859880917E-2</v>
+      </c>
+      <c r="F42" s="25">
+        <v>4.7E-2</v>
+      </c>
+      <c r="G42" s="25"/>
+      <c r="H42" s="25">
+        <v>2</v>
+      </c>
+      <c r="I42" s="25">
+        <v>100</v>
+      </c>
+      <c r="J42" s="25">
+        <v>1</v>
+      </c>
+      <c r="K42" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="L42" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="M42" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="N42" s="25">
+        <v>50</v>
+      </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A43" s="13" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="49" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C49" s="7"/>
-      <c r="F49" s="7"/>
-      <c r="G49" s="7"/>
+      <c r="A43" s="27"/>
+      <c r="B43" s="33">
+        <v>3</v>
+      </c>
+      <c r="C43" s="25">
+        <v>100</v>
+      </c>
+      <c r="D43" s="25">
+        <f t="shared" ref="D43:D44" si="3">2*LOG(C43)/(C43-1)</f>
+        <v>4.0404040404040407E-2</v>
+      </c>
+      <c r="E43" s="25">
+        <f t="shared" si="2"/>
+        <v>4.6051701859880917E-2</v>
+      </c>
+      <c r="F43" s="25">
+        <v>4.7E-2</v>
+      </c>
+      <c r="G43" s="25"/>
+      <c r="H43" s="25">
+        <v>4</v>
+      </c>
+      <c r="I43" s="25">
+        <v>100</v>
+      </c>
+      <c r="J43" s="25">
+        <v>1</v>
+      </c>
+      <c r="K43" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="L43" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="M43" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="N43" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A44" s="27"/>
+      <c r="B44" s="33">
+        <v>4</v>
+      </c>
+      <c r="C44" s="25">
+        <v>100</v>
+      </c>
+      <c r="D44" s="25">
+        <f t="shared" si="3"/>
+        <v>4.0404040404040407E-2</v>
+      </c>
+      <c r="E44" s="25">
+        <f t="shared" si="2"/>
+        <v>4.6051701859880917E-2</v>
+      </c>
+      <c r="F44" s="25">
+        <v>4.7E-2</v>
+      </c>
+      <c r="G44" s="25"/>
+      <c r="H44" s="25">
+        <v>8</v>
+      </c>
+      <c r="I44" s="25">
+        <v>100</v>
+      </c>
+      <c r="J44" s="25">
+        <v>1</v>
+      </c>
+      <c r="K44" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="L44" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="M44" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="N44" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A45" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="23"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1"/>
+      <c r="K45" s="1"/>
+      <c r="L45" s="1"/>
+      <c r="M45" s="1"/>
+      <c r="N45" s="1"/>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A46" s="13" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="52" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C52" s="7"/>
+      <c r="F52" s="7"/>
+      <c r="G52" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="9">
+    <mergeCell ref="A41:A44"/>
     <mergeCell ref="A36:A40"/>
     <mergeCell ref="A31:A35"/>
     <mergeCell ref="A2:A7"/>
@@ -17626,6 +17793,7 @@
     <mergeCell ref="A11:A16"/>
     <mergeCell ref="A20:A24"/>
     <mergeCell ref="A25:A30"/>
+    <mergeCell ref="A18:A19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -18731,15 +18899,15 @@
       <c r="E40">
         <v>0.91530000000300005</v>
       </c>
-      <c r="I40" s="29" t="s">
-        <v>105</v>
-      </c>
-      <c r="J40" s="29"/>
-      <c r="K40" s="29"/>
-      <c r="L40" s="29"/>
-      <c r="M40" s="29"/>
-      <c r="N40" s="29"/>
-      <c r="O40" s="29"/>
+      <c r="I40" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="J40" s="28"/>
+      <c r="K40" s="28"/>
+      <c r="L40" s="28"/>
+      <c r="M40" s="28"/>
+      <c r="N40" s="28"/>
+      <c r="O40" s="28"/>
     </row>
     <row r="41" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B41">
@@ -18755,20 +18923,20 @@
         <v>0.61020000000200003</v>
       </c>
       <c r="I41" t="s">
-        <v>109</v>
-      </c>
-      <c r="J41" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="J41" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="K41" s="29"/>
+      <c r="L41" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="K41" s="30"/>
-      <c r="L41" s="30" t="s">
+      <c r="M41" s="29"/>
+      <c r="N41" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="M41" s="30"/>
-      <c r="N41" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="O41" s="30"/>
+      <c r="O41" s="29"/>
     </row>
     <row r="42" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B42">
@@ -18789,18 +18957,18 @@
       <c r="I42">
         <v>10</v>
       </c>
-      <c r="J42" s="30">
+      <c r="J42" s="29">
         <v>1.2</v>
       </c>
-      <c r="K42" s="30"/>
-      <c r="L42" s="30">
+      <c r="K42" s="29"/>
+      <c r="L42" s="29">
         <v>3</v>
       </c>
-      <c r="M42" s="30"/>
-      <c r="N42" s="30">
+      <c r="M42" s="29"/>
+      <c r="N42" s="29">
         <v>1.7929999999999999</v>
       </c>
-      <c r="O42" s="30"/>
+      <c r="O42" s="29"/>
     </row>
     <row r="43" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B43">
@@ -18821,18 +18989,18 @@
       <c r="I43">
         <v>20</v>
       </c>
-      <c r="J43" s="30">
+      <c r="J43" s="29">
         <v>1.3</v>
       </c>
-      <c r="K43" s="30"/>
-      <c r="L43" s="30">
+      <c r="K43" s="29"/>
+      <c r="L43" s="29">
         <v>4</v>
       </c>
-      <c r="M43" s="30"/>
-      <c r="N43" s="30">
+      <c r="M43" s="29"/>
+      <c r="N43" s="29">
         <v>1.8839999999999999</v>
       </c>
-      <c r="O43" s="30"/>
+      <c r="O43" s="29"/>
     </row>
     <row r="44" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B44">
@@ -18853,18 +19021,18 @@
       <c r="I44">
         <v>50</v>
       </c>
-      <c r="J44" s="30">
+      <c r="J44" s="29">
         <v>2.36</v>
       </c>
-      <c r="K44" s="30"/>
-      <c r="L44" s="30">
+      <c r="K44" s="29"/>
+      <c r="L44" s="29">
         <v>6</v>
       </c>
-      <c r="M44" s="30"/>
-      <c r="N44" s="30">
+      <c r="M44" s="29"/>
+      <c r="N44" s="29">
         <v>2.2669999999999999</v>
       </c>
-      <c r="O44" s="30"/>
+      <c r="O44" s="29"/>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45">
@@ -18885,18 +19053,18 @@
       <c r="I45">
         <v>100</v>
       </c>
-      <c r="J45" s="30">
+      <c r="J45" s="29">
         <v>2.5499999999999998</v>
       </c>
-      <c r="K45" s="30"/>
-      <c r="L45" s="30">
+      <c r="K45" s="29"/>
+      <c r="L45" s="29">
         <v>8</v>
       </c>
-      <c r="M45" s="30"/>
-      <c r="N45" s="30">
+      <c r="M45" s="29"/>
+      <c r="N45" s="29">
         <v>2.8820000000000001</v>
       </c>
-      <c r="O45" s="30"/>
+      <c r="O45" s="29"/>
     </row>
     <row r="46" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B46">
@@ -18917,18 +19085,18 @@
       <c r="I46">
         <v>1000</v>
       </c>
-      <c r="J46" s="30">
+      <c r="J46" s="29">
         <v>3.55</v>
       </c>
-      <c r="K46" s="30"/>
-      <c r="L46" s="30">
+      <c r="K46" s="29"/>
+      <c r="L46" s="29">
         <v>12</v>
       </c>
-      <c r="M46" s="30"/>
-      <c r="N46" s="30">
+      <c r="M46" s="29"/>
+      <c r="N46" s="29">
         <v>4.1079999999999997</v>
       </c>
-      <c r="O46" s="30"/>
+      <c r="O46" s="29"/>
     </row>
     <row r="47" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B47">
@@ -19028,6 +19196,12 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="N46:O46"/>
+    <mergeCell ref="J46:K46"/>
+    <mergeCell ref="L43:M43"/>
+    <mergeCell ref="L44:M44"/>
+    <mergeCell ref="L45:M45"/>
+    <mergeCell ref="L46:M46"/>
     <mergeCell ref="N45:O45"/>
     <mergeCell ref="N44:O44"/>
     <mergeCell ref="N43:O43"/>
@@ -19035,18 +19209,12 @@
     <mergeCell ref="J43:K43"/>
     <mergeCell ref="J44:K44"/>
     <mergeCell ref="J45:K45"/>
-    <mergeCell ref="J46:K46"/>
-    <mergeCell ref="L43:M43"/>
-    <mergeCell ref="L44:M44"/>
-    <mergeCell ref="L45:M45"/>
-    <mergeCell ref="L46:M46"/>
     <mergeCell ref="J41:K41"/>
     <mergeCell ref="L41:M41"/>
     <mergeCell ref="N41:O41"/>
     <mergeCell ref="J42:K42"/>
     <mergeCell ref="L42:M42"/>
     <mergeCell ref="N42:O42"/>
-    <mergeCell ref="N46:O46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -22418,7 +22586,7 @@
         <v>43</v>
       </c>
       <c r="AC3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:49" x14ac:dyDescent="0.25">
@@ -22453,43 +22621,43 @@
         <v>31</v>
       </c>
       <c r="AD4" t="s">
+        <v>88</v>
+      </c>
+      <c r="AE4" t="s">
         <v>89</v>
       </c>
-      <c r="AE4" t="s">
-        <v>90</v>
-      </c>
       <c r="AF4" t="s">
+        <v>99</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>91</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>92</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>93</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>94</v>
+      </c>
+      <c r="AO4" t="s">
+        <v>88</v>
+      </c>
+      <c r="AP4" t="s">
+        <v>89</v>
+      </c>
+      <c r="AQ4" t="s">
+        <v>99</v>
+      </c>
+      <c r="AR4" t="s">
         <v>100</v>
       </c>
-      <c r="AG4" t="s">
-        <v>92</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>93</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>94</v>
-      </c>
-      <c r="AJ4" t="s">
-        <v>95</v>
-      </c>
-      <c r="AO4" t="s">
-        <v>89</v>
-      </c>
-      <c r="AP4" t="s">
-        <v>90</v>
-      </c>
-      <c r="AQ4" t="s">
-        <v>100</v>
-      </c>
-      <c r="AR4" t="s">
+      <c r="AS4" t="s">
         <v>101</v>
       </c>
-      <c r="AS4" t="s">
+      <c r="AT4" t="s">
         <v>102</v>
-      </c>
-      <c r="AT4" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:49" ht="15.75" x14ac:dyDescent="0.25">
@@ -22742,7 +22910,7 @@
         <v>2.9957219793944487E-2</v>
       </c>
       <c r="AL7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AM7">
         <f>_xlfn.STDEV.S(AD5:AD54)</f>
@@ -22771,7 +22939,7 @@
         <v>4.9957219793944484E-2</v>
       </c>
       <c r="AV7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AW7">
         <f>MAX(AT5:AT54)</f>
@@ -22871,7 +23039,7 @@
         <v>4.2232608630250176E-2</v>
       </c>
       <c r="AV8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AW8">
         <f>0.18845</f>
@@ -23028,7 +23196,7 @@
         <v>2.2232608630250172E-2</v>
       </c>
       <c r="AL10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AM10">
         <f>0.18845</f>
@@ -26887,10 +27055,10 @@
         <v>44</v>
       </c>
       <c r="O60" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AC60" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="61" spans="1:46" x14ac:dyDescent="0.25">
@@ -26919,25 +27087,25 @@
         <v>31</v>
       </c>
       <c r="AD61" t="s">
+        <v>88</v>
+      </c>
+      <c r="AE61" t="s">
         <v>89</v>
       </c>
-      <c r="AE61" t="s">
+      <c r="AF61" t="s">
         <v>90</v>
       </c>
-      <c r="AF61" t="s">
+      <c r="AG61" t="s">
         <v>91</v>
       </c>
-      <c r="AG61" t="s">
+      <c r="AH61" t="s">
         <v>92</v>
       </c>
-      <c r="AH61" t="s">
+      <c r="AI61" t="s">
         <v>93</v>
       </c>
-      <c r="AI61" t="s">
+      <c r="AJ61" t="s">
         <v>94</v>
-      </c>
-      <c r="AJ61" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="62" spans="1:46" x14ac:dyDescent="0.25">
@@ -27122,7 +27290,7 @@
         <v>6.410067001008506E-3</v>
       </c>
       <c r="AL64" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AM64">
         <f>_xlfn.STDEV.S(AD62:AD161)</f>
@@ -27304,7 +27472,7 @@
         <v>3.641006700100851E-2</v>
       </c>
       <c r="AL67" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AM67">
         <f>1.3581/SQRT(AM62)</f>
@@ -39825,7 +39993,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B1" s="5">
         <v>1</v>

</xml_diff>

<commit_message>
implemented result from 9th experiment
</commit_message>
<xml_diff>
--- a/Data Collection.xlsx
+++ b/Data Collection.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yoga\Desktop\University\Thesis\TrustChain-Simulator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\umeer\Desktop\University\TrustChain-Simulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{485D6F39-31DA-40C6-8A03-F727A92A478C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4031691C-9456-4D4C-A3F2-CCDFDCC82727}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{BCACAF04-D4C4-41AE-BAB0-4F6EFB70057E}"/>
   </bookViews>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="119">
   <si>
     <t>Evil Node Sleeping Transactions</t>
   </si>
@@ -390,11 +390,37 @@
   <si>
     <t>9 -  Average Path Length</t>
   </si>
+  <si>
+    <t>0.406666666668</t>
+  </si>
+  <si>
+    <t>Too long</t>
+  </si>
+  <si>
+    <t>0.40666666667</t>
+  </si>
+  <si>
+    <t>0.406819158163</t>
+  </si>
+  <si>
+    <t>0.305000000001</t>
+  </si>
+  <si>
+    <t>0.408242231292</t>
+  </si>
+  <si>
+    <t>0.408334545058</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="3">
+    <numFmt numFmtId="174" formatCode="#,##0.000000000000"/>
+    <numFmt numFmtId="175" formatCode="#,##0.0000000000000"/>
+    <numFmt numFmtId="179" formatCode="0.000000000000"/>
+  </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -679,7 +705,7 @@
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -727,6 +753,10 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="12" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -739,10 +769,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -750,6 +780,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="60% - Accent1" xfId="11" builtinId="32"/>
@@ -16778,8 +16811,8 @@
   <dimension ref="A1:T55"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A48" sqref="A48"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A42" sqref="A42:A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16854,7 +16887,7 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="31" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="4">
@@ -16898,7 +16931,7 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="28"/>
+      <c r="A3" s="30"/>
       <c r="B3" s="4">
         <v>2</v>
       </c>
@@ -16940,7 +16973,7 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="28"/>
+      <c r="A4" s="30"/>
       <c r="B4" s="4">
         <v>3</v>
       </c>
@@ -16986,7 +17019,7 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="28"/>
+      <c r="A5" s="30"/>
       <c r="B5" s="4">
         <v>4</v>
       </c>
@@ -17029,7 +17062,7 @@
       <c r="T5" s="1"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
+      <c r="A6" s="30"/>
       <c r="B6" s="4">
         <v>5</v>
       </c>
@@ -17075,7 +17108,7 @@
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="28"/>
+      <c r="A7" s="30"/>
       <c r="B7" s="4">
         <v>6</v>
       </c>
@@ -17118,7 +17151,7 @@
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="32" t="s">
         <v>25</v>
       </c>
       <c r="B8" s="5">
@@ -17165,7 +17198,7 @@
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
+      <c r="A9" s="32"/>
       <c r="B9" s="5">
         <v>2</v>
       </c>
@@ -17210,7 +17243,7 @@
       </c>
     </row>
     <row r="10" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
+      <c r="A10" s="32"/>
       <c r="B10" s="5">
         <v>3</v>
       </c>
@@ -17255,7 +17288,7 @@
       </c>
     </row>
     <row r="11" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="30"/>
+      <c r="A11" s="32"/>
       <c r="B11" s="5">
         <v>4</v>
       </c>
@@ -17298,7 +17331,7 @@
       <c r="T11" s="26"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="30" t="s">
+      <c r="A12" s="32" t="s">
         <v>26</v>
       </c>
       <c r="B12" s="6">
@@ -17342,7 +17375,7 @@
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="30"/>
+      <c r="A13" s="32"/>
       <c r="B13" s="6">
         <v>2</v>
       </c>
@@ -17384,7 +17417,7 @@
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="30"/>
+      <c r="A14" s="32"/>
       <c r="B14" s="6">
         <v>3</v>
       </c>
@@ -17426,7 +17459,7 @@
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="30"/>
+      <c r="A15" s="32"/>
       <c r="B15" s="6">
         <v>4</v>
       </c>
@@ -17468,7 +17501,7 @@
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="30"/>
+      <c r="A16" s="32"/>
       <c r="B16" s="6">
         <v>5</v>
       </c>
@@ -17510,7 +17543,7 @@
       </c>
     </row>
     <row r="17" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="30"/>
+      <c r="A17" s="32"/>
       <c r="B17" s="6">
         <v>6</v>
       </c>
@@ -17597,7 +17630,7 @@
       </c>
     </row>
     <row r="19" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="31" t="s">
+      <c r="A19" s="33" t="s">
         <v>46</v>
       </c>
       <c r="B19" s="20">
@@ -17644,7 +17677,7 @@
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="31"/>
+      <c r="A20" s="33"/>
       <c r="B20" s="20">
         <v>2</v>
       </c>
@@ -17689,7 +17722,7 @@
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="28" t="s">
+      <c r="A21" s="30" t="s">
         <v>47</v>
       </c>
       <c r="B21" s="10">
@@ -17733,7 +17766,7 @@
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="28"/>
+      <c r="A22" s="30"/>
       <c r="B22" s="11">
         <v>2</v>
       </c>
@@ -17775,7 +17808,7 @@
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="28"/>
+      <c r="A23" s="30"/>
       <c r="B23" s="10">
         <v>3</v>
       </c>
@@ -17817,7 +17850,7 @@
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="28"/>
+      <c r="A24" s="30"/>
       <c r="B24" s="11">
         <v>4</v>
       </c>
@@ -17859,7 +17892,7 @@
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25" s="28"/>
+      <c r="A25" s="30"/>
       <c r="B25" s="10">
         <v>5</v>
       </c>
@@ -17901,7 +17934,7 @@
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A26" s="28" t="s">
+      <c r="A26" s="30" t="s">
         <v>57</v>
       </c>
       <c r="B26" s="12">
@@ -17948,7 +17981,7 @@
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" s="28"/>
+      <c r="A27" s="30"/>
       <c r="B27" s="12">
         <v>2</v>
       </c>
@@ -17990,7 +18023,7 @@
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A28" s="28"/>
+      <c r="A28" s="30"/>
       <c r="B28" s="12">
         <v>3</v>
       </c>
@@ -18032,7 +18065,7 @@
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A29" s="28"/>
+      <c r="A29" s="30"/>
       <c r="B29" s="12">
         <v>4</v>
       </c>
@@ -18074,7 +18107,7 @@
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A30" s="28"/>
+      <c r="A30" s="30"/>
       <c r="B30" s="12">
         <v>5</v>
       </c>
@@ -18116,7 +18149,7 @@
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A31" s="28"/>
+      <c r="A31" s="30"/>
       <c r="B31" s="12">
         <v>6</v>
       </c>
@@ -18158,7 +18191,7 @@
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A32" s="28" t="s">
+      <c r="A32" s="30" t="s">
         <v>58</v>
       </c>
       <c r="B32" s="14">
@@ -18202,7 +18235,7 @@
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" s="28"/>
+      <c r="A33" s="30"/>
       <c r="B33" s="14">
         <v>2</v>
       </c>
@@ -18244,7 +18277,7 @@
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="28"/>
+      <c r="A34" s="30"/>
       <c r="B34" s="14">
         <v>3</v>
       </c>
@@ -18286,7 +18319,7 @@
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" s="28"/>
+      <c r="A35" s="30"/>
       <c r="B35" s="14">
         <v>4</v>
       </c>
@@ -18328,7 +18361,7 @@
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" s="28"/>
+      <c r="A36" s="30"/>
       <c r="B36" s="14">
         <v>5</v>
       </c>
@@ -18370,7 +18403,7 @@
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" s="28" t="s">
+      <c r="A37" s="30" t="s">
         <v>109</v>
       </c>
       <c r="B37" s="23">
@@ -18403,15 +18436,15 @@
       <c r="L37" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="M37" s="22" t="s">
-        <v>63</v>
+      <c r="M37" s="28" t="s">
+        <v>10</v>
       </c>
       <c r="N37" s="1">
         <v>50</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" s="28"/>
+      <c r="A38" s="30"/>
       <c r="B38" s="23">
         <v>2</v>
       </c>
@@ -18442,15 +18475,15 @@
       <c r="L38" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="M38" s="22" t="s">
-        <v>63</v>
+      <c r="M38" s="28" t="s">
+        <v>10</v>
       </c>
       <c r="N38" s="22">
         <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" s="28"/>
+      <c r="A39" s="30"/>
       <c r="B39" s="23">
         <v>3</v>
       </c>
@@ -18481,15 +18514,15 @@
       <c r="L39" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="M39" s="22" t="s">
-        <v>63</v>
+      <c r="M39" s="28" t="s">
+        <v>10</v>
       </c>
       <c r="N39" s="22">
         <v>50</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A40" s="28"/>
+      <c r="A40" s="30"/>
       <c r="B40" s="23">
         <v>4</v>
       </c>
@@ -18520,15 +18553,15 @@
       <c r="L40" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="M40" s="22" t="s">
-        <v>63</v>
+      <c r="M40" s="28" t="s">
+        <v>10</v>
       </c>
       <c r="N40" s="22">
         <v>50</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A41" s="28"/>
+      <c r="A41" s="30"/>
       <c r="B41" s="23">
         <v>5</v>
       </c>
@@ -18559,15 +18592,15 @@
       <c r="L41" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="M41" s="22" t="s">
-        <v>63</v>
+      <c r="M41" s="28" t="s">
+        <v>10</v>
       </c>
       <c r="N41" s="22">
         <v>50</v>
       </c>
     </row>
     <row r="42" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="28" t="s">
+      <c r="A42" s="30" t="s">
         <v>110</v>
       </c>
       <c r="B42" s="27">
@@ -18611,7 +18644,7 @@
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A43" s="28"/>
+      <c r="A43" s="30"/>
       <c r="B43" s="27">
         <v>2</v>
       </c>
@@ -18653,7 +18686,7 @@
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A44" s="28"/>
+      <c r="A44" s="30"/>
       <c r="B44" s="27">
         <v>3</v>
       </c>
@@ -18695,7 +18728,7 @@
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A45" s="28"/>
+      <c r="A45" s="30"/>
       <c r="B45" s="27">
         <v>4</v>
       </c>
@@ -18737,7 +18770,7 @@
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A46" s="28"/>
+      <c r="A46" s="30"/>
       <c r="B46" s="27">
         <v>5</v>
       </c>
@@ -18779,7 +18812,7 @@
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A47" s="28"/>
+      <c r="A47" s="30"/>
       <c r="B47" s="27">
         <v>6</v>
       </c>
@@ -18857,7 +18890,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF874DAA-691A-4835-ACA3-DB30922CFD6B}">
   <dimension ref="A1:W52"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
@@ -19952,15 +19985,15 @@
       <c r="E40">
         <v>0.91530000000300005</v>
       </c>
-      <c r="I40" s="33" t="s">
+      <c r="I40" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="J40" s="33"/>
-      <c r="K40" s="33"/>
-      <c r="L40" s="33"/>
-      <c r="M40" s="33"/>
-      <c r="N40" s="33"/>
-      <c r="O40" s="33"/>
+      <c r="J40" s="34"/>
+      <c r="K40" s="34"/>
+      <c r="L40" s="34"/>
+      <c r="M40" s="34"/>
+      <c r="N40" s="34"/>
+      <c r="O40" s="34"/>
     </row>
     <row r="41" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B41">
@@ -19978,18 +20011,18 @@
       <c r="I41" t="s">
         <v>107</v>
       </c>
-      <c r="J41" s="32" t="s">
+      <c r="J41" s="35" t="s">
         <v>104</v>
       </c>
-      <c r="K41" s="32"/>
-      <c r="L41" s="32" t="s">
+      <c r="K41" s="35"/>
+      <c r="L41" s="35" t="s">
         <v>105</v>
       </c>
-      <c r="M41" s="32"/>
-      <c r="N41" s="32" t="s">
+      <c r="M41" s="35"/>
+      <c r="N41" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="O41" s="32"/>
+      <c r="O41" s="35"/>
     </row>
     <row r="42" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B42">
@@ -20010,18 +20043,18 @@
       <c r="I42">
         <v>10</v>
       </c>
-      <c r="J42" s="32">
+      <c r="J42" s="35">
         <v>1.2</v>
       </c>
-      <c r="K42" s="32"/>
-      <c r="L42" s="32">
+      <c r="K42" s="35"/>
+      <c r="L42" s="35">
         <v>3</v>
       </c>
-      <c r="M42" s="32"/>
-      <c r="N42" s="32">
+      <c r="M42" s="35"/>
+      <c r="N42" s="35">
         <v>1.7929999999999999</v>
       </c>
-      <c r="O42" s="32"/>
+      <c r="O42" s="35"/>
     </row>
     <row r="43" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B43">
@@ -20042,18 +20075,18 @@
       <c r="I43">
         <v>20</v>
       </c>
-      <c r="J43" s="32">
+      <c r="J43" s="35">
         <v>1.3</v>
       </c>
-      <c r="K43" s="32"/>
-      <c r="L43" s="32">
+      <c r="K43" s="35"/>
+      <c r="L43" s="35">
         <v>4</v>
       </c>
-      <c r="M43" s="32"/>
-      <c r="N43" s="32">
+      <c r="M43" s="35"/>
+      <c r="N43" s="35">
         <v>1.8839999999999999</v>
       </c>
-      <c r="O43" s="32"/>
+      <c r="O43" s="35"/>
     </row>
     <row r="44" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B44">
@@ -20074,18 +20107,18 @@
       <c r="I44">
         <v>50</v>
       </c>
-      <c r="J44" s="32">
+      <c r="J44" s="35">
         <v>2.36</v>
       </c>
-      <c r="K44" s="32"/>
-      <c r="L44" s="32">
+      <c r="K44" s="35"/>
+      <c r="L44" s="35">
         <v>6</v>
       </c>
-      <c r="M44" s="32"/>
-      <c r="N44" s="32">
+      <c r="M44" s="35"/>
+      <c r="N44" s="35">
         <v>2.2669999999999999</v>
       </c>
-      <c r="O44" s="32"/>
+      <c r="O44" s="35"/>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45">
@@ -20106,18 +20139,18 @@
       <c r="I45">
         <v>100</v>
       </c>
-      <c r="J45" s="32">
+      <c r="J45" s="35">
         <v>2.5499999999999998</v>
       </c>
-      <c r="K45" s="32"/>
-      <c r="L45" s="32">
+      <c r="K45" s="35"/>
+      <c r="L45" s="35">
         <v>8</v>
       </c>
-      <c r="M45" s="32"/>
-      <c r="N45" s="32">
+      <c r="M45" s="35"/>
+      <c r="N45" s="35">
         <v>2.8820000000000001</v>
       </c>
-      <c r="O45" s="32"/>
+      <c r="O45" s="35"/>
     </row>
     <row r="46" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B46">
@@ -20138,18 +20171,18 @@
       <c r="I46">
         <v>1000</v>
       </c>
-      <c r="J46" s="32">
+      <c r="J46" s="35">
         <v>3.55</v>
       </c>
-      <c r="K46" s="32"/>
-      <c r="L46" s="32">
+      <c r="K46" s="35"/>
+      <c r="L46" s="35">
         <v>12</v>
       </c>
-      <c r="M46" s="32"/>
-      <c r="N46" s="32">
+      <c r="M46" s="35"/>
+      <c r="N46" s="35">
         <v>4.1079999999999997</v>
       </c>
-      <c r="O46" s="32"/>
+      <c r="O46" s="35"/>
     </row>
     <row r="47" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B47">
@@ -20249,6 +20282,15 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="N46:O46"/>
+    <mergeCell ref="J46:K46"/>
+    <mergeCell ref="L43:M43"/>
+    <mergeCell ref="L44:M44"/>
+    <mergeCell ref="L45:M45"/>
+    <mergeCell ref="L46:M46"/>
+    <mergeCell ref="N45:O45"/>
+    <mergeCell ref="N44:O44"/>
+    <mergeCell ref="N43:O43"/>
     <mergeCell ref="I40:O40"/>
     <mergeCell ref="J43:K43"/>
     <mergeCell ref="J44:K44"/>
@@ -20259,15 +20301,6 @@
     <mergeCell ref="J42:K42"/>
     <mergeCell ref="L42:M42"/>
     <mergeCell ref="N42:O42"/>
-    <mergeCell ref="N46:O46"/>
-    <mergeCell ref="J46:K46"/>
-    <mergeCell ref="L43:M43"/>
-    <mergeCell ref="L44:M44"/>
-    <mergeCell ref="L45:M45"/>
-    <mergeCell ref="L46:M46"/>
-    <mergeCell ref="N45:O45"/>
-    <mergeCell ref="N44:O44"/>
-    <mergeCell ref="N43:O43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -38823,7 +38856,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CE560BB-010F-4538-8606-72D35C2079F1}">
   <dimension ref="A1:Z209"/>
   <sheetViews>
-    <sheetView topLeftCell="A103" workbookViewId="0">
+    <sheetView topLeftCell="A124" workbookViewId="0">
       <selection activeCell="V130" sqref="V130"/>
     </sheetView>
   </sheetViews>
@@ -41476,7 +41509,7 @@
       </c>
     </row>
     <row r="108" spans="1:26" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="34" t="s">
+      <c r="A108" s="36" t="s">
         <v>110</v>
       </c>
       <c r="B108" s="5">
@@ -41499,7 +41532,7 @@
       </c>
     </row>
     <row r="109" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="35"/>
+      <c r="A109" s="37"/>
       <c r="B109">
         <v>1.32</v>
       </c>
@@ -41544,7 +41577,7 @@
       <c r="Z109" s="18"/>
     </row>
     <row r="110" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="35"/>
+      <c r="A110" s="37"/>
       <c r="B110">
         <v>4.9858304269760003</v>
       </c>
@@ -41577,7 +41610,7 @@
       <c r="Z110" s="16"/>
     </row>
     <row r="111" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A111" s="35"/>
+      <c r="A111" s="37"/>
       <c r="B111">
         <v>6.3728169473809997</v>
       </c>
@@ -41634,7 +41667,7 @@
       </c>
     </row>
     <row r="112" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A112" s="35"/>
+      <c r="A112" s="37"/>
       <c r="B112">
         <v>9.3210768256519998</v>
       </c>
@@ -46393,16 +46426,22 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6DE4954-B822-463F-AF49-CD5C62D3DBE0}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>111</v>
       </c>
@@ -46420,6 +46459,1154 @@
       </c>
       <c r="F1" s="5">
         <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2" s="40">
+        <v>0.91563134253</v>
+      </c>
+      <c r="E2" s="39">
+        <v>1.118953564755</v>
+      </c>
+      <c r="F2" s="38">
+        <v>13.725000000045</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D3" s="40">
+        <v>0.813333333336</v>
+      </c>
+      <c r="E3" s="39">
+        <v>1.5255667304439999</v>
+      </c>
+      <c r="F3" s="38">
+        <v>16.970000000079999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D4" s="40">
+        <v>0.813333333336</v>
+      </c>
+      <c r="E4" s="39">
+        <v>1.4150000000089999</v>
+      </c>
+      <c r="F4" s="38">
+        <v>22.671705261644998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D5" s="40">
+        <v>0.71166666666900003</v>
+      </c>
+      <c r="E5" s="39">
+        <v>1.3223165833999999</v>
+      </c>
+      <c r="F5" s="38">
+        <v>15.656666666717999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>112</v>
+      </c>
+      <c r="D6" s="40">
+        <v>0.91621866739400004</v>
+      </c>
+      <c r="E6" s="39">
+        <v>1.4233333333380001</v>
+      </c>
+      <c r="F6" s="38">
+        <v>24.400000000079999</v>
+      </c>
+      <c r="I6" s="29"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D7" s="40">
+        <v>0.71206885930599995</v>
+      </c>
+      <c r="E7" s="39">
+        <v>1.525307829498</v>
+      </c>
+      <c r="F7" s="38">
+        <v>5.3733333333919999</v>
+      </c>
+      <c r="I7" s="29"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>115</v>
+      </c>
+      <c r="D8" s="40">
+        <v>0.813333333336</v>
+      </c>
+      <c r="E8" s="39">
+        <v>1.7283333333390001</v>
+      </c>
+      <c r="F8" s="38">
+        <v>25.315000000083</v>
+      </c>
+      <c r="I8" s="29"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D9" s="40">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="E9" s="39">
+        <v>1.2200000000040001</v>
+      </c>
+      <c r="F9" s="38">
+        <v>2.9483333333430002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>112</v>
+      </c>
+      <c r="D10" s="40">
+        <v>0.814149369949</v>
+      </c>
+      <c r="E10" s="39">
+        <v>0.71166666666900003</v>
+      </c>
+      <c r="F10" s="38">
+        <v>23.180000000075999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D11" s="40">
+        <v>0.71255452715699996</v>
+      </c>
+      <c r="E11" s="39">
+        <v>1.118333333337</v>
+      </c>
+      <c r="F11" s="38">
+        <v>10.370000000034</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>116</v>
+      </c>
+      <c r="D12" s="40">
+        <v>0.71166666666900003</v>
+      </c>
+      <c r="E12" s="39">
+        <v>1.2200000000040001</v>
+      </c>
+      <c r="F12" s="38">
+        <v>10.573333333368</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>112</v>
+      </c>
+      <c r="D13" s="40">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="E13" s="39">
+        <v>1.1150000000069999</v>
+      </c>
+      <c r="F13" s="38">
+        <v>16.876666666721999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>117</v>
+      </c>
+      <c r="D14" s="40">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="E14" s="39">
+        <v>1.2200000000040001</v>
+      </c>
+      <c r="F14" s="38">
+        <v>0.71166666666900003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>118</v>
+      </c>
+      <c r="D15" s="40">
+        <v>0.71182149176099996</v>
+      </c>
+      <c r="E15" s="39">
+        <v>1.2200000000040001</v>
+      </c>
+      <c r="F15" s="38">
+        <v>9.7600000000320009</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D16" s="40">
+        <v>0.61063478136299998</v>
+      </c>
+      <c r="E16" s="39">
+        <v>1.0181384666819999</v>
+      </c>
+      <c r="F16" s="38">
+        <v>2.135000000007</v>
+      </c>
+    </row>
+    <row r="17" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D17" s="40">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="E17" s="39">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="F17" s="38">
+        <v>22.875755746039999</v>
+      </c>
+    </row>
+    <row r="18" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D18" s="40">
+        <v>0.81333720015199995</v>
+      </c>
+      <c r="E18" s="39">
+        <v>1.5250000000049999</v>
+      </c>
+      <c r="F18" s="38">
+        <v>4.2700000000139999</v>
+      </c>
+    </row>
+    <row r="19" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D19" s="40">
+        <v>0.71166666666900003</v>
+      </c>
+      <c r="E19" s="39">
+        <v>1.0166666666699999</v>
+      </c>
+      <c r="F19" s="38">
+        <v>1.4233333333380001</v>
+      </c>
+    </row>
+    <row r="20" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D20" s="40">
+        <v>0.813333333336</v>
+      </c>
+      <c r="E20" s="39">
+        <v>1.014315111173</v>
+      </c>
+      <c r="F20" s="38">
+        <v>13.521666666711001</v>
+      </c>
+    </row>
+    <row r="21" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D21" s="40">
+        <v>0.71166666666900003</v>
+      </c>
+      <c r="E21" s="39">
+        <v>1.3218432239610001</v>
+      </c>
+      <c r="F21" s="38">
+        <v>2.135000000007</v>
+      </c>
+    </row>
+    <row r="22" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D22" s="40">
+        <v>0.813333333336</v>
+      </c>
+      <c r="E22" s="39">
+        <v>1.119344530545</v>
+      </c>
+      <c r="F22" s="38">
+        <v>1.7283333333390001</v>
+      </c>
+    </row>
+    <row r="23" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D23" s="40">
+        <v>0.81374060575200002</v>
+      </c>
+      <c r="E23" s="39">
+        <v>1.223608787598</v>
+      </c>
+      <c r="F23" s="38">
+        <v>7.1166666666899996</v>
+      </c>
+    </row>
+    <row r="24" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D24" s="40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="E24" s="39">
+        <v>1.2200000000040001</v>
+      </c>
+      <c r="F24" s="38">
+        <v>10.370000000034</v>
+      </c>
+    </row>
+    <row r="25" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D25" s="40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="E25" s="39">
+        <v>1.7283333333390001</v>
+      </c>
+      <c r="F25" s="38">
+        <v>17.181666666723</v>
+      </c>
+    </row>
+    <row r="26" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D26" s="40">
+        <v>0.71166666666900003</v>
+      </c>
+      <c r="E26" s="39">
+        <v>1.321666666671</v>
+      </c>
+      <c r="F26" s="38">
+        <v>23.891666666745</v>
+      </c>
+    </row>
+    <row r="27" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D27" s="40">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="E27" s="39">
+        <v>1.3209963622459999</v>
+      </c>
+      <c r="F27" s="38">
+        <v>11.991666666784999</v>
+      </c>
+    </row>
+    <row r="28" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D28" s="40">
+        <v>0.50959073004800004</v>
+      </c>
+      <c r="E28" s="39">
+        <v>1.321666666671</v>
+      </c>
+      <c r="F28" s="38">
+        <v>6.6083333333549996</v>
+      </c>
+    </row>
+    <row r="29" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D29" s="40">
+        <v>0.91500000000299997</v>
+      </c>
+      <c r="E29" s="39">
+        <v>0.813333333336</v>
+      </c>
+      <c r="F29" s="38">
+        <v>10.675000000035</v>
+      </c>
+    </row>
+    <row r="30" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D30" s="40">
+        <v>0.71166666666900003</v>
+      </c>
+      <c r="E30" s="39">
+        <v>1.4233333333380001</v>
+      </c>
+      <c r="F30" s="38">
+        <v>3.761666666679</v>
+      </c>
+    </row>
+    <row r="31" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D31" s="40">
+        <v>0.813333333336</v>
+      </c>
+      <c r="E31" s="39">
+        <v>1.0166666666699999</v>
+      </c>
+      <c r="F31" s="38">
+        <v>24.908333333415001</v>
+      </c>
+    </row>
+    <row r="32" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D32" s="40">
+        <v>0.91500000000299997</v>
+      </c>
+      <c r="E32" s="39">
+        <v>1.626666666672</v>
+      </c>
+      <c r="F32" s="38">
+        <v>6.4050000000210003</v>
+      </c>
+    </row>
+    <row r="33" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D33" s="40">
+        <v>0.91500000000299997</v>
+      </c>
+      <c r="E33" s="39">
+        <v>1.321666666671</v>
+      </c>
+      <c r="F33" s="38">
+        <v>2.745000000009</v>
+      </c>
+    </row>
+    <row r="34" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D34" s="40">
+        <v>0.71166666666900003</v>
+      </c>
+      <c r="E34" s="39">
+        <v>1.321666666671</v>
+      </c>
+      <c r="F34" s="38">
+        <v>7.5233333333579999</v>
+      </c>
+    </row>
+    <row r="35" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D35" s="40">
+        <v>0.398333333337</v>
+      </c>
+      <c r="E35" s="39">
+        <v>0.915453912383</v>
+      </c>
+      <c r="F35" s="38">
+        <v>20.028333333399001</v>
+      </c>
+    </row>
+    <row r="36" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D36" s="40">
+        <v>0.71166666666900003</v>
+      </c>
+      <c r="E36" s="39">
+        <v>1.4233333333380001</v>
+      </c>
+      <c r="F36" s="38">
+        <v>24.400000000079999</v>
+      </c>
+    </row>
+    <row r="37" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D37" s="40">
+        <v>0.406666666668</v>
+      </c>
+      <c r="E37" s="39">
+        <v>1.7283333333390001</v>
+      </c>
+      <c r="F37" s="38">
+        <v>15.758333333385</v>
+      </c>
+    </row>
+    <row r="38" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D38" s="40">
+        <v>0.71245119639200005</v>
+      </c>
+      <c r="E38" s="39">
+        <v>1.321666666671</v>
+      </c>
+      <c r="F38" s="38">
+        <v>5.998333333353</v>
+      </c>
+    </row>
+    <row r="39" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D39" s="40">
+        <v>0.71166666666900003</v>
+      </c>
+      <c r="E39" s="39">
+        <v>0.91500000000299997</v>
+      </c>
+      <c r="F39" s="38">
+        <v>15.148333333383</v>
+      </c>
+    </row>
+    <row r="40" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D40" s="40">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="E40" s="39">
+        <v>1.5250000000049999</v>
+      </c>
+      <c r="F40" s="38">
+        <v>9.251666666697</v>
+      </c>
+    </row>
+    <row r="41" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D41" s="40">
+        <v>0.71166666666900003</v>
+      </c>
+      <c r="E41" s="39">
+        <v>1.7200000000119999</v>
+      </c>
+      <c r="F41" s="38">
+        <v>19.723333333397999</v>
+      </c>
+    </row>
+    <row r="42" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D42" s="40">
+        <v>0.813333333336</v>
+      </c>
+      <c r="E42" s="39">
+        <v>1.423643264589</v>
+      </c>
+      <c r="F42" s="38">
+        <v>13.521666666711001</v>
+      </c>
+    </row>
+    <row r="43" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D43" s="40">
+        <v>0.71232650197799996</v>
+      </c>
+      <c r="E43" s="39">
+        <v>1.9316666666769999</v>
+      </c>
+      <c r="F43" s="38">
+        <v>17.588333333390999</v>
+      </c>
+    </row>
+    <row r="44" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D44" s="40">
+        <v>0.813333333336</v>
+      </c>
+      <c r="E44" s="39">
+        <v>1.3229549666210001</v>
+      </c>
+      <c r="F44" s="38">
+        <v>2.5416666666749999</v>
+      </c>
+    </row>
+    <row r="45" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D45" s="40">
+        <v>0.81421186804400003</v>
+      </c>
+      <c r="E45" s="39">
+        <v>0.70333333334000003</v>
+      </c>
+      <c r="F45" s="38">
+        <v>12.200000000039999</v>
+      </c>
+    </row>
+    <row r="46" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D46" s="40">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="E46" s="39">
+        <v>1.11858909058</v>
+      </c>
+      <c r="F46" s="38">
+        <v>24.298333333413002</v>
+      </c>
+    </row>
+    <row r="47" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D47" s="40">
+        <v>0.813333333336</v>
+      </c>
+      <c r="E47" s="39">
+        <v>0.81166666667300003</v>
+      </c>
+      <c r="F47" s="38">
+        <v>5.1850000000170002</v>
+      </c>
+    </row>
+    <row r="48" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D48" s="40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="E48" s="39">
+        <v>1.321666666671</v>
+      </c>
+      <c r="F48" s="38">
+        <v>25.111666666748999</v>
+      </c>
+    </row>
+    <row r="49" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D49" s="40">
+        <v>0.712881519766</v>
+      </c>
+      <c r="E49" s="39">
+        <v>1.0166666666699999</v>
+      </c>
+      <c r="F49" s="38">
+        <v>14.843333333382001</v>
+      </c>
+    </row>
+    <row r="50" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D50" s="40">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="E50" s="39">
+        <v>1.0166666666699999</v>
+      </c>
+      <c r="F50" s="38">
+        <v>5.3883333333510004</v>
+      </c>
+    </row>
+    <row r="51" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D51" s="40">
+        <v>1.0166666666699999</v>
+      </c>
+      <c r="E51" s="39">
+        <v>0.813333333336</v>
+      </c>
+      <c r="F51" s="38">
+        <v>23.485000000077001</v>
+      </c>
+    </row>
+    <row r="52" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D52" s="40">
+        <v>0.712674432518</v>
+      </c>
+      <c r="E52" s="39">
+        <v>1.321666666671</v>
+      </c>
+      <c r="F52" s="38">
+        <v>21.451666666737001</v>
+      </c>
+    </row>
+    <row r="53" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D53" s="40">
+        <v>0.50000000000400002</v>
+      </c>
+      <c r="E53" s="39">
+        <v>1.2200000000040001</v>
+      </c>
+      <c r="F53" s="38">
+        <v>9.1500000000299995</v>
+      </c>
+    </row>
+    <row r="54" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D54" s="40">
+        <v>0.71290905487300005</v>
+      </c>
+      <c r="E54" s="39">
+        <v>0.813333333336</v>
+      </c>
+      <c r="F54" s="38">
+        <v>17.893333333392</v>
+      </c>
+    </row>
+    <row r="55" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D55" s="40">
+        <v>0.71166666666900003</v>
+      </c>
+      <c r="E55" s="39">
+        <v>1.0086411079199999</v>
+      </c>
+      <c r="F55" s="38">
+        <v>9.6583333333650003</v>
+      </c>
+    </row>
+    <row r="56" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D56" s="40">
+        <v>0.71166666666900003</v>
+      </c>
+      <c r="E56" s="39">
+        <v>0.91500000000299997</v>
+      </c>
+      <c r="F56" s="38">
+        <v>22.163333333406001</v>
+      </c>
+    </row>
+    <row r="57" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D57" s="40">
+        <v>0.813333333336</v>
+      </c>
+      <c r="E57" s="39">
+        <v>1.0116666666730001</v>
+      </c>
+      <c r="F57" s="38">
+        <v>13.521666666711001</v>
+      </c>
+    </row>
+    <row r="58" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D58" s="40">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="E58" s="39">
+        <v>1.4233333333380001</v>
+      </c>
+      <c r="F58" s="38">
+        <v>24.705000000081</v>
+      </c>
+    </row>
+    <row r="59" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D59" s="40">
+        <v>0.81392381531500002</v>
+      </c>
+      <c r="E59" s="39">
+        <v>1.0166666666699999</v>
+      </c>
+      <c r="F59" s="38">
+        <v>5.0833333333499997</v>
+      </c>
+    </row>
+    <row r="60" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D60" s="40">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="E60" s="39">
+        <v>1.118333333337</v>
+      </c>
+      <c r="F60" s="38">
+        <v>13.725000000045</v>
+      </c>
+    </row>
+    <row r="61" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D61" s="40">
+        <v>0.813333333336</v>
+      </c>
+      <c r="E61" s="39">
+        <v>1.5250000000049999</v>
+      </c>
+      <c r="F61" s="38">
+        <v>25.41666666675</v>
+      </c>
+    </row>
+    <row r="62" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D62" s="40">
+        <v>0.71166666666900003</v>
+      </c>
+      <c r="E62" s="39">
+        <v>1.5250000000049999</v>
+      </c>
+      <c r="F62" s="38">
+        <v>11.081666666703001</v>
+      </c>
+    </row>
+    <row r="63" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D63" s="40">
+        <v>0.813333333336</v>
+      </c>
+      <c r="E63" s="39">
+        <v>0.71166666666900003</v>
+      </c>
+      <c r="F63" s="38">
+        <v>16.470000000054</v>
+      </c>
+    </row>
+    <row r="64" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D64" s="40">
+        <v>0.61253165500399998</v>
+      </c>
+      <c r="E64" s="39">
+        <v>1.118333333337</v>
+      </c>
+      <c r="F64" s="38">
+        <v>3.5583333333449998</v>
+      </c>
+    </row>
+    <row r="65" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D65" s="40">
+        <v>0.813333333336</v>
+      </c>
+      <c r="E65" s="39">
+        <v>1.5250000000049999</v>
+      </c>
+      <c r="F65" s="38">
+        <v>18.503333333394</v>
+      </c>
+    </row>
+    <row r="66" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D66" s="40">
+        <v>0.61105895923300002</v>
+      </c>
+      <c r="E66" s="39">
+        <v>1.0166666666699999</v>
+      </c>
+      <c r="F66" s="38">
+        <v>1.8300000000059999</v>
+      </c>
+    </row>
+    <row r="67" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D67" s="40">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="E67" s="39">
+        <v>1.2200000000040001</v>
+      </c>
+      <c r="F67" s="38">
+        <v>1.118333333337</v>
+      </c>
+    </row>
+    <row r="68" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D68" s="40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="E68" s="39">
+        <v>1.321666666671</v>
+      </c>
+      <c r="F68" s="38">
+        <v>22.570000000074</v>
+      </c>
+    </row>
+    <row r="69" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D69" s="40">
+        <v>0.71166666666900003</v>
+      </c>
+      <c r="E69" s="39">
+        <v>1.5250000000049999</v>
+      </c>
+      <c r="F69" s="38">
+        <v>10.573333333368</v>
+      </c>
+    </row>
+    <row r="70" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D70" s="40">
+        <v>0.406666666668</v>
+      </c>
+      <c r="E70" s="39">
+        <v>0.71166666666900003</v>
+      </c>
+      <c r="F70" s="38">
+        <v>4.8800000000160004</v>
+      </c>
+    </row>
+    <row r="71" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D71" s="40">
+        <v>0.71166666666900003</v>
+      </c>
+      <c r="E71" s="39">
+        <v>1.4233333333380001</v>
+      </c>
+      <c r="F71" s="38">
+        <v>2.4400000000080002</v>
+      </c>
+    </row>
+    <row r="72" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D72" s="40">
+        <v>0.50862001970100001</v>
+      </c>
+      <c r="E72" s="39">
+        <v>1.626666666672</v>
+      </c>
+      <c r="F72" s="38">
+        <v>10.878333333369</v>
+      </c>
+    </row>
+    <row r="73" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D73" s="40">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="E73" s="39">
+        <v>1.118333333337</v>
+      </c>
+      <c r="F73" s="38">
+        <v>14.436666666714</v>
+      </c>
+    </row>
+    <row r="74" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D74" s="40">
+        <v>0.71283777864700004</v>
+      </c>
+      <c r="E74" s="39">
+        <v>1.1206611285170001</v>
+      </c>
+      <c r="F74" s="38">
+        <v>20.435000000066999</v>
+      </c>
+    </row>
+    <row r="75" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D75" s="40">
+        <v>0.915249587127</v>
+      </c>
+      <c r="E75" s="39">
+        <v>1.0166666666699999</v>
+      </c>
+      <c r="F75" s="38">
+        <v>4.5750000000149997</v>
+      </c>
+    </row>
+    <row r="76" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D76" s="40">
+        <v>0.91594992243700002</v>
+      </c>
+      <c r="E76" s="39">
+        <v>1.5250000000049999</v>
+      </c>
+      <c r="F76" s="38">
+        <v>4.3716666666809996</v>
+      </c>
+    </row>
+    <row r="77" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D77" s="40">
+        <v>0.71166666666900003</v>
+      </c>
+      <c r="E77" s="39">
+        <v>1.2200000000040001</v>
+      </c>
+      <c r="F77" s="38">
+        <v>21.756666666737999</v>
+      </c>
+    </row>
+    <row r="78" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D78" s="40">
+        <v>0.71166666666900003</v>
+      </c>
+      <c r="E78" s="39">
+        <v>1.626666666672</v>
+      </c>
+      <c r="F78" s="38">
+        <v>19.520000000064002</v>
+      </c>
+    </row>
+    <row r="79" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D79" s="40">
+        <v>0.71259857409000005</v>
+      </c>
+      <c r="E79" s="39">
+        <v>1.321666666671</v>
+      </c>
+      <c r="F79" s="38">
+        <v>15.555000000051001</v>
+      </c>
+    </row>
+    <row r="80" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D80" s="40">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="E80" s="39">
+        <v>1.321666666671</v>
+      </c>
+      <c r="F80" s="38">
+        <v>8.6300000001299999</v>
+      </c>
+    </row>
+    <row r="81" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D81" s="40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="E81" s="39">
+        <v>1.0166666666699999</v>
+      </c>
+      <c r="F81" s="38">
+        <v>6.501666666717</v>
+      </c>
+    </row>
+    <row r="82" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D82" s="40">
+        <v>0.91500000000299997</v>
+      </c>
+      <c r="E82" s="39">
+        <v>1.6268751444189999</v>
+      </c>
+      <c r="F82" s="38">
+        <v>1.0166666666699999</v>
+      </c>
+    </row>
+    <row r="83" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D83" s="40">
+        <v>0.813333333336</v>
+      </c>
+      <c r="E83" s="39">
+        <v>0.91642535700500005</v>
+      </c>
+      <c r="F83" s="38">
+        <v>11.183333333369999</v>
+      </c>
+    </row>
+    <row r="84" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D84" s="40">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="E84" s="39">
+        <v>1.2206580116700001</v>
+      </c>
+      <c r="F84" s="38">
+        <v>21.960000000072</v>
+      </c>
+    </row>
+    <row r="85" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D85" s="40">
+        <v>0.91500000000299997</v>
+      </c>
+      <c r="E85" s="39">
+        <v>2.0342196351139998</v>
+      </c>
+      <c r="F85" s="38">
+        <v>3.253333333344</v>
+      </c>
+    </row>
+    <row r="86" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D86" s="40">
+        <v>0.71166666666900003</v>
+      </c>
+      <c r="E86" s="39">
+        <v>1.8300000000059999</v>
+      </c>
+      <c r="F86" s="38">
+        <v>3.863333333346</v>
+      </c>
+    </row>
+    <row r="87" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D87" s="40">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="E87" s="39">
+        <v>1.220709063518</v>
+      </c>
+      <c r="F87" s="38">
+        <v>9.3533333333640005</v>
+      </c>
+    </row>
+    <row r="88" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D88" s="40">
+        <v>0.813333333336</v>
+      </c>
+      <c r="E88" s="39">
+        <v>1.0166666666699999</v>
+      </c>
+      <c r="F88" s="38">
+        <v>0.406666666668</v>
+      </c>
+    </row>
+    <row r="89" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D89" s="40">
+        <v>0.81438485076199996</v>
+      </c>
+      <c r="E89" s="39">
+        <v>1.5250000000049999</v>
+      </c>
+      <c r="F89" s="38">
+        <v>19.418333333397001</v>
+      </c>
+    </row>
+    <row r="90" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D90" s="40">
+        <v>0.813333333336</v>
+      </c>
+      <c r="E90" s="39">
+        <v>1.5250000000049999</v>
+      </c>
+      <c r="F90" s="38">
+        <v>3.3550000000110001</v>
+      </c>
+    </row>
+    <row r="91" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D91" s="40">
+        <v>0.813333333336</v>
+      </c>
+      <c r="E91" s="39">
+        <v>1.0166666666699999</v>
+      </c>
+      <c r="F91" s="38">
+        <v>14.538333333381001</v>
+      </c>
+    </row>
+    <row r="92" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D92" s="40">
+        <v>0.81449857277299997</v>
+      </c>
+      <c r="E92" s="39">
+        <v>1.2200000000040001</v>
+      </c>
+      <c r="F92" s="38">
+        <v>13.623333333378</v>
+      </c>
+    </row>
+    <row r="93" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D93" s="40">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="E93" s="39">
+        <v>1.6279593533309999</v>
+      </c>
+      <c r="F93" s="38">
+        <v>8.2350000000270001</v>
+      </c>
+    </row>
+    <row r="94" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D94" s="40">
+        <v>0.61006028218099995</v>
+      </c>
+      <c r="E94" s="39">
+        <v>1.931666666673</v>
+      </c>
+      <c r="F94" s="38">
+        <v>11.590000000038</v>
+      </c>
+    </row>
+    <row r="95" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D95" s="40">
+        <v>0.813333333336</v>
+      </c>
+      <c r="E95" s="39">
+        <v>1.0166666666699999</v>
+      </c>
+      <c r="F95" s="38">
+        <v>11.793333333372001</v>
+      </c>
+    </row>
+    <row r="96" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D96" s="40">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="E96" s="39">
+        <v>1.1191459290379999</v>
+      </c>
+      <c r="F96" s="38">
+        <v>19.825000000065</v>
+      </c>
+    </row>
+    <row r="97" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D97" s="40">
+        <v>0.71166666666900003</v>
+      </c>
+      <c r="E97" s="39">
+        <v>1.7227540103900001</v>
+      </c>
+      <c r="F97" s="38">
+        <v>9.8616666666989996</v>
+      </c>
+    </row>
+    <row r="98" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D98" s="40">
+        <v>0.71166666666900003</v>
+      </c>
+      <c r="E98" s="39">
+        <v>1.8300000000059999</v>
+      </c>
+      <c r="F98" s="38">
+        <v>0.30500000000100003</v>
+      </c>
+    </row>
+    <row r="99" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D99" s="40">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="E99" s="39">
+        <v>1.931666666673</v>
+      </c>
+      <c r="F99" s="38">
+        <v>23.586666666744001</v>
+      </c>
+    </row>
+    <row r="100" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D100" s="40">
+        <v>0.71166666666900003</v>
+      </c>
+      <c r="E100" s="39">
+        <v>1.0166666666699999</v>
+      </c>
+      <c r="F100" s="38">
+        <v>8.7433333333619991</v>
+      </c>
+    </row>
+    <row r="101" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D101" s="40">
+        <v>0.71166666666900003</v>
+      </c>
+      <c r="E101" s="39">
+        <v>1.5250000000049999</v>
+      </c>
+      <c r="F101" s="38">
+        <v>10.776666666702001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>